<commit_message>
refactor: Process All Rows to Update or Create Levels and Sub-collections from Excel file
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C9C6C88-752B-4042-8A8F-ECC3CCE8E4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B005D-2544-8F43-B761-BE182874223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="37920" windowHeight="18840" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>A1</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>ستسمع في هذا الدرس بعض الكلمات، حاول كتابتها بشكل صحيح. يمكنك سماع كل كلمة كم مرة تريد. تم أخذ كل هذه الكلمات لذا لن تجدها صعبة للغاية (إذا كنت قد قمت بتدوين الملاحظات:)​</t>
+  </si>
+  <si>
+    <t>ribhi</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -440,9 +449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -501,7 +512,60 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: Implement method to dynamically determine question type in base model
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B005D-2544-8F43-B761-BE182874223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7250BF09-BD0F-BF4D-9B17-7EA796C752FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="37920" windowHeight="18840" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>A1</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>dictation</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +463,7 @@
     <col min="8" max="8" width="169.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +488,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -511,8 +517,11 @@
       <c r="H2" t="s">
         <v>9</v>
       </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -537,8 +546,11 @@
       <c r="H3" t="s">
         <v>11</v>
       </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -562,6 +574,9 @@
       </c>
       <c r="H4" t="s">
         <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Update upload data method to handle multiple question types, deprecate previous commit
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7250BF09-BD0F-BF4D-9B17-7EA796C752FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADB6877-50D4-8D44-8EF0-376B60C51673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="37920" windowHeight="18840" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>A1</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>dictation</t>
+  </si>
+  <si>
+    <t>Girl,People,School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl </t>
+  </si>
+  <si>
+    <t>multipleChoice</t>
   </si>
 </sst>
 </file>
@@ -452,18 +461,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="169.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +500,13 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -518,10 +532,13 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -547,10 +564,13 @@
         <v>11</v>
       </c>
       <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -576,7 +596,42 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: add reading question types into Firestore data upload method
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADB6877-50D4-8D44-8EF0-376B60C51673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460F8403-9B65-7A43-AD09-2104AC4392C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="740" windowWidth="37920" windowHeight="18840" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>A1</t>
   </si>
@@ -59,37 +59,67 @@
     <t>Girl,People,School,Animals,Cat,Fish,Lion,Elephant,Sheep,Chair,Door,Jacket,City,Beautiful,Yellow,Orange,Rainbow,Ice</t>
   </si>
   <si>
-    <t>Unit2</t>
-  </si>
-  <si>
-    <t>ستسمع في هذا الدرس بعض الكلمات، حاول كتابتها بشكل صحيح. يمكنك سماع كل كلمة كم مرة تريد. تم أخذ كل هذه الكلمات لذا لن تجدها صعبة للغاية (إذا كنت قد قمت بتدوين الملاحظات؛))​</t>
-  </si>
-  <si>
-    <t>she,he,them,i sit on the bench,she sits on the bench,moon,money,noodles,orange,oven,Pineapple,park ,queen,question,rainbow,time,umbrella,ear,zebra,violin,white,hear,glue,paint,five apples,eight apples</t>
-  </si>
-  <si>
     <t>ستسمع في هذا الدرس بعض الكلمات، حاول كتابتها بشكل صحيح. يمكنك سماع كل كلمة كم مرة تريد. تم أخذ كل هذه الكلمات لذا لن تجدها صعبة للغاية (إذا كنت قد قمت بتدوين الملاحظات:)​</t>
   </si>
   <si>
-    <t>ribhi</t>
-  </si>
-  <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>dictation</t>
   </si>
   <si>
-    <t>Girl,People,School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Girl </t>
-  </si>
-  <si>
-    <t>multipleChoice</t>
+    <t xml:space="preserve">Reading </t>
+  </si>
+  <si>
+    <t>In this lesson you will read a small text . When you are ready to start press the button and speak into the microphone . Keep trying until you get it right ! Don’t worry about making mistakes , mistakes mean you are improving ​</t>
+  </si>
+  <si>
+    <t>من النص هل يمكنك ايجاد الكلمة الانجليزية للكلامات الاتية ؟ ​</t>
+  </si>
+  <si>
+    <t>Friendship,Paint,Brush,Through,Field,Picnic,Yummy,Watermelon,Grapes,Rainbow,Says,Play</t>
+  </si>
+  <si>
+    <t>صداقة,الصبغ او الرسم بالالوان,فرشاة او ريشة,عبر او خلال,حقل,نزهة,لذيذة,بطيخة,عنب,قوس قزح,يقول,يلعب </t>
+  </si>
+  <si>
+    <t>Friendship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الصداقة </t>
+  </si>
+  <si>
+    <t>In a little village, there were three friends: Red, Blue, and Green.​  Red likes to play with his red ball. Blue likes to paint with her blue brush. And Green likes to run through the green fields.​  They want to have a picnic. Red brings juicy red apples, Blue brings yummy watermelon and Green brings crunchy green grapes.​  They sit on a colorful blanket and enjoy their picnic under the bright sun. Suddenly, they see a rainbow in the sky.​  "It's so pretty!" says Blue.​  "I see red, blue, and green!" says Red.​  "And yellow, purple, and orange too!" adds Green.​  They laugh and play, feeling happy and colorful together. And from that day on, they know that friendship was the brightest color of all.</t>
+  </si>
+  <si>
+    <t>في قرية صغيرة، كان هناك ثلاثة أصدقاء: الأحمر والأزرق والأخضر.​  يحب الأحمر اللعب بكرته الحمراء. يحب الأزرق الرسم بفرشاته الزرقاء. والأخضر يحب الركض عبر الحقول الخضراء.​  يريدون الذهاب الى نزهة . الأحمر يجلب التفاح الأحمر العصير، والأزرق يجلب البطيخ اللذيذ والأخضر يجلب العنب الأخضر المقرمش. ​  يجلسون على بطانية ملونة ويستمتعون بنزهة تحت أشعة الشمس الساطعة. وفجأة رأوا قوس قزح في السماء.​  "انها جميلة جدا!" يقول الأزرق.​  "أرى الأحمر والأزرق والأخضر!" يقول الأحمر.​  "والأصفر والأرجواني والبرتقالي أيضًا!" يضيف الأخضر.​  إنهم يضحكون ويلعبون، ويشعرون بالسعادة والألوان معًا.​   ومن ذلك اليوم فصاعدًا، عرفوا أن الصداقة كانت ألمع الألوان على الإطلاق.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>findWordsFromPassage</t>
+  </si>
+  <si>
+    <t>جاوب على الاسئلة الاتية و قارن بنفسك الاجوبة . لا تنسى كتابة الاجوبة الصحيحة على الدفتر ! حاول بقدر ما تسطيع الاجابة , نعلم انها صعبة قليلا لكن بالصعوبة نترقى ! ​</t>
+  </si>
+  <si>
+    <t>Emily </t>
+  </si>
+  <si>
+    <t>إيميلي ​</t>
+  </si>
+  <si>
+    <t>Hello! My name is Emily. I am six years old. I have three red balloons. I like red because it's my favorite color. I also have two blue toy cars and one green teddy bear. My teddy bear's name is Teddy. He's my best friend. I like to play with my toys in the park. Yesterday, I saw five birds flying in the sky. They were colorful: two were blue, two were yellow, and one was green. It was a beautiful sight! There were also three colorful balloons floating in the air: one red, one blue, and one yellow. After painting, I played with my favorite toys. I have five stuffed animals: a brown bear, a white bunny, a black and white panda, a pink elephant, and a purple unicorn. Each of them has their own special spot on my bed. I love spending time with my toys and creating new adventures for them to go on!</t>
+  </si>
+  <si>
+    <t>مرحبًا! إسمي إيميلي. أنا ست سنوات من العمر. لدي ثلاث بالونات حمراء. أحب اللون الأحمر لأنه لوني المفضل. لدي أيضًا سيارتان لعبة باللون الأزرق ودبدوب أخضر. اسم الدبدوب الخاص بي هو تيدي. انه صديقي المفضل. أحب اللعب بألعابي في الحديقة. بالأمس رأيت خمسة طيور تحلق في السماء. كانت ملونة: اثنان باللون الأزرق، واثنان باللون الأصفر، وواحد باللون الأخضر. كان منظرا جميلا! كانت هناك أيضًا ثلاثة بالونات ملونة تطفو في الهواء: واحدة حمراء، وواحدة زرقاء، وواحدة صفراء. بعد الرسم، لعبت بألعابي المفضلة. لدي خمسة حيوانات محشوة: دب بني، وأرنب أبيض، وباندا أبيض وأسود، وفيل وردي، ووحيد قرن أرجواني. كل واحد منهم لديه مكانه الخاص على سريري. أحب قضاء الوقت مع ألعابي وخلق مغامرات جديدة لهم للاستمرار فيها!</t>
+  </si>
+  <si>
+    <t>answerQuestionsFromPassage</t>
+  </si>
+  <si>
+    <t>What is the name of the speaker? ما هو اسم المتحدث؟​,How old is the speaker? كم عمر المتحدث؟​,How many birds were there in the sky ? كم كان عدد الطيور في السماء؟​,How many stuffed animals does the speaker have? كم عدد الحيوانات المحشية التي يملكها المتحدث؟,What does the speaker like to do ? ماذا يحب المتحدث أن يفعل؟ ​</t>
+  </si>
+  <si>
+    <t>The name of the speaker is Emily,The speaker is six years old ​,There were 5 birds flying in the sky​,The speaker has 5 stuffed animals​,She loves spending time with my toys and creating new adventures for them to go on!</t>
   </si>
 </sst>
 </file>
@@ -461,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,9 +502,10 @@
     <col min="8" max="8" width="169.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -503,135 +534,107 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: upload vocabulary question to firestore
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460F8403-9B65-7A43-AD09-2104AC4392C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C090A1B-DDBE-244B-A9DE-BAB1D3317912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="37920" windowHeight="18840" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
+    <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,102 +36,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>Listening</t>
-  </si>
-  <si>
     <t>Unit1</t>
   </si>
   <si>
-    <t>In this lesson you will hear some words , try typing them correctly . You can hear each word how much ever you like . All of these words are taken before so you wont find them so hard (if you have taken notes ;)​</t>
-  </si>
-  <si>
-    <t>Write down what you are hearing</t>
-  </si>
-  <si>
-    <t>اكتب ما تسمعه</t>
-  </si>
-  <si>
-    <t>Girl,People,School,Animals,Cat,Fish,Lion,Elephant,Sheep,Chair,Door,Jacket,City,Beautiful,Yellow,Orange,Rainbow,Ice</t>
-  </si>
-  <si>
-    <t>ستسمع في هذا الدرس بعض الكلمات، حاول كتابتها بشكل صحيح. يمكنك سماع كل كلمة كم مرة تريد. تم أخذ كل هذه الكلمات لذا لن تجدها صعبة للغاية (إذا كنت قد قمت بتدوين الملاحظات:)​</t>
-  </si>
-  <si>
-    <t>dictation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reading </t>
-  </si>
-  <si>
-    <t>In this lesson you will read a small text . When you are ready to start press the button and speak into the microphone . Keep trying until you get it right ! Don’t worry about making mistakes , mistakes mean you are improving ​</t>
-  </si>
-  <si>
-    <t>من النص هل يمكنك ايجاد الكلمة الانجليزية للكلامات الاتية ؟ ​</t>
-  </si>
-  <si>
-    <t>Friendship,Paint,Brush,Through,Field,Picnic,Yummy,Watermelon,Grapes,Rainbow,Says,Play</t>
-  </si>
-  <si>
-    <t>صداقة,الصبغ او الرسم بالالوان,فرشاة او ريشة,عبر او خلال,حقل,نزهة,لذيذة,بطيخة,عنب,قوس قزح,يقول,يلعب </t>
-  </si>
-  <si>
-    <t>Friendship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الصداقة </t>
-  </si>
-  <si>
-    <t>In a little village, there were three friends: Red, Blue, and Green.​  Red likes to play with his red ball. Blue likes to paint with her blue brush. And Green likes to run through the green fields.​  They want to have a picnic. Red brings juicy red apples, Blue brings yummy watermelon and Green brings crunchy green grapes.​  They sit on a colorful blanket and enjoy their picnic under the bright sun. Suddenly, they see a rainbow in the sky.​  "It's so pretty!" says Blue.​  "I see red, blue, and green!" says Red.​  "And yellow, purple, and orange too!" adds Green.​  They laugh and play, feeling happy and colorful together. And from that day on, they know that friendship was the brightest color of all.</t>
-  </si>
-  <si>
-    <t>في قرية صغيرة، كان هناك ثلاثة أصدقاء: الأحمر والأزرق والأخضر.​  يحب الأحمر اللعب بكرته الحمراء. يحب الأزرق الرسم بفرشاته الزرقاء. والأخضر يحب الركض عبر الحقول الخضراء.​  يريدون الذهاب الى نزهة . الأحمر يجلب التفاح الأحمر العصير، والأزرق يجلب البطيخ اللذيذ والأخضر يجلب العنب الأخضر المقرمش. ​  يجلسون على بطانية ملونة ويستمتعون بنزهة تحت أشعة الشمس الساطعة. وفجأة رأوا قوس قزح في السماء.​  "انها جميلة جدا!" يقول الأزرق.​  "أرى الأحمر والأزرق والأخضر!" يقول الأحمر.​  "والأصفر والأرجواني والبرتقالي أيضًا!" يضيف الأخضر.​  إنهم يضحكون ويلعبون، ويشعرون بالسعادة والألوان معًا.​   ومن ذلك اليوم فصاعدًا، عرفوا أن الصداقة كانت ألمع الألوان على الإطلاق.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>findWordsFromPassage</t>
-  </si>
-  <si>
-    <t>جاوب على الاسئلة الاتية و قارن بنفسك الاجوبة . لا تنسى كتابة الاجوبة الصحيحة على الدفتر ! حاول بقدر ما تسطيع الاجابة , نعلم انها صعبة قليلا لكن بالصعوبة نترقى ! ​</t>
-  </si>
-  <si>
-    <t>Emily </t>
-  </si>
-  <si>
-    <t>إيميلي ​</t>
-  </si>
-  <si>
-    <t>Hello! My name is Emily. I am six years old. I have three red balloons. I like red because it's my favorite color. I also have two blue toy cars and one green teddy bear. My teddy bear's name is Teddy. He's my best friend. I like to play with my toys in the park. Yesterday, I saw five birds flying in the sky. They were colorful: two were blue, two were yellow, and one was green. It was a beautiful sight! There were also three colorful balloons floating in the air: one red, one blue, and one yellow. After painting, I played with my favorite toys. I have five stuffed animals: a brown bear, a white bunny, a black and white panda, a pink elephant, and a purple unicorn. Each of them has their own special spot on my bed. I love spending time with my toys and creating new adventures for them to go on!</t>
-  </si>
-  <si>
-    <t>مرحبًا! إسمي إيميلي. أنا ست سنوات من العمر. لدي ثلاث بالونات حمراء. أحب اللون الأحمر لأنه لوني المفضل. لدي أيضًا سيارتان لعبة باللون الأزرق ودبدوب أخضر. اسم الدبدوب الخاص بي هو تيدي. انه صديقي المفضل. أحب اللعب بألعابي في الحديقة. بالأمس رأيت خمسة طيور تحلق في السماء. كانت ملونة: اثنان باللون الأزرق، واثنان باللون الأصفر، وواحد باللون الأخضر. كان منظرا جميلا! كانت هناك أيضًا ثلاثة بالونات ملونة تطفو في الهواء: واحدة حمراء، وواحدة زرقاء، وواحدة صفراء. بعد الرسم، لعبت بألعابي المفضلة. لدي خمسة حيوانات محشوة: دب بني، وأرنب أبيض، وباندا أبيض وأسود، وفيل وردي، ووحيد قرن أرجواني. كل واحد منهم لديه مكانه الخاص على سريري. أحب قضاء الوقت مع ألعابي وخلق مغامرات جديدة لهم للاستمرار فيها!</t>
-  </si>
-  <si>
-    <t>answerQuestionsFromPassage</t>
-  </si>
-  <si>
-    <t>What is the name of the speaker? ما هو اسم المتحدث؟​,How old is the speaker? كم عمر المتحدث؟​,How many birds were there in the sky ? كم كان عدد الطيور في السماء؟​,How many stuffed animals does the speaker have? كم عدد الحيوانات المحشية التي يملكها المتحدث؟,What does the speaker like to do ? ماذا يحب المتحدث أن يفعل؟ ​</t>
-  </si>
-  <si>
-    <t>The name of the speaker is Emily,The speaker is six years old ​,There were 5 birds flying in the sky​,The speaker has 5 stuffed animals​,She loves spending time with my toys and creating new adventures for them to go on!</t>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>No Intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ملاحظة : هناك ثلاث اقسام للمفردات​
+قسم الجمل و على الطالب حفظها​
+قسم الاسماء و عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
+قسم الافعال و ايضا عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
+سوف يتم استخدام المفردات في درس المحادثة لذالك يجي دراستها بجدية </t>
+  </si>
+  <si>
+    <t>The boy eats an apple الولد يأكل التفاحة,The book is on the table الكتاب على الطاولة,I am a student انا تلميذ,I can speak English انا استطيع التحدث بالانجليزية,Come here  تعال الى هنا</t>
+  </si>
+  <si>
+    <t>Teacher معلمة : I love my teacher  انا احب معلمتي,School مدرسة  : I go to school every day  انا اذهب الى المدرسة كل يوم,Smart ذكية  : she is smart هي ذكية,Week اسبوع : see you next week اراك الاسبوع القادم,Lesson درس  : I love English lessons انا احب الدروس الانجليزي</t>
+  </si>
+  <si>
+    <t>No intro</t>
+  </si>
+  <si>
+    <t>Run اركض : I run everyday  انا اركض كل يوم,Eat أكل  : I eat banana انا اكل موزة,Have لدي : they have a dog  لديهم كلب,Write يكتب : she writes on the book هي تكتب على الكتاب,Say يقول : he says hello  هو يقول مرحبا</t>
+  </si>
+  <si>
+    <t>vocabulary</t>
+  </si>
+  <si>
+    <t>sentence</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>verb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -155,8 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,151 +463,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="169.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="168.5" customWidth="1"/>
+    <col min="9" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Upload mcq to firestore
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C090A1B-DDBE-244B-A9DE-BAB1D3317912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE4BC07-B4B6-FA42-9F1C-2EEC9D8B6340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="28">
   <si>
     <t>A1</t>
   </si>
@@ -44,44 +44,82 @@
     <t>Unit1</t>
   </si>
   <si>
+    <t xml:space="preserve">Reading </t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Vocabulary</t>
-  </si>
-  <si>
-    <t>No Intro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ملاحظة : هناك ثلاث اقسام للمفردات​
-قسم الجمل و على الطالب حفظها​
-قسم الاسماء و عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
-قسم الافعال و ايضا عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
-سوف يتم استخدام المفردات في درس المحادثة لذالك يجي دراستها بجدية </t>
-  </si>
-  <si>
-    <t>The boy eats an apple الولد يأكل التفاحة,The book is on the table الكتاب على الطاولة,I am a student انا تلميذ,I can speak English انا استطيع التحدث بالانجليزية,Come here  تعال الى هنا</t>
-  </si>
-  <si>
-    <t>Teacher معلمة : I love my teacher  انا احب معلمتي,School مدرسة  : I go to school every day  انا اذهب الى المدرسة كل يوم,Smart ذكية  : she is smart هي ذكية,Week اسبوع : see you next week اراك الاسبوع القادم,Lesson درس  : I love English lessons انا احب الدروس الانجليزي</t>
-  </si>
-  <si>
-    <t>No intro</t>
-  </si>
-  <si>
-    <t>Run اركض : I run everyday  انا اركض كل يوم,Eat أكل  : I eat banana انا اكل موزة,Have لدي : they have a dog  لديهم كلب,Write يكتب : she writes on the book هي تكتب على الكتاب,Say يقول : he says hello  هو يقول مرحبا</t>
-  </si>
-  <si>
-    <t>vocabulary</t>
-  </si>
-  <si>
-    <t>sentence</t>
-  </si>
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>verb</t>
+    <t>passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali </t>
+  </si>
+  <si>
+    <t>علي </t>
+  </si>
+  <si>
+    <t>Ali ​  Once upon a time, there was a smart boy named Ali who loved to learn new things. Every day, Ali would go to school. He would wake up early, eat a banana for breakfast, and run to school. Ali loved English lessons the most. He could speak English very well and enjoyed practicing with his friends.​  One day, his teacher gave them a special lesson. She said, "Today, we are going to write a short story." Ali was excited. He loved his teacher and always paid attention to her lessons. He thought for a moment and then began to write on his notebook, "The boy eats an apple," he started.​  At lunch, Ali sat with his friends and talked about their stories. "I can speak English," he proudly told them. They all agreed that learning English was fun. After school, Ali ran home to share his story with his parents. His mother smiled and said, "You are very smart, Ali."​  Before going to bed, Ali looked at the book on the table beside his bed. He said to himself, "I love my school and my teacher. I can't wait for next week to learn more." And with that happy thought, he drifted off to sleep, dreaming of all the new things he would learn.​  See you next week, Ali thought, as he closed his eyes, ready for another exciting day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questions </t>
+  </si>
+  <si>
+    <t>اسئلة</t>
+  </si>
+  <si>
+    <t>Smart , Ali , was </t>
+  </si>
+  <si>
+    <t>في يوم من الأيام، كان هناك ولد ذكي اسمه علي يحب تعلم أشياء جديدة. كل يوم، كان علي يذهب إلى المدرسة. كان يستيقظ مبكرًا، يأكل موزة على الإفطار، ويركض إلى المدرسة. كان علي يحب دروس اللغة الإنجليزية أكثر من أي شيء آخر. كان يستطيع التحدث بالإنجليزية جيدًا ويستمتع بالتدرب مع أصدقائه.في يوم من الأيام، أعطتهم معلمتهم درسًا خاصًا. قالت، "اليوم، سنكتب قصة قصيرة." كان علي متحمسًا. كان يحب معلمته ودائمًا ما كان ينتبه إلى دروسها. فكر للحظة ثم بدأ يكتب في دفتره، "الولد يأكل التفاحة"، بدأ.في وقت الغداء، جلس علي مع أصدقائه وتحدثوا عن قصصهم. قال لهم بفخر، "أنا أستطيع التحدث بالإنجليزية." اتفقوا جميعًا على أن تعلم الإنجليزية ممتع. بعد المدرسة، ركض علي إلى المنزل ليشارك قصته مع والديه. ابتسمت والدته وقالت، "أنت ذكي جدًا يا علي."قبل الذهاب إلى الفراش، نظر علي إلى الكتاب على الطاولة بجانب سريره. قال لنفسه، "أنا أحب مدرستي ومعلمتي. لا أستطيع الانتظار للأسبوع القادم لأتعلم المزيد." ومع هذا الفكر السعيد، غط في النوم، يحلم بكل الأشياء الجديدة التي سيتعلمها."أراك الأسبوع القادم"، فكر علي وهو يغلق عينيه، مستعدًا ليوم آخر مثير.</t>
+  </si>
+  <si>
+    <t>Breakfast , school, banana</t>
+  </si>
+  <si>
+    <t>English , apple, teacher ​</t>
+  </si>
+  <si>
+    <t>What subject does Ali love the most?​​​ما هو الموضوع الذي يحبه علي أكثر شيء؟,Ali loves ______ lessons the most.</t>
+  </si>
+  <si>
+    <t>What does Ali eat for breakfast?​​ماذا يأكل علي على الإفطار؟,Ali eats a ______  for breakfast.</t>
+  </si>
+  <si>
+    <t>Friends , parents , mother</t>
+  </si>
+  <si>
+    <t>Who did Ali share his story with after school?​مع من شارك علي قصته بعد المدرسة؟​,Ali shared his story with his ______ after school.</t>
+  </si>
+  <si>
+    <t>What did Ali's mother say to him?ماذا قالت والدة علي له؟,Ali's mother said, “_______”</t>
+  </si>
+  <si>
+    <t>You are very smart, Ali​, I can speak English, I can't wait for next week to learn more​</t>
+  </si>
+  <si>
+    <t>Bed , parents, table ​</t>
+  </si>
+  <si>
+    <t>Where was the book that Ali looked at before going to bed?أين كان الكتاب الذي نظر إليه علي قبل الذهاب إلى الفراش؟,The book was on the_______beside his bed.</t>
+  </si>
+  <si>
+    <t>What did Ali say he loves?​ماذا قال علي أنه يحب؟,Ali said “________”</t>
+  </si>
+  <si>
+    <t>I love my school and my teacher,  I can't wait for next week to learn more, Ali who loved to learn new things​</t>
+  </si>
+  <si>
+    <t>What is Ali excited about for next week?عن ماذا كان علي متحمسًا للأسبوع القادم؟,-</t>
+  </si>
+  <si>
+    <t>Ali is excited about learning more next week, Ali thought as he closed his eyes, See you next week​</t>
+  </si>
+  <si>
+    <t>What is the name of the smart boy in the story? ​ما اسم الولد الذكي في القصة؟​,The name of the smart boy is ______ .</t>
+  </si>
+  <si>
+    <t>multipleChoice</t>
   </si>
 </sst>
 </file>
@@ -463,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A4:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,162 +515,432 @@
     <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="4" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I13" s="2"/>
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I15" s="2"/>
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I16" s="2"/>
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I17" s="2"/>

</xml_diff>

<commit_message>
feat: Upload fill in the blanks question to Firestore
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE4BC07-B4B6-FA42-9F1C-2EEC9D8B6340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B34C65-A49E-984B-BA4F-4ED538DE85A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
   <si>
     <t>A1</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Ali is excited about learning more next week, Ali thought as he closed his eyes, See you next week​</t>
+  </si>
+  <si>
+    <t>What is the meaning of the word</t>
+  </si>
+  <si>
+    <t>Special,اشياء ,bed  ,Home ,Happy </t>
+  </si>
+  <si>
+    <t>خاص,Things,فراش,منزل ,سعيد</t>
+  </si>
+  <si>
+    <t>fillTheBlanks</t>
   </si>
   <si>
     <t>What is the name of the smart boy in the story? ​ما اسم الولد الذكي في القصة؟​,The name of the smart boy is ______ .</t>
@@ -503,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -598,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>
@@ -645,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
         <v>3</v>
@@ -692,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L11" t="s">
         <v>3</v>
@@ -739,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
@@ -786,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L13" t="s">
         <v>3</v>
@@ -833,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
         <v>3</v>
@@ -880,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L15" t="s">
         <v>3</v>
@@ -927,29 +939,67 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
         <v>27</v>
       </c>
-      <c r="L16" t="s">
-        <v>3</v>
-      </c>
-      <c r="M16" t="s">
-        <v>3</v>
-      </c>
-      <c r="N16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: upload listening questions to firestore
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B34C65-A49E-984B-BA4F-4ED538DE85A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD2A48-E4EF-ED40-8F37-6F83F2DF884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
+    <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="49">
   <si>
     <t>A1</t>
   </si>
   <si>
+    <t>Listening</t>
+  </si>
+  <si>
     <t>Unit1</t>
   </si>
   <si>
@@ -50,6 +53,31 @@
     <t>-</t>
   </si>
   <si>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>No Intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ملاحظة : هناك ثلاث اقسام للمفردات​
+قسم الجمل و على الطالب حفظها​
+قسم الاسماء و عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
+قسم الافعال و ايضا عليها جمل على الطالب فقط حفظ الكلمات و فهم الجمل ليستطيع تركيب جملته باستخدام الكلمات المعطائة ​
+سوف يتم استخدام المفردات في درس المحادثة لذالك يجي دراستها بجدية </t>
+  </si>
+  <si>
+    <t>The boy eats an apple الولد يأكل التفاحة,The book is on the table الكتاب على الطاولة,I am a student انا تلميذ,I can speak English انا استطيع التحدث بالانجليزية,Come here  تعال الى هنا</t>
+  </si>
+  <si>
+    <t>Teacher معلمة : I love my teacher  انا احب معلمتي,School مدرسة  : I go to school every day  انا اذهب الى المدرسة كل يوم,Smart ذكية  : she is smart هي ذكية,Week اسبوع : see you next week اراك الاسبوع القادم,Lesson درس  : I love English lessons انا احب الدروس الانجليزي</t>
+  </si>
+  <si>
+    <t>No intro</t>
+  </si>
+  <si>
+    <t>Run اركض : I run everyday  انا اركض كل يوم,Eat أكل  : I eat banana انا اكل موزة,Have لدي : they have a dog  لديهم كلب,Write يكتب : she writes on the book هي تكتب على الكتاب,Say يقول : he says hello  هو يقول مرحبا</t>
+  </si>
+  <si>
     <t>passage</t>
   </si>
   <si>
@@ -128,10 +156,37 @@
     <t>fillTheBlanks</t>
   </si>
   <si>
+    <t>vocabulary</t>
+  </si>
+  <si>
+    <t>sentence</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
     <t>What is the name of the smart boy in the story? ​ما اسم الولد الذكي في القصة؟​,The name of the smart boy is ______ .</t>
   </si>
   <si>
     <t>multipleChoice</t>
+  </si>
+  <si>
+    <t>Unit2</t>
+  </si>
+  <si>
+    <t>Nice to meet you سررت بلقائك,How are you ? كيف حالك,I have two cats لدي قطتان​,How old are you ? كم عمرك​,I love playing football احب لعب كرة القدم</t>
+  </si>
+  <si>
+    <t>Ant نملة  :  The ant is very small  النملة صغيرة جدا,Bed فراش  :  My bed is pink فراشي زهري,Circle دائرة :  I drew a circle رسمت دائرة,Door باب  :  Open the door افتح الباب,Egg بيضة   : The chicken is sitting on the egg الدجاجة جالسة على البيضة,Flower وردة  : The flower smells nice الوردة رائحتها جميلة,Gum  علكة : Don’t swallow the gum لا تبلع العلكة,Hot حار   : Be careful it’s too hot انتبه انه حار جدا,Ice ثلج  : I love ice احب الثلج,Juice عصير : I want apple juice اريد عصير تفاح,Key مفتاح : Don’t forget the keys لا تنسى المفاتيح,Lion اسد : The lion is scary الاسد مخيف</t>
+  </si>
+  <si>
+    <t>Mary loves animals. She has two fish , one dog and  two cat . In the farm, she has two cows , and one horse . She has apple tree and flowers in her garden. Her house is big and white . I like to go to her house and play with her ​</t>
+  </si>
+  <si>
+    <t>listening</t>
   </si>
 </sst>
 </file>
@@ -513,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:O17"/>
+  <dimension ref="A4:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,55 +582,192 @@
     <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="1"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="M8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="N8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="O8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -583,46 +775,46 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -630,46 +822,46 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -677,46 +869,46 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -724,46 +916,46 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -771,46 +963,46 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -818,46 +1010,46 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -865,46 +1057,46 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -912,46 +1104,46 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -959,48 +1151,237 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N17" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" t="s">
-        <v>3</v>
-      </c>
-    </row>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
refactor: Update delimiter for splitting question text in
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD2A48-E4EF-ED40-8F37-6F83F2DF884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45BF6D5-88B6-3145-B6B9-544FAC3114D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
   <si>
     <t>A1</t>
   </si>
@@ -66,18 +66,9 @@
 سوف يتم استخدام المفردات في درس المحادثة لذالك يجي دراستها بجدية </t>
   </si>
   <si>
-    <t>The boy eats an apple الولد يأكل التفاحة,The book is on the table الكتاب على الطاولة,I am a student انا تلميذ,I can speak English انا استطيع التحدث بالانجليزية,Come here  تعال الى هنا</t>
-  </si>
-  <si>
-    <t>Teacher معلمة : I love my teacher  انا احب معلمتي,School مدرسة  : I go to school every day  انا اذهب الى المدرسة كل يوم,Smart ذكية  : she is smart هي ذكية,Week اسبوع : see you next week اراك الاسبوع القادم,Lesson درس  : I love English lessons انا احب الدروس الانجليزي</t>
-  </si>
-  <si>
     <t>No intro</t>
   </si>
   <si>
-    <t>Run اركض : I run everyday  انا اركض كل يوم,Eat أكل  : I eat banana انا اكل موزة,Have لدي : they have a dog  لديهم كلب,Write يكتب : she writes on the book هي تكتب على الكتاب,Say يقول : he says hello  هو يقول مرحبا</t>
-  </si>
-  <si>
     <t>passage</t>
   </si>
   <si>
@@ -90,69 +81,15 @@
     <t>Ali ​  Once upon a time, there was a smart boy named Ali who loved to learn new things. Every day, Ali would go to school. He would wake up early, eat a banana for breakfast, and run to school. Ali loved English lessons the most. He could speak English very well and enjoyed practicing with his friends.​  One day, his teacher gave them a special lesson. She said, "Today, we are going to write a short story." Ali was excited. He loved his teacher and always paid attention to her lessons. He thought for a moment and then began to write on his notebook, "The boy eats an apple," he started.​  At lunch, Ali sat with his friends and talked about their stories. "I can speak English," he proudly told them. They all agreed that learning English was fun. After school, Ali ran home to share his story with his parents. His mother smiled and said, "You are very smart, Ali."​  Before going to bed, Ali looked at the book on the table beside his bed. He said to himself, "I love my school and my teacher. I can't wait for next week to learn more." And with that happy thought, he drifted off to sleep, dreaming of all the new things he would learn.​  See you next week, Ali thought, as he closed his eyes, ready for another exciting day.</t>
   </si>
   <si>
-    <t xml:space="preserve">Questions </t>
-  </si>
-  <si>
-    <t>اسئلة</t>
-  </si>
-  <si>
-    <t>Smart , Ali , was </t>
-  </si>
-  <si>
     <t>في يوم من الأيام، كان هناك ولد ذكي اسمه علي يحب تعلم أشياء جديدة. كل يوم، كان علي يذهب إلى المدرسة. كان يستيقظ مبكرًا، يأكل موزة على الإفطار، ويركض إلى المدرسة. كان علي يحب دروس اللغة الإنجليزية أكثر من أي شيء آخر. كان يستطيع التحدث بالإنجليزية جيدًا ويستمتع بالتدرب مع أصدقائه.في يوم من الأيام، أعطتهم معلمتهم درسًا خاصًا. قالت، "اليوم، سنكتب قصة قصيرة." كان علي متحمسًا. كان يحب معلمته ودائمًا ما كان ينتبه إلى دروسها. فكر للحظة ثم بدأ يكتب في دفتره، "الولد يأكل التفاحة"، بدأ.في وقت الغداء، جلس علي مع أصدقائه وتحدثوا عن قصصهم. قال لهم بفخر، "أنا أستطيع التحدث بالإنجليزية." اتفقوا جميعًا على أن تعلم الإنجليزية ممتع. بعد المدرسة، ركض علي إلى المنزل ليشارك قصته مع والديه. ابتسمت والدته وقالت، "أنت ذكي جدًا يا علي."قبل الذهاب إلى الفراش، نظر علي إلى الكتاب على الطاولة بجانب سريره. قال لنفسه، "أنا أحب مدرستي ومعلمتي. لا أستطيع الانتظار للأسبوع القادم لأتعلم المزيد." ومع هذا الفكر السعيد، غط في النوم، يحلم بكل الأشياء الجديدة التي سيتعلمها."أراك الأسبوع القادم"، فكر علي وهو يغلق عينيه، مستعدًا ليوم آخر مثير.</t>
   </si>
   <si>
-    <t>Breakfast , school, banana</t>
-  </si>
-  <si>
-    <t>English , apple, teacher ​</t>
-  </si>
-  <si>
-    <t>What subject does Ali love the most?​​​ما هو الموضوع الذي يحبه علي أكثر شيء؟,Ali loves ______ lessons the most.</t>
-  </si>
-  <si>
-    <t>What does Ali eat for breakfast?​​ماذا يأكل علي على الإفطار؟,Ali eats a ______  for breakfast.</t>
-  </si>
-  <si>
-    <t>Friends , parents , mother</t>
-  </si>
-  <si>
-    <t>Who did Ali share his story with after school?​مع من شارك علي قصته بعد المدرسة؟​,Ali shared his story with his ______ after school.</t>
-  </si>
-  <si>
-    <t>What did Ali's mother say to him?ماذا قالت والدة علي له؟,Ali's mother said, “_______”</t>
-  </si>
-  <si>
-    <t>You are very smart, Ali​, I can speak English, I can't wait for next week to learn more​</t>
-  </si>
-  <si>
-    <t>Bed , parents, table ​</t>
-  </si>
-  <si>
-    <t>Where was the book that Ali looked at before going to bed?أين كان الكتاب الذي نظر إليه علي قبل الذهاب إلى الفراش؟,The book was on the_______beside his bed.</t>
-  </si>
-  <si>
-    <t>What did Ali say he loves?​ماذا قال علي أنه يحب؟,Ali said “________”</t>
-  </si>
-  <si>
-    <t>I love my school and my teacher,  I can't wait for next week to learn more, Ali who loved to learn new things​</t>
-  </si>
-  <si>
-    <t>What is Ali excited about for next week?عن ماذا كان علي متحمسًا للأسبوع القادم؟,-</t>
-  </si>
-  <si>
-    <t>Ali is excited about learning more next week, Ali thought as he closed his eyes, See you next week​</t>
-  </si>
-  <si>
     <t>What is the meaning of the word</t>
   </si>
   <si>
     <t>Special,اشياء ,bed  ,Home ,Happy </t>
   </si>
   <si>
-    <t>خاص,Things,فراش,منزل ,سعيد</t>
-  </si>
-  <si>
     <t>fillTheBlanks</t>
   </si>
   <si>
@@ -168,25 +105,262 @@
     <t>verb</t>
   </si>
   <si>
-    <t>What is the name of the smart boy in the story? ​ما اسم الولد الذكي في القصة؟​,The name of the smart boy is ______ .</t>
-  </si>
-  <si>
     <t>multipleChoice</t>
   </si>
   <si>
     <t>Unit2</t>
   </si>
   <si>
-    <t>Nice to meet you سررت بلقائك,How are you ? كيف حالك,I have two cats لدي قطتان​,How old are you ? كم عمرك​,I love playing football احب لعب كرة القدم</t>
-  </si>
-  <si>
-    <t>Ant نملة  :  The ant is very small  النملة صغيرة جدا,Bed فراش  :  My bed is pink فراشي زهري,Circle دائرة :  I drew a circle رسمت دائرة,Door باب  :  Open the door افتح الباب,Egg بيضة   : The chicken is sitting on the egg الدجاجة جالسة على البيضة,Flower وردة  : The flower smells nice الوردة رائحتها جميلة,Gum  علكة : Don’t swallow the gum لا تبلع العلكة,Hot حار   : Be careful it’s too hot انتبه انه حار جدا,Ice ثلج  : I love ice احب الثلج,Juice عصير : I want apple juice اريد عصير تفاح,Key مفتاح : Don’t forget the keys لا تنسى المفاتيح,Lion اسد : The lion is scary الاسد مخيف</t>
-  </si>
-  <si>
     <t>Mary loves animals. She has two fish , one dog and  two cat . In the farm, she has two cows , and one horse . She has apple tree and flowers in her garden. Her house is big and white . I like to go to her house and play with her ​</t>
   </si>
   <si>
     <t>listening</t>
+  </si>
+  <si>
+    <t>word </t>
+  </si>
+  <si>
+    <t>Unit3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarah </t>
+  </si>
+  <si>
+    <t>سارة </t>
+  </si>
+  <si>
+    <t>Sara was born in a small town. She lives in a cozy house with her family. Every morning, she wakes up early to study and do her homework. She likes to read books and learn new things.​  One day, Sara realized she needed a big box to organize her toys and books. She decided to go to the store nearby to find one. When she arrived at the store, she met her friend Ali. Ali was also looking for something at the store.​  Sara and Ali talked for a while and then Ali had a great idea. He suggested they have a party at Sara's house on the weekend. Sara loved the idea and agreed. They bought the box and some decorations for the party.​  On Saturday morning, Sara and Ali started preparing for the party. They decorated the wall with colorful balloons and streamers. They set up games and prepared snacks for their friends. By the afternoon, everything was ready.​  Their friends arrived, and everyone was excited. They played games, danced to music, and enjoyed delicious snacks. The party was a huge success. Sara was very happy to see everyone having fun.​  After the party, Sara and Ali sat down and talked about their day. They were tired but very satisfied. It was a wonderful day filled with joy and laughter. Sara realized how much she enjoyed spending time with her friends and making happy memories.</t>
+  </si>
+  <si>
+    <t>ولدت سارة في بلدة صغيرة. تعيش في بيت مريح مع عائلتها. كل صباح، تستيقظ مبكرًا لتدرس وتقوم بواجبها المنزلي. تحب قراءة الكتب وتعلم أشياء جديدة.​  في أحد الأيام، أدركت سارة أنها تحتاج إلى صندوق كبير لتنظيم ألعابها وكتبها. قررت الذهاب إلى المتجر القريب لتجد واحدًا. عندما وصلت إلى المتجر، التقت بصديقها علي. كان علي يبحث أيضًا عن شيء في المتجر.​  تحدثت سارة وعلي لفترة، ثم خطرت لعلي فكرة رائعة. اقترح إقامة حفلة في بيت سارة في نهاية الأسبوع. أحبت سارة الفكرة ووافقت. اشتروا الصندوق وبعض الزينة للحفلة.​  في صباح السبت، بدأت سارة وعلي التحضير للحفلة. زينوا الجدار ببالونات ملونة وشرائط. أعدوا الألعاب وجهزوا وجبات خفيفة لأصدقائهم. بحلول فترة الظهيرة، كان كل شيء جاهزًا.​  وصل أصدقاؤهم، وكان الجميع متحمسًا. لعبوا الألعاب، ورقصوا على الموسيقى، واستمتعوا بالوجبات اللذيذة. كانت الحفلة ناجحة جدًا. كانت سارة سعيدة جدًا برؤية الجميع يستمتعون بوقتهم.​  بعد الحفلة، جلست سارة وعلي وتحدثا عن يومهما. كانا متعبين لكن راضيين جدًا. كان يومًا رائعًا مليئًا بالفرح والضحك. أدركت سارة كم تستمتع بقضاء الوقت مع أصدقائها وصنع ذكريات سعيدة.</t>
+  </si>
+  <si>
+    <t>Where was Sara born?</t>
+  </si>
+  <si>
+    <t>أين وُلدت سارة؟​</t>
+  </si>
+  <si>
+    <t>Sara was born in a________.​</t>
+  </si>
+  <si>
+    <t>Who does Sara live with?​</t>
+  </si>
+  <si>
+    <t>مَع من تعيش سارة؟</t>
+  </si>
+  <si>
+    <t>What does Sara do every morning?​</t>
+  </si>
+  <si>
+    <t>ماذا تفعل سارة كل صباح؟</t>
+  </si>
+  <si>
+    <t>Why did Sara go to the store?​</t>
+  </si>
+  <si>
+    <t>لماذا ذهبت سارة إلى المتجر؟</t>
+  </si>
+  <si>
+    <t>Who did Sara meet at the store?​</t>
+  </si>
+  <si>
+    <t>من التقت بها سارة في المتجر؟</t>
+  </si>
+  <si>
+    <t>What idea did Ali have at the store?​</t>
+  </si>
+  <si>
+    <t>ما هي الفكرة التي كانت لدى علي في المتجر؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Where did Sara and Ali decide to have the party? ​</t>
+  </si>
+  <si>
+    <t>أين قررت سارة وعلي إقامة الحفلة؟</t>
+  </si>
+  <si>
+    <t>What did Sara and Ali buy at the store?​</t>
+  </si>
+  <si>
+    <t>ماذا اشتروا سارة وعلي من المتجر؟</t>
+  </si>
+  <si>
+    <t>How did Sara and Ali decorate for the party?​</t>
+  </si>
+  <si>
+    <t>كيف زينت سارة وعلي للحفلة؟</t>
+  </si>
+  <si>
+    <t>What did they do at the party?​</t>
+  </si>
+  <si>
+    <t>ماذا فعلوا في الحفلة؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> How did Sara feel after the party?​</t>
+  </si>
+  <si>
+    <t>كيف شعرت سارة بعد الحفلة؟</t>
+  </si>
+  <si>
+    <t>tired but very satisfied;​  Sara loved the idea and agreed;​  Sara was very happy to see everyone having fun;</t>
+  </si>
+  <si>
+    <t>What did Sara realize about her day with Ali?​</t>
+  </si>
+  <si>
+    <t>ماذا أدركت سارة عن يومها مع علي؟</t>
+  </si>
+  <si>
+    <t>They were tired but very satisfied. It was a wonderful day filled with joy and laughter;​  Sara realized how much she enjoyed spending time with her friends;​  Sara was born in a small town;</t>
+  </si>
+  <si>
+    <t>The boy eats an apple الولد يأكل التفاحة;The book is on the table الكتاب على الطاولة;I am a student انا تلميذ,I can speak English انا استطيع التحدث بالانجليزية;Come here  تعال الى هنا</t>
+  </si>
+  <si>
+    <t>Teacher معلمة : I love my teacher  انا احب معلمتي;School مدرسة  : I go to school every day  انا اذهب الى المدرسة كل يوم;Smart ذكية  : she is smart هي ذكية;Week اسبوع : see you next week اراك الاسبوع القادم;Lesson درس  : I love English lessons انا احب الدروس الانجليزي</t>
+  </si>
+  <si>
+    <t>Run اركض : I run everyday  انا اركض كل يوم;Eat أكل  : I eat banana انا اكل موزة;Have لدي : they have a dog  لديهم كلب;Write يكتب : she writes on the book هي تكتب على الكتاب;Say يقول : he says hello  هو يقول مرحبا</t>
+  </si>
+  <si>
+    <t>What is the name of the smart boy in the story?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ​​The name of the smart boy is ______ .</t>
+  </si>
+  <si>
+    <t>ما اسم الولد الذكي في القصة؟</t>
+  </si>
+  <si>
+    <t>What does Ali eat for breakfast?</t>
+  </si>
+  <si>
+    <t>ماذا يأكل علي على الإفطار؟</t>
+  </si>
+  <si>
+    <t>​​Ali eats a ______  for breakfast.</t>
+  </si>
+  <si>
+    <t>What subject does Ali love the most?</t>
+  </si>
+  <si>
+    <t>ما هو الموضوع الذي يحبه علي أكثر شيء؟</t>
+  </si>
+  <si>
+    <t>​​​Ali loves ______ lessons the most.</t>
+  </si>
+  <si>
+    <t>Who did Ali share his story with after school?</t>
+  </si>
+  <si>
+    <t>​Ali shared his story with his ______ after school.</t>
+  </si>
+  <si>
+    <t>​مع من شارك علي قصته بعد المدرسة؟</t>
+  </si>
+  <si>
+    <t>What did Ali's mother say to him?</t>
+  </si>
+  <si>
+    <t>ماذا قالت والدة علي له؟</t>
+  </si>
+  <si>
+    <t>Ali's mother said, “_______”</t>
+  </si>
+  <si>
+    <t>Where was the book that Ali looked at before going to bed?</t>
+  </si>
+  <si>
+    <t>The book was on the_______beside his bed.</t>
+  </si>
+  <si>
+    <t>أين كان الكتاب الذي نظر إليه علي قبل الذهاب إلى الفراش؟</t>
+  </si>
+  <si>
+    <t>What did Ali say he loves?</t>
+  </si>
+  <si>
+    <t>​Ali said “________”</t>
+  </si>
+  <si>
+    <t>ماذا قال علي أنه يحب؟</t>
+  </si>
+  <si>
+    <t>What is Ali excited about for next week?</t>
+  </si>
+  <si>
+    <t>عن ماذا كان علي متحمسًا للأسبوع القادم؟</t>
+  </si>
+  <si>
+    <t>Smart ; Ali ; was </t>
+  </si>
+  <si>
+    <t>Breakfast ; school; banana</t>
+  </si>
+  <si>
+    <t>English ;apple;teacher ​</t>
+  </si>
+  <si>
+    <t>Friends ; parents ; mother</t>
+  </si>
+  <si>
+    <t>You are very smart; Ali​; I can speak English;I can't wait for next week to learn more​</t>
+  </si>
+  <si>
+    <t>Bed; parents; table ​</t>
+  </si>
+  <si>
+    <t>I love my school and my teacher;  I can't wait for next week to learn more; Ali who loved to learn new things​</t>
+  </si>
+  <si>
+    <t>Ali is excited about learning more next week; Ali thought as he closed his eyes; See you next week​</t>
+  </si>
+  <si>
+    <t>خاص ;Things;فراش;منزل ;سعيد</t>
+  </si>
+  <si>
+    <t>Nice to meet you سررت بلقائك;How are you ? كيف حالك;I have two cats لدي قطتان​;How old are you ? كم عمرك​;I love playing football احب لعب كرة القدم</t>
+  </si>
+  <si>
+    <t>Ant نملة  :  The ant is very small  النملة صغيرة جدا;Bed فراش  :  My bed is pink فراشي زهري;Circle دائرة :  I drew a circle رسمت دائرة;Door باب  :  Open the door افتح الباب;Egg بيضة   : The chicken is sitting on the egg الدجاجة جالسة على البيضة;Flower وردة  : The flower smells nice الوردة رائحتها جميلة,Gum  علكة : Don’t swallow the gum لا تبلع العلكة,Hot حار   : Be careful it’s too hot انتبه انه حار جدا,Ice ثلج  : I love ice احب الثلج,Juice عصير : I want apple juice اريد عصير تفاح,Key مفتاح : Don’t forget the keys لا تنسى المفاتيح,Lion اسد : The lion is scary الاسد مخيف</t>
+  </si>
+  <si>
+    <t>Box صندوق  :  The cat is in the box القطة في الصندوق;Wall حائط    :  There is an insect on the wall هناك حشرة على الحائط;Party حفلة    :  You are invited to the party انت معزوم للحفلة;Homework وظيفة :    Did you do your homework ? هل حليت و ظيفتك ؟;Store متجر :    Is the store open ? هل المتجر مفتوح ؟</t>
+  </si>
+  <si>
+    <t>To live  يعيش : I live in Turkey انا اعيش في تركيا;Born ولد : I was born in Germany ولدت في المانيا;Meet يلتقي : I meet my friends in school التقي باصدقائي في المدرسة;Wake up يستيقظ  : She wakes up early هي تستيقظ باكرا;Study يدرس : We study hard for the test ندرس باجتهاد للامتحان</t>
+  </si>
+  <si>
+    <t>Where is the book ?اين الكتاب;When were you born? متى و لدت;When does the store open ? متى يفتح المتجر;Where are you from ? من اين انت;Where are you ? اين انت</t>
+  </si>
+  <si>
+    <t>Cozy house; small town; her family​</t>
+  </si>
+  <si>
+    <t>Read books and learn new things; wakes up early and do her homework </t>
+  </si>
+  <si>
+    <t>To buy a box ; to meet her friend ​</t>
+  </si>
+  <si>
+    <t>Ali; Sarah; her mom</t>
+  </si>
+  <si>
+    <t>Sara and Ali talked for a while;​   to have a party at Sara's house ;​  to bring the box and some decorations</t>
+  </si>
+  <si>
+    <t>Ali’s house ; Sarah’s house ​</t>
+  </si>
+  <si>
+    <t>big box and some decorations; idea; colorful balloons and streamers​</t>
+  </si>
+  <si>
+    <t>Sara and Ali sat down and talked about their day.;​    They played games, danced to music, and enjoyed delicious snacks.;​    Sara realized how much she enjoyed spending time with her friends;</t>
+  </si>
+  <si>
+    <t>They decorated the wall with colorful balloons and streamers;​    They played games, danced to music, and enjoyed delicious snacks;​    Sara and Ali sat down and talked about their day;</t>
   </si>
 </sst>
 </file>
@@ -568,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:O23"/>
+  <dimension ref="A4:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,13 +773,13 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -614,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
         <v>4</v>
@@ -646,13 +820,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -661,7 +835,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -687,19 +861,19 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -708,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
@@ -755,19 +929,19 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>13</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -787,22 +961,22 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L9" t="s">
         <v>4</v>
@@ -834,22 +1008,22 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L10" t="s">
         <v>4</v>
@@ -881,22 +1055,22 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>21</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>43</v>
       </c>
       <c r="L11" t="s">
         <v>4</v>
@@ -928,22 +1102,22 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L12" t="s">
         <v>4</v>
@@ -975,22 +1149,22 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L13" t="s">
         <v>4</v>
@@ -1022,22 +1196,22 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L14" t="s">
         <v>4</v>
@@ -1069,22 +1243,22 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L15" t="s">
         <v>4</v>
@@ -1116,22 +1290,22 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L16" t="s">
         <v>4</v>
@@ -1163,22 +1337,22 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="J17" t="s">
         <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="L17" t="s">
         <v>4</v>
@@ -1201,7 +1375,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1210,13 +1384,13 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="I19" t="s">
         <v>4</v>
@@ -1225,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L19" t="s">
         <v>4</v>
@@ -1248,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1257,13 +1431,13 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="I20" t="s">
         <v>4</v>
@@ -1272,7 +1446,7 @@
         <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L20" t="s">
         <v>4</v>
@@ -1295,22 +1469,22 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I21" t="s">
         <v>4</v>
@@ -1319,7 +1493,7 @@
         <v>4</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
@@ -1342,46 +1516,798 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" t="s">
+        <v>4</v>
+      </c>
+      <c r="O24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" t="s">
+        <v>4</v>
+      </c>
+      <c r="O25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" t="s">
+        <v>98</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>100</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" t="s">
+        <v>4</v>
+      </c>
+      <c r="N33" t="s">
+        <v>4</v>
+      </c>
+      <c r="O33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>4</v>
+      </c>
+      <c r="O34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" t="s">
         <v>47</v>
       </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" t="s">
+        <v>4</v>
+      </c>
+      <c r="M35" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
         <v>48</v>
       </c>
-      <c r="L22" t="s">
-        <v>4</v>
-      </c>
-      <c r="M22" t="s">
-        <v>4</v>
-      </c>
-      <c r="N22" t="s">
-        <v>4</v>
-      </c>
-      <c r="O22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" t="s">
+        <v>4</v>
+      </c>
+      <c r="M38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" t="s">
+        <v>4</v>
+      </c>
+      <c r="M39" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" t="s">
+        <v>4</v>
+      </c>
+      <c r="O39" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
refactor: support nullable fields in different models
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45BF6D5-88B6-3145-B6B9-544FAC3114D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747B8CC-7BE7-8E4B-B476-1AB6A40F0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
refactor: Update word field in ListeningQuestionModel to accept multiple words
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747B8CC-7BE7-8E4B-B476-1AB6A40F0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006345E5-B90E-554B-B765-657A7342E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="149">
   <si>
     <t>A1</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Vocabulary</t>
-  </si>
-  <si>
-    <t>No Intro</t>
   </si>
   <si>
     <t xml:space="preserve">ملاحظة : هناك ثلاث اقسام للمفردات​
@@ -66,9 +63,6 @@
 سوف يتم استخدام المفردات في درس المحادثة لذالك يجي دراستها بجدية </t>
   </si>
   <si>
-    <t>No intro</t>
-  </si>
-  <si>
     <t>passage</t>
   </si>
   <si>
@@ -361,6 +355,138 @@
   </si>
   <si>
     <t>They decorated the wall with colorful balloons and streamers;​    They played games, danced to music, and enjoyed delicious snacks;​    Sara and Ali sat down and talked about their day;</t>
+  </si>
+  <si>
+    <t>Unit4</t>
+  </si>
+  <si>
+    <t>Milk  حليب:  I drink milk before sleeping  انا اشرب الحليب قبل النوم;Numbers  ارقام : I know numbers in Italian  اعلم الارقام بالايطالية;Olive  زيتون : I eat olive during breakfast  اكل زيتون على الفطور;People ناس  : There are many people in here  هناك الكثير من الناس هنا;Queen ملكة : The queen died last year الملكة ماتت العام الماضي;Rainbow قوس قزح : There is a rainbow outside  هناك قوس قزح بالخارج;Spoon  حساء  : Soup is eaten with a spoon  الحساء يأكل بالملعقة;Turtle  سلحفاة :  Turtles walk so slow السلاحف يمشون ببطئ;Umbrella   مظلة :  Don’t forget your umbrella لاتنسى مظلتك;Voice  صوت  : She has a nice voice لديها صوت جميل;Water  ماء : Water is so important الماء مهم جدا;Yogurt لبن : We need to bring Yogurt نحتاج الى شراء اللبن</t>
+  </si>
+  <si>
+    <t>Don’t forget your umbrella لاتنسى مظلتك;Water is so important الماء مهم جدا;She has a nice voice لديها صوت جميل;There are many people in here  هناك الكثير من الناس هنا</t>
+  </si>
+  <si>
+    <t>Lina wakes up early. She drinks a glass of milk. She likes milk very much.;Lina sees her pet turtle in the garden. The turtle is slow but cute. Lina counts the flowers in the garden. The number of flowers is five.;Lina goes to the kitchen. She takes a spoon and eats yogurt for breakfast.; She also eats some olives. Olives are the best .</t>
+  </si>
+  <si>
+    <t>Unit5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Unit5</t>
+  </si>
+  <si>
+    <t>Beautiful جميل:  She is very beautiful  هي جميلة جدا ;Tall طويل : I am a tall man انا رجل طويل ;Blond اشقر :  Her friend is blond  صديقتها شقراء ;Blond اشقر :  Her friend is blond  صديقتها شقراء ;Hospital مستشفى : We are going to the hospital  ذاهبون الى المستشفى ;Kiss قبلة : The kid gave her dad a kiss  الطفلة اعطت ابها قبلة</t>
+  </si>
+  <si>
+    <t>I am 10 years old انا عمري عشر سنوات;Can you help me ?هل يمكنك مساعدتي;This gift is for you هذه الهدية لك;I talked to him انا تحدثت معه</t>
+  </si>
+  <si>
+    <t>Sarah and I ​</t>
+  </si>
+  <si>
+    <t>انا و سارة ​</t>
+  </si>
+  <si>
+    <t>My name is Emma. I am seven years old. I have a beautiful, tall, blond friend named Sarah. Sarah is very nice and always helps me.​  One day, Sarah got sick and went to the hospital. I was very worried about her. I wanted to know if she was okay, so I asked my mom to call the hospital. The nurse said Sarah was fine and could come home soon.​  When Sarah came back home, I was so happy! I went to her house to see her. I talked to her and told her how much I missed her. She gave me a big kiss on the cheek and said, "Thank you for caring about me."​  Sarah loves to learn new things. She likes to teach me what she learns at school. She teaches me how to read and write. I am very lucky to have a friend like her.​  On Sarah's birthday, I wanted to give her a special gift. I asked my mom, "Can you help me find a gift for Sarah?" We went to the store and found a beautiful book. I said, "This gift is for you, Sarah. I hope you like it."​  Sarah was very happy and gave me a big hug. She said, "Thank you, Emma. You are the best friend ever." I felt so happy and proud.</t>
+  </si>
+  <si>
+    <t>اسمي إيما. عمري سبع سنوات. لدي صديقة جميلة، طويلة، وشقراء اسمها سارة. سارة لطيفة جدًا وتساعدني دائمًا.​  في أحد الأيام، مرضت سارة وذهبت إلى المستشفى. كنت قلقة جدًا عليها. أردت أن أعرف إذا كانت بخير، لذا طلبت من أمي أن تتصل بالمستشفى. قالت الممرضة إن سارة بخير ويمكنها العودة إلى المنزل قريبًا.​  عندما عادت سارة إلى المنزل، كنت سعيدة جدًا! ذهبت إلى منزلها لرؤيتها. تحدثت معها وأخبرتها كم اشتقت إليها. أعطتني قبلة كبيرة على الخد وقالت، "شكرًا لاهتمامك بي."​  تحب سارة تعلم أشياء جديدة. تحب أن تعلمني ما تتعلمه في المدرسة. تعلمني كيف أقرأ وأكتب. أنا محظوظة جدًا بوجود صديقة مثلها.​  في عيد ميلاد سارة، أردت أن أقدم لها هدية خاصة. سألت أمي، "هل يمكنك مساعدتي في العثور على هدية لسارة؟" ذهبنا إلى المتجر ووجدنا كتابًا جميلًا. قلت، "هذه الهدية لكِ، سارة. أتمنى أن تعجبكِ."​  كانت سارة سعيدة جدًا وعانقتني بقوة. قالت، "شكرًا لكِ، إيما. أنتِ أفضل صديقة على الإطلاق." شعرت بالسعادة والفخر.</t>
+  </si>
+  <si>
+    <t>How old is Emma?</t>
+  </si>
+  <si>
+    <t>كم عمر إيما؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>Five years old;Seven years old;Ten years old</t>
+  </si>
+  <si>
+    <t>ما اسم صديقة إيما؟</t>
+  </si>
+  <si>
+    <t>What is the name of Emma's friend?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> أين ذهبت سارة عندما مرضت؟</t>
+  </si>
+  <si>
+    <t>Where did Sarah go when she got sick?</t>
+  </si>
+  <si>
+    <t>Who did Emma ask to call the hospital?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> من طلبت إيما أن يتصل بالمستشفى؟</t>
+  </si>
+  <si>
+    <t>What did Sarah do when Emma visited her at home?</t>
+  </si>
+  <si>
+    <t>ماذا فعلت سارة عندما زارتها إيما في المنزل؟</t>
+  </si>
+  <si>
+    <t>What does Sarah like to do?</t>
+  </si>
+  <si>
+    <t>ماذا تحب سارة أن تفعل؟</t>
+  </si>
+  <si>
+    <t>What did Emma give Sarah for her birthday?</t>
+  </si>
+  <si>
+    <t>ماذا قدمت إيما لسارة في عيد ميلادها؟</t>
+  </si>
+  <si>
+    <t>How did Sarah feel about the gift?</t>
+  </si>
+  <si>
+    <t>كيف شعرت سارة بشأن الهدية؟</t>
+  </si>
+  <si>
+    <t>What did Emma ask her mom to help with?</t>
+  </si>
+  <si>
+    <t>بماذا طلبت إيما من والدتها المساعدة؟</t>
+  </si>
+  <si>
+    <t>What did Emma feel after giving the gift to Sarah?</t>
+  </si>
+  <si>
+    <t>ماذا شعرت إيما بعد أن قدمت الهدية لسارة؟</t>
+  </si>
+  <si>
+    <t>Lily;Sarah;Anna</t>
+  </si>
+  <si>
+    <t>To the park;To the hospital;To the school</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Her dad;Her mom;Her teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> She gave Emma a toy;She gave Emma a big kiss on the cheek;She made a cake</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To swim; To learn new things and teach Emma;To play video games​</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A beautiful book;A new dress;A toy car</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> She was sad;She was very happy and gave Emma a big hug;She was angry​</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To cook dinner;To find a gift for Sarah;To clean the house</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sad;Proud and happy;Nervous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To talk يتكلم : I talk to my mom daily اتكلم مع امي يوميا;To call يتصل : She called me when I was out اتصلت بي عندما كنت بالخارج;To know يعلم : I know your secret اعلم سرك;To learn يتعلم : Many students learn English الكثير من التلامذ يتعلمون الإنجليزية;To teach يعلم : My teacher teaches us معلمتي تعلمنا </t>
   </si>
 </sst>
 </file>
@@ -742,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:O39"/>
+  <dimension ref="A4:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,19 +893,19 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -788,7 +914,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
         <v>4</v>
@@ -814,19 +940,19 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -835,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -861,19 +987,19 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -882,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
@@ -929,19 +1055,19 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>10</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>11</v>
-      </c>
-      <c r="N8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -961,22 +1087,22 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
-        <v>63</v>
-      </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L9" t="s">
         <v>4</v>
@@ -1008,22 +1134,22 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
         <v>64</v>
       </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>66</v>
-      </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
         <v>4</v>
@@ -1055,22 +1181,22 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
       <c r="I11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L11" t="s">
         <v>4</v>
@@ -1102,22 +1228,22 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
         <v>70</v>
       </c>
-      <c r="G12" t="s">
-        <v>72</v>
-      </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L12" t="s">
         <v>4</v>
@@ -1149,22 +1275,22 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" t="s">
         <v>73</v>
       </c>
-      <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L13" t="s">
         <v>4</v>
@@ -1196,22 +1322,22 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
         <v>76</v>
       </c>
-      <c r="G14" t="s">
-        <v>78</v>
-      </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
         <v>4</v>
@@ -1243,22 +1369,22 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
         <v>79</v>
       </c>
-      <c r="G15" t="s">
-        <v>81</v>
-      </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L15" t="s">
         <v>4</v>
@@ -1290,22 +1416,22 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L16" t="s">
         <v>4</v>
@@ -1337,22 +1463,22 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
         <v>14</v>
-      </c>
-      <c r="G17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" t="s">
-        <v>16</v>
       </c>
       <c r="L17" t="s">
         <v>4</v>
@@ -1375,22 +1501,22 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I19" t="s">
         <v>4</v>
@@ -1399,7 +1525,7 @@
         <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L19" t="s">
         <v>4</v>
@@ -1422,22 +1548,22 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
         <v>4</v>
@@ -1446,7 +1572,7 @@
         <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L20" t="s">
         <v>4</v>
@@ -1469,22 +1595,22 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s">
         <v>4</v>
@@ -1493,7 +1619,7 @@
         <v>4</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
@@ -1516,31 +1642,31 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
         <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" t="s">
-        <v>24</v>
       </c>
       <c r="L22" t="s">
         <v>4</v>
@@ -1564,22 +1690,22 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I24" t="s">
         <v>4</v>
@@ -1588,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="K24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L24" t="s">
         <v>4</v>
@@ -1611,22 +1737,22 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I25" t="s">
         <v>4</v>
@@ -1635,7 +1761,7 @@
         <v>4</v>
       </c>
       <c r="K25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L25" t="s">
         <v>4</v>
@@ -1658,22 +1784,22 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I26" t="s">
         <v>4</v>
@@ -1682,7 +1808,7 @@
         <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L26" t="s">
         <v>4</v>
@@ -1705,43 +1831,43 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" t="s">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>27</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>28</v>
-      </c>
-      <c r="N27" t="s">
-        <v>29</v>
-      </c>
-      <c r="O27" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -1752,7 +1878,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -1761,22 +1887,22 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
         <v>31</v>
       </c>
-      <c r="G28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" t="s">
-        <v>33</v>
-      </c>
       <c r="I28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L28" t="s">
         <v>4</v>
@@ -1799,7 +1925,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -1808,22 +1934,22 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J29">
         <v>2</v>
       </c>
       <c r="K29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L29" t="s">
         <v>4</v>
@@ -1846,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -1855,22 +1981,22 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L30" t="s">
         <v>4</v>
@@ -1893,7 +2019,7 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -1902,22 +2028,22 @@
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L31" t="s">
         <v>4</v>
@@ -1940,7 +2066,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -1949,22 +2075,22 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L32" t="s">
         <v>4</v>
@@ -1987,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -1996,22 +2122,22 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L33" t="s">
         <v>4</v>
@@ -2034,7 +2160,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -2043,22 +2169,22 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J34">
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L34" t="s">
         <v>4</v>
@@ -2081,7 +2207,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -2090,22 +2216,22 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H35" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
       <c r="K35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L35" t="s">
         <v>4</v>
@@ -2128,7 +2254,7 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -2137,22 +2263,22 @@
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H36" t="s">
         <v>4</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L36" t="s">
         <v>4</v>
@@ -2175,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -2184,22 +2310,22 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L37" t="s">
         <v>4</v>
@@ -2222,7 +2348,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -2231,22 +2357,22 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G38" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L38" t="s">
         <v>4</v>
@@ -2269,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -2278,22 +2404,22 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G39" t="s">
-        <v>56</v>
-      </c>
-      <c r="H39" t="s">
-        <v>4</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="J39">
         <v>0</v>
       </c>
       <c r="K39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L39" t="s">
         <v>4</v>
@@ -2307,6 +2433,811 @@
       <c r="O39" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M40" t="s">
+        <v>4</v>
+      </c>
+      <c r="N40" t="s">
+        <v>4</v>
+      </c>
+      <c r="O40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>107</v>
+      </c>
+      <c r="I41" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" t="s">
+        <v>4</v>
+      </c>
+      <c r="N41" t="s">
+        <v>4</v>
+      </c>
+      <c r="O41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" t="s">
+        <v>4</v>
+      </c>
+      <c r="M42" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" t="s">
+        <v>4</v>
+      </c>
+      <c r="O42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>111</v>
+      </c>
+      <c r="I44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" t="s">
+        <v>4</v>
+      </c>
+      <c r="N44" t="s">
+        <v>4</v>
+      </c>
+      <c r="O44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J45" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" t="s">
+        <v>15</v>
+      </c>
+      <c r="L45" t="s">
+        <v>4</v>
+      </c>
+      <c r="M45" t="s">
+        <v>4</v>
+      </c>
+      <c r="N45" t="s">
+        <v>4</v>
+      </c>
+      <c r="O45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>148</v>
+      </c>
+      <c r="I46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K46" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" t="s">
+        <v>4</v>
+      </c>
+      <c r="M46" t="s">
+        <v>4</v>
+      </c>
+      <c r="N46" t="s">
+        <v>4</v>
+      </c>
+      <c r="O46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" t="s">
+        <v>4</v>
+      </c>
+      <c r="K47" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47" t="s">
+        <v>113</v>
+      </c>
+      <c r="M47" t="s">
+        <v>114</v>
+      </c>
+      <c r="N47" t="s">
+        <v>115</v>
+      </c>
+      <c r="O47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" t="s">
+        <v>118</v>
+      </c>
+      <c r="H48" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48" t="s">
+        <v>120</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" t="s">
+        <v>4</v>
+      </c>
+      <c r="M48" t="s">
+        <v>4</v>
+      </c>
+      <c r="N48" t="s">
+        <v>4</v>
+      </c>
+      <c r="O48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>122</v>
+      </c>
+      <c r="G49" t="s">
+        <v>121</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>139</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" t="s">
+        <v>4</v>
+      </c>
+      <c r="M49" t="s">
+        <v>4</v>
+      </c>
+      <c r="N49" t="s">
+        <v>4</v>
+      </c>
+      <c r="O49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>140</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" t="s">
+        <v>4</v>
+      </c>
+      <c r="M50" t="s">
+        <v>4</v>
+      </c>
+      <c r="N50" t="s">
+        <v>4</v>
+      </c>
+      <c r="O50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>141</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" t="s">
+        <v>4</v>
+      </c>
+      <c r="M51" t="s">
+        <v>4</v>
+      </c>
+      <c r="N51" t="s">
+        <v>4</v>
+      </c>
+      <c r="O51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" t="s">
+        <v>128</v>
+      </c>
+      <c r="H52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" t="s">
+        <v>142</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M52" t="s">
+        <v>4</v>
+      </c>
+      <c r="N52" t="s">
+        <v>4</v>
+      </c>
+      <c r="O52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" t="s">
+        <v>4</v>
+      </c>
+      <c r="M53" t="s">
+        <v>4</v>
+      </c>
+      <c r="N53" t="s">
+        <v>4</v>
+      </c>
+      <c r="O53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" t="s">
+        <v>132</v>
+      </c>
+      <c r="H54" t="s">
+        <v>4</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L54" t="s">
+        <v>4</v>
+      </c>
+      <c r="M54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N54" t="s">
+        <v>4</v>
+      </c>
+      <c r="O54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" t="s">
+        <v>134</v>
+      </c>
+      <c r="H55" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55" t="s">
+        <v>4</v>
+      </c>
+      <c r="M55" t="s">
+        <v>4</v>
+      </c>
+      <c r="N55" t="s">
+        <v>4</v>
+      </c>
+      <c r="O55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" t="s">
+        <v>136</v>
+      </c>
+      <c r="H56" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56" t="s">
+        <v>4</v>
+      </c>
+      <c r="M56" t="s">
+        <v>4</v>
+      </c>
+      <c r="N56" t="s">
+        <v>4</v>
+      </c>
+      <c r="O56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>137</v>
+      </c>
+      <c r="G57" t="s">
+        <v>138</v>
+      </c>
+      <c r="H57" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" t="s">
+        <v>4</v>
+      </c>
+      <c r="M57" t="s">
+        <v>4</v>
+      </c>
+      <c r="N57" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I59" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: add initial test data to Excel file
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006345E5-B90E-554B-B765-657A7342E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E056E7-BEC9-6847-9355-7D72382993CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
+    <workbookView xWindow="38640" yWindow="3100" windowWidth="33360" windowHeight="20260" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="202">
   <si>
     <t>A1</t>
   </si>
@@ -72,9 +72,6 @@
     <t>علي </t>
   </si>
   <si>
-    <t>Ali ​  Once upon a time, there was a smart boy named Ali who loved to learn new things. Every day, Ali would go to school. He would wake up early, eat a banana for breakfast, and run to school. Ali loved English lessons the most. He could speak English very well and enjoyed practicing with his friends.​  One day, his teacher gave them a special lesson. She said, "Today, we are going to write a short story." Ali was excited. He loved his teacher and always paid attention to her lessons. He thought for a moment and then began to write on his notebook, "The boy eats an apple," he started.​  At lunch, Ali sat with his friends and talked about their stories. "I can speak English," he proudly told them. They all agreed that learning English was fun. After school, Ali ran home to share his story with his parents. His mother smiled and said, "You are very smart, Ali."​  Before going to bed, Ali looked at the book on the table beside his bed. He said to himself, "I love my school and my teacher. I can't wait for next week to learn more." And with that happy thought, he drifted off to sleep, dreaming of all the new things he would learn.​  See you next week, Ali thought, as he closed his eyes, ready for another exciting day.</t>
-  </si>
-  <si>
     <t>في يوم من الأيام، كان هناك ولد ذكي اسمه علي يحب تعلم أشياء جديدة. كل يوم، كان علي يذهب إلى المدرسة. كان يستيقظ مبكرًا، يأكل موزة على الإفطار، ويركض إلى المدرسة. كان علي يحب دروس اللغة الإنجليزية أكثر من أي شيء آخر. كان يستطيع التحدث بالإنجليزية جيدًا ويستمتع بالتدرب مع أصدقائه.في يوم من الأيام، أعطتهم معلمتهم درسًا خاصًا. قالت، "اليوم، سنكتب قصة قصيرة." كان علي متحمسًا. كان يحب معلمته ودائمًا ما كان ينتبه إلى دروسها. فكر للحظة ثم بدأ يكتب في دفتره، "الولد يأكل التفاحة"، بدأ.في وقت الغداء، جلس علي مع أصدقائه وتحدثوا عن قصصهم. قال لهم بفخر، "أنا أستطيع التحدث بالإنجليزية." اتفقوا جميعًا على أن تعلم الإنجليزية ممتع. بعد المدرسة، ركض علي إلى المنزل ليشارك قصته مع والديه. ابتسمت والدته وقالت، "أنت ذكي جدًا يا علي."قبل الذهاب إلى الفراش، نظر علي إلى الكتاب على الطاولة بجانب سريره. قال لنفسه، "أنا أحب مدرستي ومعلمتي. لا أستطيع الانتظار للأسبوع القادم لأتعلم المزيد." ومع هذا الفكر السعيد، غط في النوم، يحلم بكل الأشياء الجديدة التي سيتعلمها."أراك الأسبوع القادم"، فكر علي وهو يغلق عينيه، مستعدًا ليوم آخر مثير.</t>
   </si>
   <si>
@@ -487,13 +484,263 @@
   </si>
   <si>
     <t xml:space="preserve">To talk يتكلم : I talk to my mom daily اتكلم مع امي يوميا;To call يتصل : She called me when I was out اتصلت بي عندما كنت بالخارج;To know يعلم : I know your secret اعلم سرك;To learn يتعلم : Many students learn English الكثير من التلامذ يتعلمون الإنجليزية;To teach يعلم : My teacher teaches us معلمتي تعلمنا </t>
+  </si>
+  <si>
+    <t>Once upon a time, there was a smart boy named Ali who loved to learn new things. Every day, Ali would go to school. He would wake up early, eat a banana for breakfast, and run to school. Ali loved English lessons the most. He could speak English very well and enjoyed practicing with his friends.​  One day, his teacher gave them a special lesson. She said, "Today, we are going to write a short story." Ali was excited. He loved his teacher and always paid attention to her lessons. He thought for a moment and then began to write on his notebook, "The boy eats an apple," he started.​  At lunch, Ali sat with his friends and talked about their stories. "I can speak English," he proudly told them. They all agreed that learning English was fun. After school, Ali ran home to share his story with his parents. His mother smiled and said, "You are very smart, Ali."​  Before going to bed, Ali looked at the book on the table beside his bed. He said to himself, "I love my school and my teacher. I can't wait for next week to learn more." And with that happy thought, he drifted off to sleep, dreaming of all the new things he would learn.​  See you next week, Ali thought, as he closed his eyes, ready for another exciting day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t>The ____ has long blonde hair</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He is a very kind _____</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> They have one _____</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> She ______ speak Turkish</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> They _____ one cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I ____ a student</t>
+  </si>
+  <si>
+    <t>boy; girl ; thing</t>
+  </si>
+  <si>
+    <t>person; animal; month</t>
+  </si>
+  <si>
+    <t>child; person; happiness</t>
+  </si>
+  <si>
+    <t>he; she ; you</t>
+  </si>
+  <si>
+    <t>we; he ; it</t>
+  </si>
+  <si>
+    <t>they; she ; I</t>
+  </si>
+  <si>
+    <t>can ; say; has</t>
+  </si>
+  <si>
+    <t>have; say ; go</t>
+  </si>
+  <si>
+    <t>go; write; am</t>
+  </si>
+  <si>
+    <t>Complete the sentence based on the Arabic translation provided:</t>
+  </si>
+  <si>
+    <t>أكمل الجملة بناءً على الترجمة العربية المقدمة:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>My sister</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is visiting us.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Ahmed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a good student.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> The children</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are playing outside.</t>
+    </r>
+  </si>
+  <si>
+    <t>here;always</t>
+  </si>
+  <si>
+    <t>The dog is _____ the table</t>
+  </si>
+  <si>
+    <t>under;in; on</t>
+  </si>
+  <si>
+    <t>Select the option that best describes the image above</t>
+  </si>
+  <si>
+    <t>The table is ____ the dog and the cat</t>
+  </si>
+  <si>
+    <t>between;in;on</t>
+  </si>
+  <si>
+    <t>Do you want to drink coffee ____ tea ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I got a gift ___ you</t>
+  </si>
+  <si>
+    <t>or;and</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> while;but</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I want to buy a new dress ____ I don’t have money</t>
+  </si>
+  <si>
+    <t>because;for</t>
+  </si>
+  <si>
+    <t>At lunch, Ali sat with his friends and talked about their stories. "I can speak English," he proudly told them. They all agreed that learning English was fun. After school, Ali ran home to share his story with his parents. His mother smiled and said, "You are very smart, Ali."​</t>
+  </si>
+  <si>
+    <t>Read the following passage and answer the question with one word.</t>
+  </si>
+  <si>
+    <t>اقرأ الفقرة التالية وأجب عن السؤال بكلمة واحدة.</t>
+  </si>
+  <si>
+    <t>With whom did Ali share his story? ________;They all agreed that learning English is _______;Where did Ali run? ______​;"غداء" ______;"ام"_______</t>
+  </si>
+  <si>
+    <t>Parents;Fun;Home;Lunch;Mother</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">She is waiting for you ____ : هي تنتظرك </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>هنا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">; I will _____ love you : انا سأحبك </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>دائما</t>
+    </r>
+  </si>
+  <si>
+    <t>The book is on the table</t>
+  </si>
+  <si>
+    <t>The boy eats an apple</t>
+  </si>
+  <si>
+    <t>I can speak English</t>
+  </si>
+  <si>
+    <t>الكتاب على الطاولة ; الكتاب في الطاولة</t>
+  </si>
+  <si>
+    <t>انا استطيع التحدث بالانجليزية ; من الممكن ان اتكلم الانجليزية</t>
+  </si>
+  <si>
+    <t>الولد يأكل التفاحة ; الولد ياكل الموزة</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> اسبوع  =  ________;مدرسة = _______;ذكية =  ______​</t>
+  </si>
+  <si>
+    <t>week;School;smart</t>
+  </si>
+  <si>
+    <t>she ______ on the bool</t>
+  </si>
+  <si>
+    <t>I ____ banana</t>
+  </si>
+  <si>
+    <t>He ____ hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reads; says; writes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eat; run; have</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reads; writes; says</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,6 +753,17 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -868,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:O59"/>
+  <dimension ref="A4:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,13 +1157,13 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -914,7 +1172,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
         <v>4</v>
@@ -946,13 +1204,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -961,7 +1219,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -993,13 +1251,13 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -1008,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
@@ -1021,6 +1279,53 @@
       </c>
       <c r="O6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -1040,34 +1345,34 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" t="s">
-        <v>4</v>
+        <v>81</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1087,22 +1392,22 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
         <v>82</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" t="s">
         <v>4</v>
@@ -1134,22 +1439,22 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
         <v>83</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" t="s">
         <v>4</v>
@@ -1181,22 +1486,22 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L11" t="s">
         <v>4</v>
@@ -1228,22 +1533,22 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" t="s">
         <v>4</v>
@@ -1275,22 +1580,22 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>86</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13" t="s">
         <v>4</v>
@@ -1322,22 +1627,22 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>87</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" t="s">
         <v>4</v>
@@ -1369,13 +1674,13 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>88</v>
@@ -1384,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
         <v>4</v>
@@ -1416,22 +1721,22 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
         <v>89</v>
       </c>
-      <c r="J16">
-        <v>0</v>
+      <c r="J16" t="s">
+        <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L16" t="s">
         <v>4</v>
@@ -1451,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1463,22 +1768,22 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" t="s">
-        <v>4</v>
+        <v>150</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L17" t="s">
         <v>4</v>
@@ -1490,6 +1795,53 @@
         <v>4</v>
       </c>
       <c r="O17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>151</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1498,34 +1850,34 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>6</v>
+      <c r="E19" t="s">
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
-        <v>4</v>
+        <v>152</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L19" t="s">
         <v>4</v>
@@ -1545,10 +1897,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1557,22 +1909,22 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" t="s">
-        <v>4</v>
+        <v>167</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L20" t="s">
         <v>4</v>
@@ -1592,10 +1944,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1604,22 +1956,22 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" t="s">
-        <v>4</v>
+        <v>168</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
@@ -1639,10 +1991,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1657,16 +2009,16 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
-        <v>4</v>
+        <v>169</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L22" t="s">
         <v>4</v>
@@ -1681,40 +2033,86 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>6</v>
+      <c r="E24" t="s">
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
-        <v>4</v>
+        <v>154</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L24" t="s">
         <v>4</v>
@@ -1734,10 +2132,10 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1746,22 +2144,22 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
-        <v>4</v>
+        <v>155</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
       </c>
       <c r="K25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L25" t="s">
         <v>4</v>
@@ -1776,39 +2174,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G26" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="H26" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="I26" t="s">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="J26" t="s">
         <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L26" t="s">
         <v>4</v>
@@ -1828,10 +2226,10 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -1840,34 +2238,34 @@
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" t="s">
-        <v>4</v>
+        <v>171</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="M27" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="N27" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="O27" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -1875,10 +2273,10 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -1887,22 +2285,22 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>29</v>
+        <v>173</v>
       </c>
       <c r="G28" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" t="s">
-        <v>96</v>
+        <v>174</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28" t="s">
         <v>4</v>
@@ -1922,10 +2320,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -1934,22 +2332,22 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>96</v>
+        <v>176</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L29" t="s">
         <v>4</v>
@@ -1969,10 +2367,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -1981,22 +2379,22 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" t="s">
-        <v>97</v>
+        <v>177</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L30" t="s">
         <v>4</v>
@@ -2016,10 +2414,10 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -2028,22 +2426,22 @@
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>98</v>
+        <v>180</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L31" t="s">
         <v>4</v>
@@ -2063,10 +2461,10 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -2075,22 +2473,22 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" t="s">
-        <v>99</v>
+        <v>188</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L32" t="s">
         <v>4</v>
@@ -2105,15 +2503,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -2122,22 +2520,22 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>4</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>100</v>
+        <v>190</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L33" t="s">
         <v>4</v>
@@ -2152,15 +2550,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -2169,22 +2567,22 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>4</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>101</v>
+        <v>189</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L34" t="s">
         <v>4</v>
@@ -2199,15 +2597,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -2216,22 +2614,22 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="G35" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
+        <v>194</v>
+      </c>
+      <c r="I35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J35" t="s">
+        <v>4</v>
       </c>
       <c r="K35" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L35" t="s">
         <v>4</v>
@@ -2246,15 +2644,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -2263,22 +2661,22 @@
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>104</v>
+        <v>196</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L36" t="s">
         <v>4</v>
@@ -2293,15 +2691,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -2310,22 +2708,22 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>103</v>
+        <v>197</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L37" t="s">
         <v>4</v>
@@ -2340,15 +2738,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -2357,22 +2755,22 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>52</v>
+        <v>198</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L38" t="s">
         <v>4</v>
@@ -2387,15 +2785,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -2404,22 +2802,22 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="G39" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
+      <c r="I39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" t="s">
+        <v>4</v>
       </c>
       <c r="K39" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="L39" t="s">
         <v>4</v>
@@ -2428,7 +2826,7 @@
         <v>4</v>
       </c>
       <c r="N39" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
       <c r="O39" t="s">
         <v>4</v>
@@ -2439,34 +2837,34 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>6</v>
+      <c r="E40" t="s">
+        <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="I40" t="s">
-        <v>4</v>
+        <v>186</v>
       </c>
       <c r="J40" t="s">
         <v>4</v>
       </c>
       <c r="K40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L40" t="s">
         <v>4</v>
@@ -2481,763 +2879,1768 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
-        <v>107</v>
-      </c>
-      <c r="I41" t="s">
-        <v>4</v>
-      </c>
-      <c r="J41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K41" t="s">
-        <v>15</v>
-      </c>
-      <c r="L41" t="s">
-        <v>4</v>
-      </c>
-      <c r="M41" t="s">
-        <v>4</v>
-      </c>
-      <c r="N41" t="s">
-        <v>4</v>
-      </c>
-      <c r="O41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" t="s">
-        <v>108</v>
-      </c>
-      <c r="I42" t="s">
-        <v>4</v>
-      </c>
-      <c r="J42" t="s">
-        <v>4</v>
-      </c>
-      <c r="K42" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" t="s">
-        <v>4</v>
-      </c>
-      <c r="M42" t="s">
-        <v>4</v>
-      </c>
-      <c r="N42" t="s">
-        <v>4</v>
-      </c>
-      <c r="O42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" t="s">
-        <v>4</v>
-      </c>
-      <c r="H44" t="s">
-        <v>111</v>
-      </c>
-      <c r="I44" t="s">
-        <v>4</v>
-      </c>
-      <c r="J44" t="s">
-        <v>4</v>
-      </c>
-      <c r="K44" t="s">
-        <v>15</v>
-      </c>
-      <c r="L44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M44" t="s">
-        <v>4</v>
-      </c>
-      <c r="N44" t="s">
-        <v>4</v>
-      </c>
-      <c r="O44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" t="s">
-        <v>112</v>
-      </c>
-      <c r="I45" t="s">
-        <v>4</v>
-      </c>
-      <c r="J45" t="s">
-        <v>4</v>
-      </c>
-      <c r="K45" t="s">
-        <v>15</v>
-      </c>
-      <c r="L45" t="s">
-        <v>4</v>
-      </c>
-      <c r="M45" t="s">
-        <v>4</v>
-      </c>
-      <c r="N45" t="s">
-        <v>4</v>
-      </c>
-      <c r="O45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" t="s">
-        <v>4</v>
-      </c>
-      <c r="H46" t="s">
-        <v>148</v>
-      </c>
-      <c r="I46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K46" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" t="s">
-        <v>4</v>
-      </c>
-      <c r="M46" t="s">
-        <v>4</v>
-      </c>
-      <c r="N46" t="s">
-        <v>4</v>
-      </c>
-      <c r="O46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" t="s">
-        <v>4</v>
-      </c>
-      <c r="G47" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" t="s">
-        <v>4</v>
-      </c>
-      <c r="I47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J47" t="s">
-        <v>4</v>
-      </c>
-      <c r="K47" t="s">
-        <v>7</v>
-      </c>
-      <c r="L47" t="s">
-        <v>113</v>
-      </c>
-      <c r="M47" t="s">
-        <v>114</v>
-      </c>
-      <c r="N47" t="s">
-        <v>115</v>
-      </c>
-      <c r="O47" t="s">
-        <v>116</v>
-      </c>
-    </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" t="s">
-        <v>117</v>
-      </c>
-      <c r="G48" t="s">
-        <v>118</v>
-      </c>
-      <c r="H48" t="s">
-        <v>119</v>
-      </c>
-      <c r="I48" t="s">
-        <v>120</v>
-      </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-      <c r="K48" t="s">
-        <v>19</v>
-      </c>
-      <c r="L48" t="s">
-        <v>4</v>
-      </c>
-      <c r="M48" t="s">
-        <v>4</v>
-      </c>
-      <c r="N48" t="s">
-        <v>4</v>
-      </c>
-      <c r="O48" t="s">
-        <v>4</v>
-      </c>
+      <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" t="s">
-        <v>122</v>
-      </c>
-      <c r="G49" t="s">
-        <v>121</v>
-      </c>
-      <c r="H49" t="s">
-        <v>4</v>
-      </c>
-      <c r="I49" t="s">
-        <v>139</v>
-      </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-      <c r="K49" t="s">
-        <v>19</v>
-      </c>
-      <c r="L49" t="s">
-        <v>4</v>
-      </c>
-      <c r="M49" t="s">
-        <v>4</v>
-      </c>
-      <c r="N49" t="s">
-        <v>4</v>
-      </c>
-      <c r="O49" t="s">
-        <v>4</v>
-      </c>
+      <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" t="s">
-        <v>124</v>
-      </c>
-      <c r="G50" t="s">
-        <v>123</v>
-      </c>
-      <c r="H50" t="s">
-        <v>4</v>
-      </c>
-      <c r="I50" t="s">
-        <v>140</v>
-      </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="K50" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M50" t="s">
-        <v>4</v>
-      </c>
-      <c r="N50" t="s">
-        <v>4</v>
-      </c>
-      <c r="O50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" t="s">
-        <v>125</v>
-      </c>
-      <c r="G51" t="s">
-        <v>126</v>
-      </c>
-      <c r="H51" t="s">
-        <v>4</v>
-      </c>
-      <c r="I51" t="s">
-        <v>141</v>
-      </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-      <c r="K51" t="s">
-        <v>19</v>
-      </c>
-      <c r="L51" t="s">
-        <v>4</v>
-      </c>
-      <c r="M51" t="s">
-        <v>4</v>
-      </c>
-      <c r="N51" t="s">
-        <v>4</v>
-      </c>
-      <c r="O51" t="s">
-        <v>4</v>
-      </c>
+      <c r="I50" s="2"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" t="s">
-        <v>128</v>
-      </c>
-      <c r="H52" t="s">
-        <v>4</v>
-      </c>
-      <c r="I52" t="s">
-        <v>142</v>
-      </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
-      <c r="K52" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" t="s">
-        <v>4</v>
-      </c>
-      <c r="M52" t="s">
-        <v>4</v>
-      </c>
-      <c r="N52" t="s">
-        <v>4</v>
-      </c>
-      <c r="O52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" t="s">
-        <v>130</v>
-      </c>
-      <c r="H53" t="s">
-        <v>4</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J53">
-        <v>1</v>
-      </c>
-      <c r="K53" t="s">
-        <v>19</v>
-      </c>
-      <c r="L53" t="s">
-        <v>4</v>
-      </c>
-      <c r="M53" t="s">
-        <v>4</v>
-      </c>
-      <c r="N53" t="s">
-        <v>4</v>
-      </c>
-      <c r="O53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" t="s">
-        <v>131</v>
-      </c>
-      <c r="G54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H54" t="s">
-        <v>4</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54" t="s">
-        <v>19</v>
-      </c>
-      <c r="L54" t="s">
-        <v>4</v>
-      </c>
-      <c r="M54" t="s">
-        <v>4</v>
-      </c>
-      <c r="N54" t="s">
-        <v>4</v>
-      </c>
-      <c r="O54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" t="s">
-        <v>133</v>
-      </c>
-      <c r="G55" t="s">
-        <v>134</v>
-      </c>
-      <c r="H55" t="s">
-        <v>4</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="J55">
-        <v>1</v>
-      </c>
-      <c r="K55" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" t="s">
-        <v>4</v>
-      </c>
-      <c r="M55" t="s">
-        <v>4</v>
-      </c>
-      <c r="N55" t="s">
-        <v>4</v>
-      </c>
-      <c r="O55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" t="s">
-        <v>136</v>
-      </c>
-      <c r="H56" t="s">
-        <v>4</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="J56">
-        <v>1</v>
-      </c>
-      <c r="K56" t="s">
-        <v>19</v>
-      </c>
-      <c r="L56" t="s">
-        <v>4</v>
-      </c>
-      <c r="M56" t="s">
-        <v>4</v>
-      </c>
-      <c r="N56" t="s">
-        <v>4</v>
-      </c>
-      <c r="O56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D57" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" t="s">
-        <v>137</v>
-      </c>
-      <c r="G57" t="s">
-        <v>138</v>
-      </c>
-      <c r="H57" t="s">
-        <v>4</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-      <c r="K57" t="s">
-        <v>19</v>
-      </c>
-      <c r="L57" t="s">
-        <v>4</v>
-      </c>
-      <c r="M57" t="s">
-        <v>4</v>
-      </c>
-      <c r="N57" t="s">
-        <v>4</v>
-      </c>
-      <c r="O57" t="s">
-        <v>4</v>
-      </c>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I54" s="2"/>
     </row>
     <row r="58" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I59" s="1"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>90</v>
+      </c>
+      <c r="I62" t="s">
+        <v>4</v>
+      </c>
+      <c r="J62" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" t="s">
+        <v>14</v>
+      </c>
+      <c r="L62" t="s">
+        <v>4</v>
+      </c>
+      <c r="M62" t="s">
+        <v>4</v>
+      </c>
+      <c r="N62" t="s">
+        <v>4</v>
+      </c>
+      <c r="O62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" t="s">
+        <v>91</v>
+      </c>
+      <c r="I63" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" t="s">
+        <v>4</v>
+      </c>
+      <c r="K63" t="s">
+        <v>14</v>
+      </c>
+      <c r="L63" t="s">
+        <v>4</v>
+      </c>
+      <c r="M63" t="s">
+        <v>4</v>
+      </c>
+      <c r="N63" t="s">
+        <v>4</v>
+      </c>
+      <c r="O63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" t="s">
+        <v>57</v>
+      </c>
+      <c r="I64" t="s">
+        <v>4</v>
+      </c>
+      <c r="J64" t="s">
+        <v>4</v>
+      </c>
+      <c r="K64" t="s">
+        <v>14</v>
+      </c>
+      <c r="L64" t="s">
+        <v>4</v>
+      </c>
+      <c r="M64" t="s">
+        <v>4</v>
+      </c>
+      <c r="N64" t="s">
+        <v>4</v>
+      </c>
+      <c r="O64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" t="s">
+        <v>4</v>
+      </c>
+      <c r="K65" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" t="s">
+        <v>4</v>
+      </c>
+      <c r="M65" t="s">
+        <v>4</v>
+      </c>
+      <c r="N65" t="s">
+        <v>4</v>
+      </c>
+      <c r="O65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>92</v>
+      </c>
+      <c r="I67" t="s">
+        <v>4</v>
+      </c>
+      <c r="J67" t="s">
+        <v>4</v>
+      </c>
+      <c r="K67" t="s">
+        <v>14</v>
+      </c>
+      <c r="L67" t="s">
+        <v>4</v>
+      </c>
+      <c r="M67" t="s">
+        <v>4</v>
+      </c>
+      <c r="N67" t="s">
+        <v>4</v>
+      </c>
+      <c r="O67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" t="s">
+        <v>93</v>
+      </c>
+      <c r="I68" t="s">
+        <v>4</v>
+      </c>
+      <c r="J68" t="s">
+        <v>4</v>
+      </c>
+      <c r="K68" t="s">
+        <v>14</v>
+      </c>
+      <c r="L68" t="s">
+        <v>4</v>
+      </c>
+      <c r="M68" t="s">
+        <v>4</v>
+      </c>
+      <c r="N68" t="s">
+        <v>4</v>
+      </c>
+      <c r="O68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" t="s">
+        <v>94</v>
+      </c>
+      <c r="I69" t="s">
+        <v>4</v>
+      </c>
+      <c r="J69" t="s">
+        <v>4</v>
+      </c>
+      <c r="K69" t="s">
+        <v>14</v>
+      </c>
+      <c r="L69" t="s">
+        <v>4</v>
+      </c>
+      <c r="M69" t="s">
+        <v>4</v>
+      </c>
+      <c r="N69" t="s">
+        <v>4</v>
+      </c>
+      <c r="O69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" t="s">
+        <v>4</v>
+      </c>
+      <c r="H70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70" t="s">
+        <v>4</v>
+      </c>
+      <c r="J70" t="s">
+        <v>4</v>
+      </c>
+      <c r="K70" t="s">
+        <v>7</v>
+      </c>
+      <c r="L70" t="s">
+        <v>24</v>
+      </c>
+      <c r="M70" t="s">
+        <v>25</v>
+      </c>
+      <c r="N70" t="s">
+        <v>26</v>
+      </c>
+      <c r="O70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" t="s">
+        <v>30</v>
+      </c>
+      <c r="I71" t="s">
+        <v>95</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71" t="s">
+        <v>18</v>
+      </c>
+      <c r="L71" t="s">
+        <v>4</v>
+      </c>
+      <c r="M71" t="s">
+        <v>4</v>
+      </c>
+      <c r="N71" t="s">
+        <v>4</v>
+      </c>
+      <c r="O71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" t="s">
+        <v>32</v>
+      </c>
+      <c r="H72" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" t="s">
+        <v>95</v>
+      </c>
+      <c r="J72">
+        <v>2</v>
+      </c>
+      <c r="K72" t="s">
+        <v>18</v>
+      </c>
+      <c r="L72" t="s">
+        <v>4</v>
+      </c>
+      <c r="M72" t="s">
+        <v>4</v>
+      </c>
+      <c r="N72" t="s">
+        <v>4</v>
+      </c>
+      <c r="O72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73" t="s">
+        <v>96</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>18</v>
+      </c>
+      <c r="L73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" t="s">
+        <v>36</v>
+      </c>
+      <c r="H74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" t="s">
+        <v>97</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>18</v>
+      </c>
+      <c r="L74" t="s">
+        <v>4</v>
+      </c>
+      <c r="M74" t="s">
+        <v>4</v>
+      </c>
+      <c r="N74" t="s">
+        <v>4</v>
+      </c>
+      <c r="O74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75" t="s">
+        <v>98</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75" t="s">
+        <v>18</v>
+      </c>
+      <c r="L75" t="s">
+        <v>4</v>
+      </c>
+      <c r="M75" t="s">
+        <v>4</v>
+      </c>
+      <c r="N75" t="s">
+        <v>4</v>
+      </c>
+      <c r="O75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>39</v>
+      </c>
+      <c r="G76" t="s">
+        <v>40</v>
+      </c>
+      <c r="H76" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76" t="s">
+        <v>18</v>
+      </c>
+      <c r="L76" t="s">
+        <v>4</v>
+      </c>
+      <c r="M76" t="s">
+        <v>4</v>
+      </c>
+      <c r="N76" t="s">
+        <v>4</v>
+      </c>
+      <c r="O76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" t="s">
+        <v>41</v>
+      </c>
+      <c r="G77" t="s">
+        <v>42</v>
+      </c>
+      <c r="H77" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77" t="s">
+        <v>18</v>
+      </c>
+      <c r="L77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" t="s">
+        <v>43</v>
+      </c>
+      <c r="G78" t="s">
+        <v>44</v>
+      </c>
+      <c r="H78" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78" t="s">
+        <v>18</v>
+      </c>
+      <c r="L78" t="s">
+        <v>4</v>
+      </c>
+      <c r="M78" t="s">
+        <v>4</v>
+      </c>
+      <c r="N78" t="s">
+        <v>4</v>
+      </c>
+      <c r="O78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" t="s">
+        <v>45</v>
+      </c>
+      <c r="G79" t="s">
+        <v>46</v>
+      </c>
+      <c r="H79" t="s">
+        <v>4</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79" t="s">
+        <v>18</v>
+      </c>
+      <c r="L79" t="s">
+        <v>4</v>
+      </c>
+      <c r="M79" t="s">
+        <v>4</v>
+      </c>
+      <c r="N79" t="s">
+        <v>4</v>
+      </c>
+      <c r="O79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" t="s">
+        <v>48</v>
+      </c>
+      <c r="H80" t="s">
+        <v>4</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>18</v>
+      </c>
+      <c r="L80" t="s">
+        <v>4</v>
+      </c>
+      <c r="M80" t="s">
+        <v>4</v>
+      </c>
+      <c r="N80" t="s">
+        <v>4</v>
+      </c>
+      <c r="O80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>49</v>
+      </c>
+      <c r="G81" t="s">
+        <v>50</v>
+      </c>
+      <c r="H81" t="s">
+        <v>4</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81" t="s">
+        <v>18</v>
+      </c>
+      <c r="L81" t="s">
+        <v>4</v>
+      </c>
+      <c r="M81" t="s">
+        <v>4</v>
+      </c>
+      <c r="N81" t="s">
+        <v>4</v>
+      </c>
+      <c r="O81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
+        <v>52</v>
+      </c>
+      <c r="G82" t="s">
+        <v>53</v>
+      </c>
+      <c r="H82" t="s">
+        <v>4</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82" t="s">
+        <v>18</v>
+      </c>
+      <c r="L82" t="s">
+        <v>4</v>
+      </c>
+      <c r="M82" t="s">
+        <v>4</v>
+      </c>
+      <c r="N82" t="s">
+        <v>4</v>
+      </c>
+      <c r="O82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>104</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" t="s">
+        <v>105</v>
+      </c>
+      <c r="I83" t="s">
+        <v>4</v>
+      </c>
+      <c r="J83" t="s">
+        <v>4</v>
+      </c>
+      <c r="K83" t="s">
+        <v>14</v>
+      </c>
+      <c r="L83" t="s">
+        <v>4</v>
+      </c>
+      <c r="M83" t="s">
+        <v>4</v>
+      </c>
+      <c r="N83" t="s">
+        <v>4</v>
+      </c>
+      <c r="O83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>104</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" t="s">
+        <v>4</v>
+      </c>
+      <c r="H84" t="s">
+        <v>106</v>
+      </c>
+      <c r="I84" t="s">
+        <v>4</v>
+      </c>
+      <c r="J84" t="s">
+        <v>4</v>
+      </c>
+      <c r="K84" t="s">
+        <v>14</v>
+      </c>
+      <c r="L84" t="s">
+        <v>4</v>
+      </c>
+      <c r="M84" t="s">
+        <v>4</v>
+      </c>
+      <c r="N84" t="s">
+        <v>4</v>
+      </c>
+      <c r="O84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>104</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" t="s">
+        <v>107</v>
+      </c>
+      <c r="I85" t="s">
+        <v>4</v>
+      </c>
+      <c r="J85" t="s">
+        <v>4</v>
+      </c>
+      <c r="K85" t="s">
+        <v>21</v>
+      </c>
+      <c r="L85" t="s">
+        <v>4</v>
+      </c>
+      <c r="M85" t="s">
+        <v>4</v>
+      </c>
+      <c r="N85" t="s">
+        <v>4</v>
+      </c>
+      <c r="O85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" t="s">
+        <v>22</v>
+      </c>
+      <c r="G87" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" t="s">
+        <v>110</v>
+      </c>
+      <c r="I87" t="s">
+        <v>4</v>
+      </c>
+      <c r="J87" t="s">
+        <v>4</v>
+      </c>
+      <c r="K87" t="s">
+        <v>14</v>
+      </c>
+      <c r="L87" t="s">
+        <v>4</v>
+      </c>
+      <c r="M87" t="s">
+        <v>4</v>
+      </c>
+      <c r="N87" t="s">
+        <v>4</v>
+      </c>
+      <c r="O87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" t="s">
+        <v>15</v>
+      </c>
+      <c r="G88" t="s">
+        <v>4</v>
+      </c>
+      <c r="H88" t="s">
+        <v>111</v>
+      </c>
+      <c r="I88" t="s">
+        <v>4</v>
+      </c>
+      <c r="J88" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" t="s">
+        <v>14</v>
+      </c>
+      <c r="L88" t="s">
+        <v>4</v>
+      </c>
+      <c r="M88" t="s">
+        <v>4</v>
+      </c>
+      <c r="N88" t="s">
+        <v>4</v>
+      </c>
+      <c r="O88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" t="s">
+        <v>4</v>
+      </c>
+      <c r="H89" t="s">
+        <v>147</v>
+      </c>
+      <c r="I89" t="s">
+        <v>4</v>
+      </c>
+      <c r="J89" t="s">
+        <v>4</v>
+      </c>
+      <c r="K89" t="s">
+        <v>14</v>
+      </c>
+      <c r="L89" t="s">
+        <v>4</v>
+      </c>
+      <c r="M89" t="s">
+        <v>4</v>
+      </c>
+      <c r="N89" t="s">
+        <v>4</v>
+      </c>
+      <c r="O89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" t="s">
+        <v>4</v>
+      </c>
+      <c r="H90" t="s">
+        <v>4</v>
+      </c>
+      <c r="I90" t="s">
+        <v>4</v>
+      </c>
+      <c r="J90" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" t="s">
+        <v>7</v>
+      </c>
+      <c r="L90" t="s">
+        <v>112</v>
+      </c>
+      <c r="M90" t="s">
+        <v>113</v>
+      </c>
+      <c r="N90" t="s">
+        <v>114</v>
+      </c>
+      <c r="O90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91" t="s">
+        <v>116</v>
+      </c>
+      <c r="G91" t="s">
+        <v>117</v>
+      </c>
+      <c r="H91" t="s">
+        <v>118</v>
+      </c>
+      <c r="I91" t="s">
+        <v>119</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91" t="s">
+        <v>18</v>
+      </c>
+      <c r="L91" t="s">
+        <v>4</v>
+      </c>
+      <c r="M91" t="s">
+        <v>4</v>
+      </c>
+      <c r="N91" t="s">
+        <v>4</v>
+      </c>
+      <c r="O91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>108</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" t="s">
+        <v>4</v>
+      </c>
+      <c r="F92" t="s">
+        <v>121</v>
+      </c>
+      <c r="G92" t="s">
+        <v>120</v>
+      </c>
+      <c r="H92" t="s">
+        <v>4</v>
+      </c>
+      <c r="I92" t="s">
+        <v>138</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" t="s">
+        <v>4</v>
+      </c>
+      <c r="M92" t="s">
+        <v>4</v>
+      </c>
+      <c r="N92" t="s">
+        <v>4</v>
+      </c>
+      <c r="O92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" t="s">
+        <v>123</v>
+      </c>
+      <c r="G93" t="s">
+        <v>122</v>
+      </c>
+      <c r="H93" t="s">
+        <v>4</v>
+      </c>
+      <c r="I93" t="s">
+        <v>139</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93" t="s">
+        <v>18</v>
+      </c>
+      <c r="L93" t="s">
+        <v>4</v>
+      </c>
+      <c r="M93" t="s">
+        <v>4</v>
+      </c>
+      <c r="N93" t="s">
+        <v>4</v>
+      </c>
+      <c r="O93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>108</v>
+      </c>
+      <c r="D94" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" t="s">
+        <v>124</v>
+      </c>
+      <c r="G94" t="s">
+        <v>125</v>
+      </c>
+      <c r="H94" t="s">
+        <v>4</v>
+      </c>
+      <c r="I94" t="s">
+        <v>140</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94" t="s">
+        <v>18</v>
+      </c>
+      <c r="L94" t="s">
+        <v>4</v>
+      </c>
+      <c r="M94" t="s">
+        <v>4</v>
+      </c>
+      <c r="N94" t="s">
+        <v>4</v>
+      </c>
+      <c r="O94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>4</v>
+      </c>
+      <c r="F95" t="s">
+        <v>126</v>
+      </c>
+      <c r="G95" t="s">
+        <v>127</v>
+      </c>
+      <c r="H95" t="s">
+        <v>4</v>
+      </c>
+      <c r="I95" t="s">
+        <v>141</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95" t="s">
+        <v>18</v>
+      </c>
+      <c r="L95" t="s">
+        <v>4</v>
+      </c>
+      <c r="M95" t="s">
+        <v>4</v>
+      </c>
+      <c r="N95" t="s">
+        <v>4</v>
+      </c>
+      <c r="O95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>108</v>
+      </c>
+      <c r="D96" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" t="s">
+        <v>4</v>
+      </c>
+      <c r="F96" t="s">
+        <v>128</v>
+      </c>
+      <c r="G96" t="s">
+        <v>129</v>
+      </c>
+      <c r="H96" t="s">
+        <v>4</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96" t="s">
+        <v>18</v>
+      </c>
+      <c r="L96" t="s">
+        <v>4</v>
+      </c>
+      <c r="M96" t="s">
+        <v>4</v>
+      </c>
+      <c r="N96" t="s">
+        <v>4</v>
+      </c>
+      <c r="O96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D97" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" t="s">
+        <v>130</v>
+      </c>
+      <c r="G97" t="s">
+        <v>131</v>
+      </c>
+      <c r="H97" t="s">
+        <v>4</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97" t="s">
+        <v>18</v>
+      </c>
+      <c r="L97" t="s">
+        <v>4</v>
+      </c>
+      <c r="M97" t="s">
+        <v>4</v>
+      </c>
+      <c r="N97" t="s">
+        <v>4</v>
+      </c>
+      <c r="O97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>108</v>
+      </c>
+      <c r="D98" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" t="s">
+        <v>4</v>
+      </c>
+      <c r="F98" t="s">
+        <v>132</v>
+      </c>
+      <c r="G98" t="s">
+        <v>133</v>
+      </c>
+      <c r="H98" t="s">
+        <v>4</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98" t="s">
+        <v>18</v>
+      </c>
+      <c r="L98" t="s">
+        <v>4</v>
+      </c>
+      <c r="M98" t="s">
+        <v>4</v>
+      </c>
+      <c r="N98" t="s">
+        <v>4</v>
+      </c>
+      <c r="O98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" t="s">
+        <v>4</v>
+      </c>
+      <c r="F99" t="s">
+        <v>134</v>
+      </c>
+      <c r="G99" t="s">
+        <v>135</v>
+      </c>
+      <c r="H99" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99" t="s">
+        <v>18</v>
+      </c>
+      <c r="L99" t="s">
+        <v>4</v>
+      </c>
+      <c r="M99" t="s">
+        <v>4</v>
+      </c>
+      <c r="N99" t="s">
+        <v>4</v>
+      </c>
+      <c r="O99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>108</v>
+      </c>
+      <c r="D100" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" t="s">
+        <v>136</v>
+      </c>
+      <c r="G100" t="s">
+        <v>137</v>
+      </c>
+      <c r="H100" t="s">
+        <v>4</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100" t="s">
+        <v>18</v>
+      </c>
+      <c r="L100" t="s">
+        <v>4</v>
+      </c>
+      <c r="M100" t="s">
+        <v>4</v>
+      </c>
+      <c r="N100" t="s">
+        <v>4</v>
+      </c>
+      <c r="O100" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: add unit 4 and 5 test data
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D6B1BB-EAF3-9F46-A99D-53B28714AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B5AE3C-F091-C54C-B2D6-0112402C1B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="3100" windowWidth="33120" windowHeight="20020" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
+    <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="290">
   <si>
     <t>A1</t>
   </si>
@@ -860,6 +860,144 @@
   </si>
   <si>
     <t>to;from;into;out of ;through</t>
+  </si>
+  <si>
+    <t>Write the word In English</t>
+  </si>
+  <si>
+    <t>Box;Wall;Party;Homework;Store</t>
+  </si>
+  <si>
+    <t>صندوق;حائط;حفلة;وظيفة;متجر</t>
+  </si>
+  <si>
+    <t>Read the following :</t>
+  </si>
+  <si>
+    <t>money;mouse;nose;octopus;pencil;queen;row; swim;train;rainbow;voice;violin;whale;x-ray;yogurt;zoo</t>
+  </si>
+  <si>
+    <t>Write the following on your notebook:</t>
+  </si>
+  <si>
+    <t>mouse;net;nest;owl power;pencil;queen; rainbow;snake;turtle;umbrella;vote;water;x-ray;yellow;zip</t>
+  </si>
+  <si>
+    <t>write what you hear</t>
+  </si>
+  <si>
+    <t>Lina goes to the kitchen. She takes a spoon and eats yogurt for breakfast. She also eats some olives. Olives are the best .​</t>
+  </si>
+  <si>
+    <t>dictation</t>
+  </si>
+  <si>
+    <t>Select the sentence that best describes the image above:</t>
+  </si>
+  <si>
+    <t>turtle;spoon;milk</t>
+  </si>
+  <si>
+    <t>olive;yogurt;milk</t>
+  </si>
+  <si>
+    <t>spoon;window;fork</t>
+  </si>
+  <si>
+    <t>people;rainbow;water</t>
+  </si>
+  <si>
+    <t>turtle;spoon;water</t>
+  </si>
+  <si>
+    <t>queen;mouse;yogurt</t>
+  </si>
+  <si>
+    <t>queen;people;owl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turtle;spoon;water) </t>
+  </si>
+  <si>
+    <t>people;turtle;numbers</t>
+  </si>
+  <si>
+    <t>We;You;They;You;You;They;You;It;He;It;She;I</t>
+  </si>
+  <si>
+    <t>نحن;انتم;هم;انت;انتن;هن;انتي;هو لغير العاقل;هو;هي لغير العاقل;هي;انا</t>
+  </si>
+  <si>
+    <t>Select the correct pronoun to complete the sentence:</t>
+  </si>
+  <si>
+    <t>_____  didn’t go to school today.</t>
+  </si>
+  <si>
+    <t>This gift is for _____ .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _____  bought a gift.</t>
+  </si>
+  <si>
+    <t>I will call _____ tomorrow.</t>
+  </si>
+  <si>
+    <t>Can you tell _____  the news?</t>
+  </si>
+  <si>
+    <t>We are looking for the cat _____ .</t>
+  </si>
+  <si>
+    <t>_____ said ‘No’.</t>
+  </si>
+  <si>
+    <t>She gave _____  the instructions.</t>
+  </si>
+  <si>
+    <t>She asked _____  to join the team. (هن)</t>
+  </si>
+  <si>
+    <t>_____  said “ no we didn’t like it “.</t>
+  </si>
+  <si>
+    <t>The movie was great. Did you like _____ ? (هو/هي لغير العاقل)</t>
+  </si>
+  <si>
+    <t>They didn't invite _____ to the party.</t>
+  </si>
+  <si>
+    <t>i;me</t>
+  </si>
+  <si>
+    <t>I;Me</t>
+  </si>
+  <si>
+    <t>i;you</t>
+  </si>
+  <si>
+    <t>Me; You​</t>
+  </si>
+  <si>
+    <t>he;him</t>
+  </si>
+  <si>
+    <t>she;her</t>
+  </si>
+  <si>
+    <t>it;her</t>
+  </si>
+  <si>
+    <t>We; Him</t>
+  </si>
+  <si>
+    <t>we;us</t>
+  </si>
+  <si>
+    <t>them;they​</t>
+  </si>
+  <si>
+    <t>they;them​</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:O151"/>
+  <dimension ref="A4:O184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="H166" zoomScale="137" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="J185" sqref="J185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5353,8 +5491,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E119" s="1"/>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" t="s">
+        <v>218</v>
+      </c>
+      <c r="C118" t="s">
+        <v>20</v>
+      </c>
+      <c r="D118" t="s">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>244</v>
+      </c>
+      <c r="G118" t="s">
+        <v>2</v>
+      </c>
+      <c r="H118" t="s">
+        <v>246</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J118" t="s">
+        <v>2</v>
+      </c>
+      <c r="K118" t="s">
+        <v>10</v>
+      </c>
+      <c r="L118" t="s">
+        <v>2</v>
+      </c>
+      <c r="M118" t="s">
+        <v>2</v>
+      </c>
+      <c r="N118" t="s">
+        <v>2</v>
+      </c>
+      <c r="O118" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
@@ -5497,39 +5679,133 @@
         <v>2</v>
       </c>
     </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" t="s">
+        <v>218</v>
+      </c>
+      <c r="C136" t="s">
+        <v>101</v>
+      </c>
+      <c r="D136" t="s">
+        <v>2</v>
+      </c>
+      <c r="E136" t="s">
+        <v>2</v>
+      </c>
+      <c r="F136" t="s">
+        <v>247</v>
+      </c>
+      <c r="G136" t="s">
+        <v>2</v>
+      </c>
+      <c r="H136" t="s">
+        <v>248</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J136" t="s">
+        <v>2</v>
+      </c>
+      <c r="K136" t="s">
+        <v>200</v>
+      </c>
+      <c r="L136" t="s">
+        <v>2</v>
+      </c>
+      <c r="M136" t="s">
+        <v>2</v>
+      </c>
+      <c r="N136" t="s">
+        <v>2</v>
+      </c>
+      <c r="O136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>218</v>
+      </c>
+      <c r="C137" t="s">
+        <v>101</v>
+      </c>
+      <c r="D137" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" t="s">
+        <v>2</v>
+      </c>
+      <c r="F137" t="s">
+        <v>249</v>
+      </c>
+      <c r="G137" t="s">
+        <v>2</v>
+      </c>
+      <c r="H137" t="s">
+        <v>250</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J137" t="s">
+        <v>2</v>
+      </c>
+      <c r="K137" t="s">
+        <v>200</v>
+      </c>
+      <c r="L137" t="s">
+        <v>2</v>
+      </c>
+      <c r="M137" t="s">
+        <v>2</v>
+      </c>
+      <c r="N137" t="s">
+        <v>2</v>
+      </c>
+      <c r="O137" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>0</v>
       </c>
       <c r="B138" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="C138" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
       </c>
-      <c r="E138" s="1" t="s">
-        <v>3</v>
+      <c r="E138" t="s">
+        <v>2</v>
       </c>
       <c r="F138" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="G138" t="s">
         <v>2</v>
       </c>
       <c r="H138" t="s">
-        <v>107</v>
-      </c>
-      <c r="I138" t="s">
+        <v>252</v>
+      </c>
+      <c r="I138" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J138" t="s">
         <v>2</v>
       </c>
       <c r="K138" t="s">
-        <v>11</v>
+        <v>253</v>
       </c>
       <c r="L138" t="s">
         <v>2</v>
@@ -5549,10 +5825,10 @@
         <v>0</v>
       </c>
       <c r="B139" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="C139" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D139" t="s">
         <v>2</v>
@@ -5561,22 +5837,22 @@
         <v>2</v>
       </c>
       <c r="F139" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
       <c r="G139" t="s">
         <v>2</v>
       </c>
       <c r="H139" t="s">
-        <v>108</v>
-      </c>
-      <c r="I139" t="s">
-        <v>2</v>
-      </c>
-      <c r="J139" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="I139" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
       </c>
       <c r="K139" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L139" t="s">
         <v>2</v>
@@ -5596,10 +5872,10 @@
         <v>0</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="C140" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D140" t="s">
         <v>2</v>
@@ -5608,22 +5884,22 @@
         <v>2</v>
       </c>
       <c r="F140" t="s">
-        <v>14</v>
+        <v>254</v>
       </c>
       <c r="G140" t="s">
         <v>2</v>
       </c>
       <c r="H140" t="s">
-        <v>144</v>
-      </c>
-      <c r="I140" t="s">
-        <v>2</v>
-      </c>
-      <c r="J140" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="I140" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
       </c>
       <c r="K140" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L140" t="s">
         <v>2</v>
@@ -5643,10 +5919,10 @@
         <v>0</v>
       </c>
       <c r="B141" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C141" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D141" t="s">
         <v>2</v>
@@ -5655,7 +5931,7 @@
         <v>2</v>
       </c>
       <c r="F141" t="s">
-        <v>2</v>
+        <v>254</v>
       </c>
       <c r="G141" t="s">
         <v>2</v>
@@ -5663,26 +5939,26 @@
       <c r="H141" t="s">
         <v>2</v>
       </c>
-      <c r="I141" t="s">
-        <v>2</v>
-      </c>
-      <c r="J141" t="s">
+      <c r="I141" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J141">
         <v>2</v>
       </c>
       <c r="K141" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L141" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="M141" t="s">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="N141" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="O141" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.2">
@@ -5690,10 +5966,10 @@
         <v>0</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C142" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D142" t="s">
         <v>2</v>
@@ -5702,19 +5978,19 @@
         <v>2</v>
       </c>
       <c r="F142" t="s">
-        <v>113</v>
+        <v>254</v>
       </c>
       <c r="G142" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="H142" t="s">
-        <v>115</v>
-      </c>
-      <c r="I142" t="s">
-        <v>116</v>
+        <v>2</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="J142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K142" t="s">
         <v>15</v>
@@ -5737,10 +6013,10 @@
         <v>0</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C143" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D143" t="s">
         <v>2</v>
@@ -5749,16 +6025,16 @@
         <v>2</v>
       </c>
       <c r="F143" t="s">
-        <v>118</v>
+        <v>254</v>
       </c>
       <c r="G143" t="s">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="H143" t="s">
         <v>2</v>
       </c>
-      <c r="I143" t="s">
-        <v>135</v>
+      <c r="I143" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="J143">
         <v>1</v>
@@ -5784,10 +6060,10 @@
         <v>0</v>
       </c>
       <c r="B144" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C144" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D144" t="s">
         <v>2</v>
@@ -5796,19 +6072,19 @@
         <v>2</v>
       </c>
       <c r="F144" t="s">
-        <v>120</v>
+        <v>254</v>
       </c>
       <c r="G144" t="s">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="H144" t="s">
         <v>2</v>
       </c>
-      <c r="I144" t="s">
-        <v>136</v>
+      <c r="I144" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="J144">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K144" t="s">
         <v>15</v>
@@ -5831,10 +6107,10 @@
         <v>0</v>
       </c>
       <c r="B145" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C145" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D145" t="s">
         <v>2</v>
@@ -5843,19 +6119,19 @@
         <v>2</v>
       </c>
       <c r="F145" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
       <c r="G145" t="s">
-        <v>122</v>
+        <v>2</v>
       </c>
       <c r="H145" t="s">
         <v>2</v>
       </c>
-      <c r="I145" t="s">
-        <v>137</v>
+      <c r="I145" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="J145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K145" t="s">
         <v>15</v>
@@ -5878,10 +6154,10 @@
         <v>0</v>
       </c>
       <c r="B146" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D146" t="s">
         <v>2</v>
@@ -5890,19 +6166,19 @@
         <v>2</v>
       </c>
       <c r="F146" t="s">
-        <v>123</v>
+        <v>254</v>
       </c>
       <c r="G146" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="H146" t="s">
         <v>2</v>
       </c>
-      <c r="I146" t="s">
-        <v>138</v>
+      <c r="I146" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="J146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K146" t="s">
         <v>15</v>
@@ -5925,233 +6201,1314 @@
         <v>0</v>
       </c>
       <c r="B147" t="s">
+        <v>218</v>
+      </c>
+      <c r="C147" t="s">
+        <v>101</v>
+      </c>
+      <c r="D147" t="s">
+        <v>2</v>
+      </c>
+      <c r="E147" t="s">
+        <v>2</v>
+      </c>
+      <c r="F147" t="s">
+        <v>254</v>
+      </c>
+      <c r="G147" t="s">
+        <v>2</v>
+      </c>
+      <c r="H147" t="s">
+        <v>2</v>
+      </c>
+      <c r="I147" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="K147" t="s">
+        <v>15</v>
+      </c>
+      <c r="L147" t="s">
+        <v>2</v>
+      </c>
+      <c r="M147" t="s">
+        <v>2</v>
+      </c>
+      <c r="N147" t="s">
+        <v>2</v>
+      </c>
+      <c r="O147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B158" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" t="s">
+        <v>105</v>
+      </c>
+      <c r="D158" t="s">
+        <v>2</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F158" t="s">
+        <v>19</v>
+      </c>
+      <c r="G158" t="s">
+        <v>2</v>
+      </c>
+      <c r="H158" t="s">
+        <v>107</v>
+      </c>
+      <c r="I158" t="s">
+        <v>2</v>
+      </c>
+      <c r="J158" t="s">
+        <v>2</v>
+      </c>
+      <c r="K158" t="s">
+        <v>11</v>
+      </c>
+      <c r="L158" t="s">
+        <v>2</v>
+      </c>
+      <c r="M158" t="s">
+        <v>2</v>
+      </c>
+      <c r="N158" t="s">
+        <v>2</v>
+      </c>
+      <c r="O158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" t="s">
+        <v>106</v>
+      </c>
+      <c r="D159" t="s">
+        <v>2</v>
+      </c>
+      <c r="E159" t="s">
+        <v>2</v>
+      </c>
+      <c r="F159" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" t="s">
+        <v>2</v>
+      </c>
+      <c r="H159" t="s">
+        <v>108</v>
+      </c>
+      <c r="I159" t="s">
+        <v>2</v>
+      </c>
+      <c r="J159" t="s">
+        <v>2</v>
+      </c>
+      <c r="K159" t="s">
+        <v>11</v>
+      </c>
+      <c r="L159" t="s">
+        <v>2</v>
+      </c>
+      <c r="M159" t="s">
+        <v>2</v>
+      </c>
+      <c r="N159" t="s">
+        <v>2</v>
+      </c>
+      <c r="O159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" t="s">
+        <v>105</v>
+      </c>
+      <c r="D160" t="s">
+        <v>2</v>
+      </c>
+      <c r="E160" t="s">
+        <v>2</v>
+      </c>
+      <c r="F160" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" t="s">
+        <v>2</v>
+      </c>
+      <c r="H160" t="s">
+        <v>144</v>
+      </c>
+      <c r="I160" t="s">
+        <v>2</v>
+      </c>
+      <c r="J160" t="s">
+        <v>2</v>
+      </c>
+      <c r="K160" t="s">
+        <v>11</v>
+      </c>
+      <c r="L160" t="s">
+        <v>2</v>
+      </c>
+      <c r="M160" t="s">
+        <v>2</v>
+      </c>
+      <c r="N160" t="s">
+        <v>2</v>
+      </c>
+      <c r="O160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161" t="s">
         <v>216</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C161" t="s">
         <v>105</v>
       </c>
-      <c r="D147" t="s">
-        <v>2</v>
-      </c>
-      <c r="E147" t="s">
-        <v>2</v>
-      </c>
-      <c r="F147" t="s">
+      <c r="D161" t="s">
+        <v>2</v>
+      </c>
+      <c r="E161" t="s">
+        <v>2</v>
+      </c>
+      <c r="F161" t="s">
+        <v>2</v>
+      </c>
+      <c r="G161" t="s">
+        <v>2</v>
+      </c>
+      <c r="H161" t="s">
+        <v>2</v>
+      </c>
+      <c r="I161" t="s">
+        <v>2</v>
+      </c>
+      <c r="J161" t="s">
+        <v>2</v>
+      </c>
+      <c r="K161" t="s">
+        <v>4</v>
+      </c>
+      <c r="L161" t="s">
+        <v>109</v>
+      </c>
+      <c r="M161" t="s">
+        <v>110</v>
+      </c>
+      <c r="N161" t="s">
+        <v>111</v>
+      </c>
+      <c r="O161" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" t="s">
+        <v>216</v>
+      </c>
+      <c r="C162" t="s">
+        <v>105</v>
+      </c>
+      <c r="D162" t="s">
+        <v>2</v>
+      </c>
+      <c r="E162" t="s">
+        <v>2</v>
+      </c>
+      <c r="F162" t="s">
+        <v>113</v>
+      </c>
+      <c r="G162" t="s">
+        <v>114</v>
+      </c>
+      <c r="H162" t="s">
+        <v>115</v>
+      </c>
+      <c r="I162" t="s">
+        <v>116</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="K162" t="s">
+        <v>15</v>
+      </c>
+      <c r="L162" t="s">
+        <v>2</v>
+      </c>
+      <c r="M162" t="s">
+        <v>2</v>
+      </c>
+      <c r="N162" t="s">
+        <v>2</v>
+      </c>
+      <c r="O162" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>0</v>
+      </c>
+      <c r="B163" t="s">
+        <v>216</v>
+      </c>
+      <c r="C163" t="s">
+        <v>105</v>
+      </c>
+      <c r="D163" t="s">
+        <v>2</v>
+      </c>
+      <c r="E163" t="s">
+        <v>2</v>
+      </c>
+      <c r="F163" t="s">
+        <v>118</v>
+      </c>
+      <c r="G163" t="s">
+        <v>117</v>
+      </c>
+      <c r="H163" t="s">
+        <v>2</v>
+      </c>
+      <c r="I163" t="s">
+        <v>135</v>
+      </c>
+      <c r="J163">
+        <v>1</v>
+      </c>
+      <c r="K163" t="s">
+        <v>15</v>
+      </c>
+      <c r="L163" t="s">
+        <v>2</v>
+      </c>
+      <c r="M163" t="s">
+        <v>2</v>
+      </c>
+      <c r="N163" t="s">
+        <v>2</v>
+      </c>
+      <c r="O163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" t="s">
+        <v>216</v>
+      </c>
+      <c r="C164" t="s">
+        <v>105</v>
+      </c>
+      <c r="D164" t="s">
+        <v>2</v>
+      </c>
+      <c r="E164" t="s">
+        <v>2</v>
+      </c>
+      <c r="F164" t="s">
+        <v>120</v>
+      </c>
+      <c r="G164" t="s">
+        <v>119</v>
+      </c>
+      <c r="H164" t="s">
+        <v>2</v>
+      </c>
+      <c r="I164" t="s">
+        <v>136</v>
+      </c>
+      <c r="J164">
+        <v>1</v>
+      </c>
+      <c r="K164" t="s">
+        <v>15</v>
+      </c>
+      <c r="L164" t="s">
+        <v>2</v>
+      </c>
+      <c r="M164" t="s">
+        <v>2</v>
+      </c>
+      <c r="N164" t="s">
+        <v>2</v>
+      </c>
+      <c r="O164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" t="s">
+        <v>216</v>
+      </c>
+      <c r="C165" t="s">
+        <v>105</v>
+      </c>
+      <c r="D165" t="s">
+        <v>2</v>
+      </c>
+      <c r="E165" t="s">
+        <v>2</v>
+      </c>
+      <c r="F165" t="s">
+        <v>121</v>
+      </c>
+      <c r="G165" t="s">
+        <v>122</v>
+      </c>
+      <c r="H165" t="s">
+        <v>2</v>
+      </c>
+      <c r="I165" t="s">
+        <v>137</v>
+      </c>
+      <c r="J165">
+        <v>1</v>
+      </c>
+      <c r="K165" t="s">
+        <v>15</v>
+      </c>
+      <c r="L165" t="s">
+        <v>2</v>
+      </c>
+      <c r="M165" t="s">
+        <v>2</v>
+      </c>
+      <c r="N165" t="s">
+        <v>2</v>
+      </c>
+      <c r="O165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" t="s">
+        <v>216</v>
+      </c>
+      <c r="C166" t="s">
+        <v>105</v>
+      </c>
+      <c r="D166" t="s">
+        <v>2</v>
+      </c>
+      <c r="E166" t="s">
+        <v>2</v>
+      </c>
+      <c r="F166" t="s">
+        <v>123</v>
+      </c>
+      <c r="G166" t="s">
+        <v>124</v>
+      </c>
+      <c r="H166" t="s">
+        <v>2</v>
+      </c>
+      <c r="I166" t="s">
+        <v>138</v>
+      </c>
+      <c r="J166">
+        <v>1</v>
+      </c>
+      <c r="K166" t="s">
+        <v>15</v>
+      </c>
+      <c r="L166" t="s">
+        <v>2</v>
+      </c>
+      <c r="M166" t="s">
+        <v>2</v>
+      </c>
+      <c r="N166" t="s">
+        <v>2</v>
+      </c>
+      <c r="O166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>0</v>
+      </c>
+      <c r="B167" t="s">
+        <v>216</v>
+      </c>
+      <c r="C167" t="s">
+        <v>105</v>
+      </c>
+      <c r="D167" t="s">
+        <v>2</v>
+      </c>
+      <c r="E167" t="s">
+        <v>2</v>
+      </c>
+      <c r="F167" t="s">
         <v>125</v>
       </c>
-      <c r="G147" t="s">
+      <c r="G167" t="s">
         <v>126</v>
       </c>
-      <c r="H147" t="s">
-        <v>2</v>
-      </c>
-      <c r="I147" t="s">
+      <c r="H167" t="s">
+        <v>2</v>
+      </c>
+      <c r="I167" t="s">
         <v>139</v>
       </c>
-      <c r="J147">
-        <v>1</v>
-      </c>
-      <c r="K147" t="s">
-        <v>15</v>
-      </c>
-      <c r="L147" t="s">
-        <v>2</v>
-      </c>
-      <c r="M147" t="s">
-        <v>2</v>
-      </c>
-      <c r="N147" t="s">
-        <v>2</v>
-      </c>
-      <c r="O147" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>0</v>
-      </c>
-      <c r="B148" t="s">
+      <c r="J167">
+        <v>1</v>
+      </c>
+      <c r="K167" t="s">
+        <v>15</v>
+      </c>
+      <c r="L167" t="s">
+        <v>2</v>
+      </c>
+      <c r="M167" t="s">
+        <v>2</v>
+      </c>
+      <c r="N167" t="s">
+        <v>2</v>
+      </c>
+      <c r="O167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" t="s">
         <v>216</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C168" t="s">
         <v>105</v>
       </c>
-      <c r="D148" t="s">
-        <v>2</v>
-      </c>
-      <c r="E148" t="s">
-        <v>2</v>
-      </c>
-      <c r="F148" t="s">
+      <c r="D168" t="s">
+        <v>2</v>
+      </c>
+      <c r="E168" t="s">
+        <v>2</v>
+      </c>
+      <c r="F168" t="s">
         <v>127</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G168" t="s">
         <v>128</v>
       </c>
-      <c r="H148" t="s">
-        <v>2</v>
-      </c>
-      <c r="I148" t="s">
+      <c r="H168" t="s">
+        <v>2</v>
+      </c>
+      <c r="I168" t="s">
         <v>140</v>
       </c>
-      <c r="J148">
-        <v>0</v>
-      </c>
-      <c r="K148" t="s">
-        <v>15</v>
-      </c>
-      <c r="L148" t="s">
-        <v>2</v>
-      </c>
-      <c r="M148" t="s">
-        <v>2</v>
-      </c>
-      <c r="N148" t="s">
-        <v>2</v>
-      </c>
-      <c r="O148" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>0</v>
-      </c>
-      <c r="B149" t="s">
+      <c r="J168">
+        <v>0</v>
+      </c>
+      <c r="K168" t="s">
+        <v>15</v>
+      </c>
+      <c r="L168" t="s">
+        <v>2</v>
+      </c>
+      <c r="M168" t="s">
+        <v>2</v>
+      </c>
+      <c r="N168" t="s">
+        <v>2</v>
+      </c>
+      <c r="O168" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169" t="s">
         <v>216</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C169" t="s">
         <v>105</v>
       </c>
-      <c r="D149" t="s">
-        <v>2</v>
-      </c>
-      <c r="E149" t="s">
-        <v>2</v>
-      </c>
-      <c r="F149" t="s">
+      <c r="D169" t="s">
+        <v>2</v>
+      </c>
+      <c r="E169" t="s">
+        <v>2</v>
+      </c>
+      <c r="F169" t="s">
         <v>129</v>
       </c>
-      <c r="G149" t="s">
+      <c r="G169" t="s">
         <v>130</v>
       </c>
-      <c r="H149" t="s">
-        <v>2</v>
-      </c>
-      <c r="I149" t="s">
+      <c r="H169" t="s">
+        <v>2</v>
+      </c>
+      <c r="I169" t="s">
         <v>141</v>
       </c>
-      <c r="J149">
-        <v>1</v>
-      </c>
-      <c r="K149" t="s">
-        <v>15</v>
-      </c>
-      <c r="L149" t="s">
-        <v>2</v>
-      </c>
-      <c r="M149" t="s">
-        <v>2</v>
-      </c>
-      <c r="N149" t="s">
-        <v>2</v>
-      </c>
-      <c r="O149" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>0</v>
-      </c>
-      <c r="B150" t="s">
+      <c r="J169">
+        <v>1</v>
+      </c>
+      <c r="K169" t="s">
+        <v>15</v>
+      </c>
+      <c r="L169" t="s">
+        <v>2</v>
+      </c>
+      <c r="M169" t="s">
+        <v>2</v>
+      </c>
+      <c r="N169" t="s">
+        <v>2</v>
+      </c>
+      <c r="O169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" t="s">
         <v>216</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C170" t="s">
         <v>105</v>
       </c>
-      <c r="D150" t="s">
-        <v>2</v>
-      </c>
-      <c r="E150" t="s">
-        <v>2</v>
-      </c>
-      <c r="F150" t="s">
+      <c r="D170" t="s">
+        <v>2</v>
+      </c>
+      <c r="E170" t="s">
+        <v>2</v>
+      </c>
+      <c r="F170" t="s">
         <v>131</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G170" t="s">
         <v>132</v>
       </c>
-      <c r="H150" t="s">
-        <v>2</v>
-      </c>
-      <c r="I150" t="s">
+      <c r="H170" t="s">
+        <v>2</v>
+      </c>
+      <c r="I170" t="s">
         <v>142</v>
       </c>
-      <c r="J150">
-        <v>1</v>
-      </c>
-      <c r="K150" t="s">
-        <v>15</v>
-      </c>
-      <c r="L150" t="s">
-        <v>2</v>
-      </c>
-      <c r="M150" t="s">
-        <v>2</v>
-      </c>
-      <c r="N150" t="s">
-        <v>2</v>
-      </c>
-      <c r="O150" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>0</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="K170" t="s">
+        <v>15</v>
+      </c>
+      <c r="L170" t="s">
+        <v>2</v>
+      </c>
+      <c r="M170" t="s">
+        <v>2</v>
+      </c>
+      <c r="N170" t="s">
+        <v>2</v>
+      </c>
+      <c r="O170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" t="s">
         <v>216</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C171" t="s">
         <v>105</v>
       </c>
-      <c r="D151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E151" t="s">
-        <v>2</v>
-      </c>
-      <c r="F151" t="s">
+      <c r="D171" t="s">
+        <v>2</v>
+      </c>
+      <c r="E171" t="s">
+        <v>2</v>
+      </c>
+      <c r="F171" t="s">
         <v>133</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G171" t="s">
         <v>134</v>
       </c>
-      <c r="H151" t="s">
-        <v>2</v>
-      </c>
-      <c r="I151" t="s">
+      <c r="H171" t="s">
+        <v>2</v>
+      </c>
+      <c r="I171" t="s">
         <v>143</v>
       </c>
-      <c r="J151">
-        <v>1</v>
-      </c>
-      <c r="K151" t="s">
-        <v>15</v>
-      </c>
-      <c r="L151" t="s">
-        <v>2</v>
-      </c>
-      <c r="M151" t="s">
-        <v>2</v>
-      </c>
-      <c r="N151" t="s">
-        <v>2</v>
-      </c>
-      <c r="O151" t="s">
+      <c r="J171">
+        <v>1</v>
+      </c>
+      <c r="K171" t="s">
+        <v>15</v>
+      </c>
+      <c r="L171" t="s">
+        <v>2</v>
+      </c>
+      <c r="M171" t="s">
+        <v>2</v>
+      </c>
+      <c r="N171" t="s">
+        <v>2</v>
+      </c>
+      <c r="O171" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>0</v>
+      </c>
+      <c r="B172" t="s">
+        <v>218</v>
+      </c>
+      <c r="C172" t="s">
+        <v>105</v>
+      </c>
+      <c r="D172" t="s">
+        <v>2</v>
+      </c>
+      <c r="E172" t="s">
+        <v>2</v>
+      </c>
+      <c r="F172" t="s">
+        <v>244</v>
+      </c>
+      <c r="G172" t="s">
+        <v>2</v>
+      </c>
+      <c r="H172" t="s">
+        <v>265</v>
+      </c>
+      <c r="I172" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J172" t="s">
+        <v>2</v>
+      </c>
+      <c r="K172" t="s">
+        <v>10</v>
+      </c>
+      <c r="L172" t="s">
+        <v>2</v>
+      </c>
+      <c r="M172" t="s">
+        <v>2</v>
+      </c>
+      <c r="N172" t="s">
+        <v>2</v>
+      </c>
+      <c r="O172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" t="s">
+        <v>218</v>
+      </c>
+      <c r="C173" t="s">
+        <v>105</v>
+      </c>
+      <c r="D173" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" t="s">
+        <v>2</v>
+      </c>
+      <c r="F173" t="s">
+        <v>266</v>
+      </c>
+      <c r="G173" t="s">
+        <v>2</v>
+      </c>
+      <c r="H173" t="s">
+        <v>278</v>
+      </c>
+      <c r="I173" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="J173">
+        <v>1</v>
+      </c>
+      <c r="K173" t="s">
+        <v>15</v>
+      </c>
+      <c r="L173" t="s">
+        <v>2</v>
+      </c>
+      <c r="M173" t="s">
+        <v>2</v>
+      </c>
+      <c r="N173" t="s">
+        <v>2</v>
+      </c>
+      <c r="O173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" t="s">
+        <v>218</v>
+      </c>
+      <c r="C174" t="s">
+        <v>105</v>
+      </c>
+      <c r="D174" t="s">
+        <v>2</v>
+      </c>
+      <c r="E174" t="s">
+        <v>2</v>
+      </c>
+      <c r="F174" t="s">
+        <v>266</v>
+      </c>
+      <c r="G174" t="s">
+        <v>2</v>
+      </c>
+      <c r="H174" t="s">
+        <v>267</v>
+      </c>
+      <c r="I174" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+      <c r="K174" t="s">
+        <v>15</v>
+      </c>
+      <c r="L174" t="s">
+        <v>2</v>
+      </c>
+      <c r="M174" t="s">
+        <v>2</v>
+      </c>
+      <c r="N174" t="s">
+        <v>2</v>
+      </c>
+      <c r="O174" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" t="s">
+        <v>218</v>
+      </c>
+      <c r="C175" t="s">
+        <v>105</v>
+      </c>
+      <c r="D175" t="s">
+        <v>2</v>
+      </c>
+      <c r="E175" t="s">
+        <v>2</v>
+      </c>
+      <c r="F175" t="s">
+        <v>266</v>
+      </c>
+      <c r="G175" t="s">
+        <v>2</v>
+      </c>
+      <c r="H175" t="s">
+        <v>268</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J175">
+        <v>1</v>
+      </c>
+      <c r="K175" t="s">
+        <v>15</v>
+      </c>
+      <c r="L175" t="s">
+        <v>2</v>
+      </c>
+      <c r="M175" t="s">
+        <v>2</v>
+      </c>
+      <c r="N175" t="s">
+        <v>2</v>
+      </c>
+      <c r="O175" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>0</v>
+      </c>
+      <c r="B176" t="s">
+        <v>218</v>
+      </c>
+      <c r="C176" t="s">
+        <v>105</v>
+      </c>
+      <c r="D176" t="s">
+        <v>2</v>
+      </c>
+      <c r="E176" t="s">
+        <v>2</v>
+      </c>
+      <c r="F176" t="s">
+        <v>266</v>
+      </c>
+      <c r="G176" t="s">
+        <v>2</v>
+      </c>
+      <c r="H176" t="s">
+        <v>269</v>
+      </c>
+      <c r="I176" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="J176">
+        <v>1</v>
+      </c>
+      <c r="K176" t="s">
+        <v>15</v>
+      </c>
+      <c r="L176" t="s">
+        <v>2</v>
+      </c>
+      <c r="M176" t="s">
+        <v>2</v>
+      </c>
+      <c r="N176" t="s">
+        <v>2</v>
+      </c>
+      <c r="O176" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" t="s">
+        <v>218</v>
+      </c>
+      <c r="C177" t="s">
+        <v>105</v>
+      </c>
+      <c r="D177" t="s">
+        <v>2</v>
+      </c>
+      <c r="E177" t="s">
+        <v>2</v>
+      </c>
+      <c r="F177" t="s">
+        <v>266</v>
+      </c>
+      <c r="G177" t="s">
+        <v>2</v>
+      </c>
+      <c r="H177" t="s">
+        <v>270</v>
+      </c>
+      <c r="I177" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="J177">
+        <v>1</v>
+      </c>
+      <c r="K177" t="s">
+        <v>15</v>
+      </c>
+      <c r="L177" t="s">
+        <v>2</v>
+      </c>
+      <c r="M177" t="s">
+        <v>2</v>
+      </c>
+      <c r="N177" t="s">
+        <v>2</v>
+      </c>
+      <c r="O177" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B178" t="s">
+        <v>218</v>
+      </c>
+      <c r="C178" t="s">
+        <v>105</v>
+      </c>
+      <c r="D178" t="s">
+        <v>2</v>
+      </c>
+      <c r="E178" t="s">
+        <v>2</v>
+      </c>
+      <c r="F178" t="s">
+        <v>266</v>
+      </c>
+      <c r="G178" t="s">
+        <v>2</v>
+      </c>
+      <c r="H178" t="s">
+        <v>271</v>
+      </c>
+      <c r="I178" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J178">
+        <v>1</v>
+      </c>
+      <c r="K178" t="s">
+        <v>15</v>
+      </c>
+      <c r="L178" t="s">
+        <v>2</v>
+      </c>
+      <c r="M178" t="s">
+        <v>2</v>
+      </c>
+      <c r="N178" t="s">
+        <v>2</v>
+      </c>
+      <c r="O178" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" t="s">
+        <v>218</v>
+      </c>
+      <c r="C179" t="s">
+        <v>105</v>
+      </c>
+      <c r="D179" t="s">
+        <v>2</v>
+      </c>
+      <c r="E179" t="s">
+        <v>2</v>
+      </c>
+      <c r="F179" t="s">
+        <v>266</v>
+      </c>
+      <c r="G179" t="s">
+        <v>2</v>
+      </c>
+      <c r="H179" t="s">
+        <v>272</v>
+      </c>
+      <c r="I179" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J179">
+        <v>1</v>
+      </c>
+      <c r="K179" t="s">
+        <v>15</v>
+      </c>
+      <c r="L179" t="s">
+        <v>2</v>
+      </c>
+      <c r="M179" t="s">
+        <v>2</v>
+      </c>
+      <c r="N179" t="s">
+        <v>2</v>
+      </c>
+      <c r="O179" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>0</v>
+      </c>
+      <c r="B180" t="s">
+        <v>218</v>
+      </c>
+      <c r="C180" t="s">
+        <v>105</v>
+      </c>
+      <c r="D180" t="s">
+        <v>2</v>
+      </c>
+      <c r="E180" t="s">
+        <v>2</v>
+      </c>
+      <c r="F180" t="s">
+        <v>266</v>
+      </c>
+      <c r="G180" t="s">
+        <v>2</v>
+      </c>
+      <c r="H180" t="s">
+        <v>277</v>
+      </c>
+      <c r="I180" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+      <c r="K180" t="s">
+        <v>15</v>
+      </c>
+      <c r="L180" t="s">
+        <v>2</v>
+      </c>
+      <c r="M180" t="s">
+        <v>2</v>
+      </c>
+      <c r="N180" t="s">
+        <v>2</v>
+      </c>
+      <c r="O180" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B181" t="s">
+        <v>218</v>
+      </c>
+      <c r="C181" t="s">
+        <v>105</v>
+      </c>
+      <c r="D181" t="s">
+        <v>2</v>
+      </c>
+      <c r="E181" t="s">
+        <v>2</v>
+      </c>
+      <c r="F181" t="s">
+        <v>266</v>
+      </c>
+      <c r="G181" t="s">
+        <v>2</v>
+      </c>
+      <c r="H181" t="s">
+        <v>273</v>
+      </c>
+      <c r="I181" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+      <c r="K181" t="s">
+        <v>15</v>
+      </c>
+      <c r="L181" t="s">
+        <v>2</v>
+      </c>
+      <c r="M181" t="s">
+        <v>2</v>
+      </c>
+      <c r="N181" t="s">
+        <v>2</v>
+      </c>
+      <c r="O181" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" t="s">
+        <v>218</v>
+      </c>
+      <c r="C182" t="s">
+        <v>105</v>
+      </c>
+      <c r="D182" t="s">
+        <v>2</v>
+      </c>
+      <c r="E182" t="s">
+        <v>2</v>
+      </c>
+      <c r="F182" t="s">
+        <v>266</v>
+      </c>
+      <c r="G182" t="s">
+        <v>2</v>
+      </c>
+      <c r="H182" t="s">
+        <v>274</v>
+      </c>
+      <c r="I182" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J182">
+        <v>1</v>
+      </c>
+      <c r="K182" t="s">
+        <v>15</v>
+      </c>
+      <c r="L182" t="s">
+        <v>2</v>
+      </c>
+      <c r="M182" t="s">
+        <v>2</v>
+      </c>
+      <c r="N182" t="s">
+        <v>2</v>
+      </c>
+      <c r="O182" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183" t="s">
+        <v>218</v>
+      </c>
+      <c r="C183" t="s">
+        <v>105</v>
+      </c>
+      <c r="D183" t="s">
+        <v>2</v>
+      </c>
+      <c r="E183" t="s">
+        <v>2</v>
+      </c>
+      <c r="F183" t="s">
+        <v>266</v>
+      </c>
+      <c r="G183" t="s">
+        <v>2</v>
+      </c>
+      <c r="H183" t="s">
+        <v>275</v>
+      </c>
+      <c r="I183" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="K183" t="s">
+        <v>15</v>
+      </c>
+      <c r="L183" t="s">
+        <v>2</v>
+      </c>
+      <c r="M183" t="s">
+        <v>2</v>
+      </c>
+      <c r="N183" t="s">
+        <v>2</v>
+      </c>
+      <c r="O183" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" t="s">
+        <v>218</v>
+      </c>
+      <c r="C184" t="s">
+        <v>105</v>
+      </c>
+      <c r="D184" t="s">
+        <v>2</v>
+      </c>
+      <c r="E184" t="s">
+        <v>2</v>
+      </c>
+      <c r="F184" t="s">
+        <v>266</v>
+      </c>
+      <c r="G184" t="s">
+        <v>2</v>
+      </c>
+      <c r="H184" t="s">
+        <v>276</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184" t="s">
+        <v>15</v>
+      </c>
+      <c r="L184" t="s">
+        <v>2</v>
+      </c>
+      <c r="M184" t="s">
+        <v>2</v>
+      </c>
+      <c r="N184" t="s">
+        <v>2</v>
+      </c>
+      <c r="O184" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: add support nullable fields in question parsing and remove unused question types
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57BAE71-46C6-3745-8AB6-63D560E1824B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8454403-240C-F542-91D0-2ABF697AEA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2860" windowWidth="33600" windowHeight="20500" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4948" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4996" uniqueCount="598">
   <si>
     <t>A1</t>
   </si>
@@ -1822,6 +1822,18 @@
   </si>
   <si>
     <t>a1_day4_test_9</t>
+  </si>
+  <si>
+    <t>dictation</t>
+  </si>
+  <si>
+    <t>Milk  حليب:  I drink milk before sleeping  انا اشرب الحليب قبل النوم;Numbers  ارقام : I know numbers in Italian  اعلم الارقام بالايطالية;Olive  زيتون : I eat olive during breakfast  اكل زيتون على الفطور;People ناس  : There are many people in here  هناك الكثير من الناس هنا;Queen ملكة : The queen died last year الملكة ماتت العام الماضي;Rainbow قوس قزح : There is a rainbow outside  هناك قوس قزح بالخارج;Spoon  حساء  : Soup is eaten with a spoon  الحساء يأكل بالملعقة;Turtle  سلحفاة :  Turtles walk so slow السلاحف يمشون ببطئ;Umbrella   مظلة :  Don’t forget your umbrella لاتنسى مظلتك;Voice  صوت  : She has a nice voice لديها صوت جميل;Water  ماء : Water is so important الماء مهم جدا;Yogurt لبن : We need to bring Yogurt نحتاج الى شراء اللبن</t>
+  </si>
+  <si>
+    <t>Don’t forget your umbrella لاتنسى مظلتك;Water is so important الماء مهم جدا;She has a nice voice لديها صوت جميل;There are many people in here  هناك الكثير من الناس هنا</t>
+  </si>
+  <si>
+    <t>Lina wakes up early. She drinks a glass of milk. She likes milk very much.;Lina sees her pet turtle in the garden. The turtle is slow but cute. Lina counts the flowers in the garden. The number of flowers is five.;Lina goes to the kitchen. She takes a spoon and eats yogurt for breakfast.; She also eats some olives. Olives are the best .</t>
   </si>
 </sst>
 </file>
@@ -2211,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
-  <dimension ref="A4:P507"/>
+  <dimension ref="A4:P506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="H320" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="P333" sqref="P333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6036,7 +6048,7 @@
         <v>2</v>
       </c>
       <c r="K103" t="s">
-        <v>18</v>
+        <v>594</v>
       </c>
       <c r="L103" t="s">
         <v>2</v>
@@ -6186,7 +6198,7 @@
         <v>2</v>
       </c>
       <c r="K106" t="s">
-        <v>18</v>
+        <v>594</v>
       </c>
       <c r="L106" t="s">
         <v>2</v>
@@ -12802,6 +12814,206 @@
         <v>2</v>
       </c>
     </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>0</v>
+      </c>
+      <c r="B330" t="s">
+        <v>11</v>
+      </c>
+      <c r="C330" t="s">
+        <v>100</v>
+      </c>
+      <c r="D330" t="s">
+        <v>2</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F330" t="s">
+        <v>13</v>
+      </c>
+      <c r="G330" t="s">
+        <v>2</v>
+      </c>
+      <c r="H330" t="s">
+        <v>595</v>
+      </c>
+      <c r="I330" t="s">
+        <v>2</v>
+      </c>
+      <c r="J330" t="s">
+        <v>2</v>
+      </c>
+      <c r="K330" t="s">
+        <v>11</v>
+      </c>
+      <c r="L330" t="s">
+        <v>2</v>
+      </c>
+      <c r="M330" t="s">
+        <v>2</v>
+      </c>
+      <c r="N330" t="s">
+        <v>2</v>
+      </c>
+      <c r="O330" t="s">
+        <v>2</v>
+      </c>
+      <c r="P330" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>0</v>
+      </c>
+      <c r="B331" t="s">
+        <v>11</v>
+      </c>
+      <c r="C331" t="s">
+        <v>100</v>
+      </c>
+      <c r="D331" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" t="s">
+        <v>2</v>
+      </c>
+      <c r="F331" t="s">
+        <v>12</v>
+      </c>
+      <c r="G331" t="s">
+        <v>2</v>
+      </c>
+      <c r="H331" t="s">
+        <v>596</v>
+      </c>
+      <c r="I331" t="s">
+        <v>2</v>
+      </c>
+      <c r="J331" t="s">
+        <v>2</v>
+      </c>
+      <c r="K331" t="s">
+        <v>11</v>
+      </c>
+      <c r="L331" t="s">
+        <v>2</v>
+      </c>
+      <c r="M331" t="s">
+        <v>2</v>
+      </c>
+      <c r="N331" t="s">
+        <v>2</v>
+      </c>
+      <c r="O331" t="s">
+        <v>2</v>
+      </c>
+      <c r="P331" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>0</v>
+      </c>
+      <c r="B332" t="s">
+        <v>18</v>
+      </c>
+      <c r="C332" t="s">
+        <v>100</v>
+      </c>
+      <c r="D332" t="s">
+        <v>2</v>
+      </c>
+      <c r="E332" t="s">
+        <v>2</v>
+      </c>
+      <c r="F332" t="s">
+        <v>2</v>
+      </c>
+      <c r="G332" t="s">
+        <v>2</v>
+      </c>
+      <c r="H332" t="s">
+        <v>597</v>
+      </c>
+      <c r="I332" t="s">
+        <v>2</v>
+      </c>
+      <c r="J332" t="s">
+        <v>2</v>
+      </c>
+      <c r="K332" t="s">
+        <v>594</v>
+      </c>
+      <c r="L332" t="s">
+        <v>2</v>
+      </c>
+      <c r="M332" t="s">
+        <v>2</v>
+      </c>
+      <c r="N332" t="s">
+        <v>2</v>
+      </c>
+      <c r="O332" t="s">
+        <v>2</v>
+      </c>
+      <c r="P332" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>0</v>
+      </c>
+      <c r="B334" t="s">
+        <v>210</v>
+      </c>
+      <c r="C334" t="s">
+        <v>100</v>
+      </c>
+      <c r="D334" t="s">
+        <v>2</v>
+      </c>
+      <c r="E334" t="s">
+        <v>2</v>
+      </c>
+      <c r="F334" t="s">
+        <v>240</v>
+      </c>
+      <c r="G334" t="s">
+        <v>2</v>
+      </c>
+      <c r="H334" t="s">
+        <v>2</v>
+      </c>
+      <c r="I334" t="s">
+        <v>584</v>
+      </c>
+      <c r="J334">
+        <v>1</v>
+      </c>
+      <c r="K334" t="s">
+        <v>15</v>
+      </c>
+      <c r="L334" t="s">
+        <v>2</v>
+      </c>
+      <c r="M334" t="s">
+        <v>2</v>
+      </c>
+      <c r="N334" t="s">
+        <v>2</v>
+      </c>
+      <c r="O334" t="s">
+        <v>2</v>
+      </c>
+      <c r="P334" t="s">
+        <v>585</v>
+      </c>
+    </row>
     <row r="335" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>0</v>
@@ -12828,10 +13040,10 @@
         <v>2</v>
       </c>
       <c r="I335" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J335">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K335" t="s">
         <v>15</v>
@@ -12849,7 +13061,7 @@
         <v>2</v>
       </c>
       <c r="P335" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="336" spans="1:16" x14ac:dyDescent="0.2">
@@ -12878,10 +13090,10 @@
         <v>2</v>
       </c>
       <c r="I336" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J336">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K336" t="s">
         <v>15</v>
@@ -12899,7 +13111,7 @@
         <v>2</v>
       </c>
       <c r="P336" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="337" spans="1:16" x14ac:dyDescent="0.2">
@@ -12928,7 +13140,7 @@
         <v>2</v>
       </c>
       <c r="I337" t="s">
-        <v>582</v>
+        <v>241</v>
       </c>
       <c r="J337">
         <v>0</v>
@@ -12949,7 +13161,7 @@
         <v>2</v>
       </c>
       <c r="P337" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="338" spans="1:16" x14ac:dyDescent="0.2">
@@ -12978,10 +13190,10 @@
         <v>2</v>
       </c>
       <c r="I338" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J338">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K338" t="s">
         <v>15</v>
@@ -12999,7 +13211,7 @@
         <v>2</v>
       </c>
       <c r="P338" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="339" spans="1:16" x14ac:dyDescent="0.2">
@@ -13028,10 +13240,10 @@
         <v>2</v>
       </c>
       <c r="I339" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J339">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K339" t="s">
         <v>15</v>
@@ -13049,7 +13261,7 @@
         <v>2</v>
       </c>
       <c r="P339" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="340" spans="1:16" x14ac:dyDescent="0.2">
@@ -13078,10 +13290,10 @@
         <v>2</v>
       </c>
       <c r="I340" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J340">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K340" t="s">
         <v>15</v>
@@ -13099,7 +13311,7 @@
         <v>2</v>
       </c>
       <c r="P340" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="341" spans="1:16" x14ac:dyDescent="0.2">
@@ -13128,10 +13340,10 @@
         <v>2</v>
       </c>
       <c r="I341" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J341">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K341" t="s">
         <v>15</v>
@@ -13149,7 +13361,7 @@
         <v>2</v>
       </c>
       <c r="P341" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="342" spans="1:16" x14ac:dyDescent="0.2">
@@ -13178,10 +13390,10 @@
         <v>2</v>
       </c>
       <c r="I342" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J342">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K342" t="s">
         <v>15</v>
@@ -13199,60 +13411,60 @@
         <v>2</v>
       </c>
       <c r="P342" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A343" t="s">
-        <v>0</v>
-      </c>
-      <c r="B343" t="s">
-        <v>210</v>
-      </c>
-      <c r="C343" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
+        <v>0</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C344" t="s">
         <v>100</v>
       </c>
-      <c r="D343" t="s">
-        <v>2</v>
-      </c>
-      <c r="E343" t="s">
-        <v>2</v>
-      </c>
-      <c r="F343" t="s">
-        <v>240</v>
-      </c>
-      <c r="G343" t="s">
-        <v>2</v>
-      </c>
-      <c r="H343" t="s">
-        <v>2</v>
-      </c>
-      <c r="I343" t="s">
-        <v>245</v>
-      </c>
-      <c r="J343">
-        <v>1</v>
-      </c>
-      <c r="K343" t="s">
-        <v>15</v>
-      </c>
-      <c r="L343" t="s">
-        <v>2</v>
-      </c>
-      <c r="M343" t="s">
-        <v>2</v>
-      </c>
-      <c r="N343" t="s">
-        <v>2</v>
-      </c>
-      <c r="O343" t="s">
-        <v>2</v>
-      </c>
-      <c r="P343" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="345" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D344" t="s">
+        <v>2</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F344" t="s">
+        <v>2</v>
+      </c>
+      <c r="G344" t="s">
+        <v>2</v>
+      </c>
+      <c r="H344" t="s">
+        <v>2</v>
+      </c>
+      <c r="I344" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J344" t="s">
+        <v>2</v>
+      </c>
+      <c r="K344" t="s">
+        <v>274</v>
+      </c>
+      <c r="L344" t="s">
+        <v>484</v>
+      </c>
+      <c r="M344" t="s">
+        <v>2</v>
+      </c>
+      <c r="N344" t="s">
+        <v>2</v>
+      </c>
+      <c r="O344" t="s">
+        <v>2</v>
+      </c>
+      <c r="P344" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>0</v>
       </c>
@@ -13265,17 +13477,17 @@
       <c r="D345" t="s">
         <v>2</v>
       </c>
-      <c r="E345" s="1" t="s">
+      <c r="E345" t="s">
         <v>2</v>
       </c>
       <c r="F345" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G345" t="s">
         <v>2</v>
       </c>
       <c r="H345" t="s">
-        <v>2</v>
+        <v>456</v>
       </c>
       <c r="I345" s="2" t="s">
         <v>2</v>
@@ -13284,7 +13496,7 @@
         <v>2</v>
       </c>
       <c r="K345" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L345" t="s">
         <v>484</v>
@@ -13319,13 +13531,13 @@
         <v>2</v>
       </c>
       <c r="F346" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G346" t="s">
         <v>2</v>
       </c>
       <c r="H346" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I346" s="2" t="s">
         <v>2</v>
@@ -13352,57 +13564,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A347" t="s">
-        <v>0</v>
-      </c>
-      <c r="B347" s="3" t="s">
+    <row r="348" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A348" t="s">
+        <v>0</v>
+      </c>
+      <c r="B348" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C348" t="s">
         <v>100</v>
       </c>
-      <c r="D347" t="s">
-        <v>2</v>
-      </c>
-      <c r="E347" t="s">
-        <v>2</v>
-      </c>
-      <c r="F347" t="s">
-        <v>194</v>
-      </c>
-      <c r="G347" t="s">
-        <v>2</v>
-      </c>
-      <c r="H347" t="s">
-        <v>457</v>
-      </c>
-      <c r="I347" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J347" t="s">
-        <v>2</v>
-      </c>
-      <c r="K347" t="s">
-        <v>192</v>
-      </c>
-      <c r="L347" t="s">
-        <v>484</v>
-      </c>
-      <c r="M347" t="s">
-        <v>2</v>
-      </c>
-      <c r="N347" t="s">
-        <v>2</v>
-      </c>
-      <c r="O347" t="s">
-        <v>2</v>
-      </c>
-      <c r="P347" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="349" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D348" t="s">
+        <v>2</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F348" t="s">
+        <v>2</v>
+      </c>
+      <c r="G348" t="s">
+        <v>2</v>
+      </c>
+      <c r="H348" t="s">
+        <v>2</v>
+      </c>
+      <c r="I348" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J348" t="s">
+        <v>2</v>
+      </c>
+      <c r="K348" t="s">
+        <v>274</v>
+      </c>
+      <c r="L348" t="s">
+        <v>485</v>
+      </c>
+      <c r="M348" t="s">
+        <v>2</v>
+      </c>
+      <c r="N348" t="s">
+        <v>2</v>
+      </c>
+      <c r="O348" t="s">
+        <v>2</v>
+      </c>
+      <c r="P348" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>0</v>
       </c>
@@ -13415,17 +13627,17 @@
       <c r="D349" t="s">
         <v>2</v>
       </c>
-      <c r="E349" s="1" t="s">
+      <c r="E349" t="s">
         <v>2</v>
       </c>
       <c r="F349" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G349" t="s">
         <v>2</v>
       </c>
       <c r="H349" t="s">
-        <v>2</v>
+        <v>458</v>
       </c>
       <c r="I349" s="2" t="s">
         <v>2</v>
@@ -13434,7 +13646,7 @@
         <v>2</v>
       </c>
       <c r="K349" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L349" t="s">
         <v>485</v>
@@ -13469,13 +13681,13 @@
         <v>2</v>
       </c>
       <c r="F350" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G350" t="s">
         <v>2</v>
       </c>
       <c r="H350" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I350" s="2" t="s">
         <v>2</v>
@@ -13502,57 +13714,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A351" t="s">
-        <v>0</v>
-      </c>
-      <c r="B351" s="3" t="s">
+    <row r="352" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>0</v>
+      </c>
+      <c r="B352" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C352" t="s">
         <v>100</v>
       </c>
-      <c r="D351" t="s">
-        <v>2</v>
-      </c>
-      <c r="E351" t="s">
-        <v>2</v>
-      </c>
-      <c r="F351" t="s">
-        <v>194</v>
-      </c>
-      <c r="G351" t="s">
-        <v>2</v>
-      </c>
-      <c r="H351" t="s">
-        <v>459</v>
-      </c>
-      <c r="I351" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J351" t="s">
-        <v>2</v>
-      </c>
-      <c r="K351" t="s">
-        <v>192</v>
-      </c>
-      <c r="L351" t="s">
-        <v>485</v>
-      </c>
-      <c r="M351" t="s">
-        <v>2</v>
-      </c>
-      <c r="N351" t="s">
-        <v>2</v>
-      </c>
-      <c r="O351" t="s">
-        <v>2</v>
-      </c>
-      <c r="P351" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="353" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D352" t="s">
+        <v>2</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F352" t="s">
+        <v>2</v>
+      </c>
+      <c r="G352" t="s">
+        <v>2</v>
+      </c>
+      <c r="H352" t="s">
+        <v>2</v>
+      </c>
+      <c r="I352" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J352" t="s">
+        <v>2</v>
+      </c>
+      <c r="K352" t="s">
+        <v>274</v>
+      </c>
+      <c r="L352" t="s">
+        <v>486</v>
+      </c>
+      <c r="M352" t="s">
+        <v>2</v>
+      </c>
+      <c r="N352" t="s">
+        <v>2</v>
+      </c>
+      <c r="O352" t="s">
+        <v>2</v>
+      </c>
+      <c r="P352" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>0</v>
       </c>
@@ -13565,17 +13777,17 @@
       <c r="D353" t="s">
         <v>2</v>
       </c>
-      <c r="E353" s="1" t="s">
+      <c r="E353" t="s">
         <v>2</v>
       </c>
       <c r="F353" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G353" t="s">
         <v>2</v>
       </c>
       <c r="H353" t="s">
-        <v>2</v>
+        <v>460</v>
       </c>
       <c r="I353" s="2" t="s">
         <v>2</v>
@@ -13584,7 +13796,7 @@
         <v>2</v>
       </c>
       <c r="K353" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L353" t="s">
         <v>486</v>
@@ -13619,13 +13831,13 @@
         <v>2</v>
       </c>
       <c r="F354" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G354" t="s">
         <v>2</v>
       </c>
       <c r="H354" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="I354" s="2" t="s">
         <v>2</v>
@@ -13652,57 +13864,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A355" t="s">
-        <v>0</v>
-      </c>
-      <c r="B355" s="3" t="s">
+    <row r="356" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>0</v>
+      </c>
+      <c r="B356" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C356" t="s">
         <v>100</v>
       </c>
-      <c r="D355" t="s">
-        <v>2</v>
-      </c>
-      <c r="E355" t="s">
-        <v>2</v>
-      </c>
-      <c r="F355" t="s">
-        <v>194</v>
-      </c>
-      <c r="G355" t="s">
-        <v>2</v>
-      </c>
-      <c r="H355" t="s">
-        <v>461</v>
-      </c>
-      <c r="I355" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J355" t="s">
-        <v>2</v>
-      </c>
-      <c r="K355" t="s">
-        <v>192</v>
-      </c>
-      <c r="L355" t="s">
-        <v>486</v>
-      </c>
-      <c r="M355" t="s">
-        <v>2</v>
-      </c>
-      <c r="N355" t="s">
-        <v>2</v>
-      </c>
-      <c r="O355" t="s">
-        <v>2</v>
-      </c>
-      <c r="P355" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="357" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D356" t="s">
+        <v>2</v>
+      </c>
+      <c r="E356" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F356" t="s">
+        <v>2</v>
+      </c>
+      <c r="G356" t="s">
+        <v>2</v>
+      </c>
+      <c r="H356" t="s">
+        <v>2</v>
+      </c>
+      <c r="I356" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J356" t="s">
+        <v>2</v>
+      </c>
+      <c r="K356" t="s">
+        <v>274</v>
+      </c>
+      <c r="L356" t="s">
+        <v>487</v>
+      </c>
+      <c r="M356" t="s">
+        <v>2</v>
+      </c>
+      <c r="N356" t="s">
+        <v>2</v>
+      </c>
+      <c r="O356" t="s">
+        <v>2</v>
+      </c>
+      <c r="P356" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>0</v>
       </c>
@@ -13715,17 +13927,17 @@
       <c r="D357" t="s">
         <v>2</v>
       </c>
-      <c r="E357" s="1" t="s">
+      <c r="E357" t="s">
         <v>2</v>
       </c>
       <c r="F357" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G357" t="s">
         <v>2</v>
       </c>
       <c r="H357" t="s">
-        <v>2</v>
+        <v>462</v>
       </c>
       <c r="I357" s="2" t="s">
         <v>2</v>
@@ -13734,7 +13946,7 @@
         <v>2</v>
       </c>
       <c r="K357" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L357" t="s">
         <v>487</v>
@@ -13769,13 +13981,13 @@
         <v>2</v>
       </c>
       <c r="F358" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G358" t="s">
         <v>2</v>
       </c>
       <c r="H358" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I358" s="2" t="s">
         <v>2</v>
@@ -13803,59 +14015,59 @@
       </c>
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A359" t="s">
-        <v>0</v>
-      </c>
-      <c r="B359" s="3" t="s">
+      <c r="P359" s="3"/>
+    </row>
+    <row r="360" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A360" t="s">
+        <v>0</v>
+      </c>
+      <c r="B360" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C360" t="s">
         <v>100</v>
       </c>
-      <c r="D359" t="s">
-        <v>2</v>
-      </c>
-      <c r="E359" t="s">
-        <v>2</v>
-      </c>
-      <c r="F359" t="s">
-        <v>194</v>
-      </c>
-      <c r="G359" t="s">
-        <v>2</v>
-      </c>
-      <c r="H359" t="s">
-        <v>463</v>
-      </c>
-      <c r="I359" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J359" t="s">
-        <v>2</v>
-      </c>
-      <c r="K359" t="s">
-        <v>192</v>
-      </c>
-      <c r="L359" t="s">
-        <v>487</v>
-      </c>
-      <c r="M359" t="s">
-        <v>2</v>
-      </c>
-      <c r="N359" t="s">
-        <v>2</v>
-      </c>
-      <c r="O359" t="s">
-        <v>2</v>
-      </c>
-      <c r="P359" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="360" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P360" s="3"/>
-    </row>
-    <row r="361" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D360" t="s">
+        <v>2</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F360" t="s">
+        <v>2</v>
+      </c>
+      <c r="G360" t="s">
+        <v>2</v>
+      </c>
+      <c r="H360" t="s">
+        <v>2</v>
+      </c>
+      <c r="I360" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J360" t="s">
+        <v>2</v>
+      </c>
+      <c r="K360" t="s">
+        <v>274</v>
+      </c>
+      <c r="L360" t="s">
+        <v>488</v>
+      </c>
+      <c r="M360" t="s">
+        <v>2</v>
+      </c>
+      <c r="N360" t="s">
+        <v>2</v>
+      </c>
+      <c r="O360" t="s">
+        <v>2</v>
+      </c>
+      <c r="P360" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>0</v>
       </c>
@@ -13868,17 +14080,17 @@
       <c r="D361" t="s">
         <v>2</v>
       </c>
-      <c r="E361" s="1" t="s">
+      <c r="E361" t="s">
         <v>2</v>
       </c>
       <c r="F361" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G361" t="s">
         <v>2</v>
       </c>
       <c r="H361" t="s">
-        <v>2</v>
+        <v>464</v>
       </c>
       <c r="I361" s="2" t="s">
         <v>2</v>
@@ -13887,7 +14099,7 @@
         <v>2</v>
       </c>
       <c r="K361" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L361" t="s">
         <v>488</v>
@@ -13922,13 +14134,13 @@
         <v>2</v>
       </c>
       <c r="F362" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G362" t="s">
         <v>2</v>
       </c>
       <c r="H362" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I362" s="2" t="s">
         <v>2</v>
@@ -13956,60 +14168,60 @@
       </c>
     </row>
     <row r="363" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A363" t="s">
-        <v>0</v>
-      </c>
-      <c r="B363" s="3" t="s">
+      <c r="I363" s="2"/>
+      <c r="P363" s="3"/>
+    </row>
+    <row r="364" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A364" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C364" t="s">
         <v>100</v>
       </c>
-      <c r="D363" t="s">
-        <v>2</v>
-      </c>
-      <c r="E363" t="s">
-        <v>2</v>
-      </c>
-      <c r="F363" t="s">
-        <v>194</v>
-      </c>
-      <c r="G363" t="s">
-        <v>2</v>
-      </c>
-      <c r="H363" t="s">
-        <v>465</v>
-      </c>
-      <c r="I363" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J363" t="s">
-        <v>2</v>
-      </c>
-      <c r="K363" t="s">
-        <v>192</v>
-      </c>
-      <c r="L363" t="s">
-        <v>488</v>
-      </c>
-      <c r="M363" t="s">
-        <v>2</v>
-      </c>
-      <c r="N363" t="s">
-        <v>2</v>
-      </c>
-      <c r="O363" t="s">
-        <v>2</v>
-      </c>
-      <c r="P363" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="364" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I364" s="2"/>
-      <c r="P364" s="3"/>
-    </row>
-    <row r="365" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D364" t="s">
+        <v>2</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F364" t="s">
+        <v>2</v>
+      </c>
+      <c r="G364" t="s">
+        <v>2</v>
+      </c>
+      <c r="H364" t="s">
+        <v>2</v>
+      </c>
+      <c r="I364" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J364" t="s">
+        <v>2</v>
+      </c>
+      <c r="K364" t="s">
+        <v>274</v>
+      </c>
+      <c r="L364" t="s">
+        <v>489</v>
+      </c>
+      <c r="M364" t="s">
+        <v>2</v>
+      </c>
+      <c r="N364" t="s">
+        <v>2</v>
+      </c>
+      <c r="O364" t="s">
+        <v>2</v>
+      </c>
+      <c r="P364" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>0</v>
       </c>
@@ -14022,17 +14234,17 @@
       <c r="D365" t="s">
         <v>2</v>
       </c>
-      <c r="E365" s="1" t="s">
+      <c r="E365" t="s">
         <v>2</v>
       </c>
       <c r="F365" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G365" t="s">
         <v>2</v>
       </c>
       <c r="H365" t="s">
-        <v>2</v>
+        <v>466</v>
       </c>
       <c r="I365" s="2" t="s">
         <v>2</v>
@@ -14041,7 +14253,7 @@
         <v>2</v>
       </c>
       <c r="K365" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L365" t="s">
         <v>489</v>
@@ -14076,13 +14288,13 @@
         <v>2</v>
       </c>
       <c r="F366" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G366" t="s">
         <v>2</v>
       </c>
       <c r="H366" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I366" s="2" t="s">
         <v>2</v>
@@ -14110,60 +14322,60 @@
       </c>
     </row>
     <row r="367" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A367" t="s">
-        <v>0</v>
-      </c>
-      <c r="B367" s="3" t="s">
+      <c r="I367" s="2"/>
+      <c r="P367" s="3"/>
+    </row>
+    <row r="368" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A368" t="s">
+        <v>0</v>
+      </c>
+      <c r="B368" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C368" t="s">
         <v>100</v>
       </c>
-      <c r="D367" t="s">
-        <v>2</v>
-      </c>
-      <c r="E367" t="s">
-        <v>2</v>
-      </c>
-      <c r="F367" t="s">
-        <v>194</v>
-      </c>
-      <c r="G367" t="s">
-        <v>2</v>
-      </c>
-      <c r="H367" t="s">
-        <v>467</v>
-      </c>
-      <c r="I367" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J367" t="s">
-        <v>2</v>
-      </c>
-      <c r="K367" t="s">
-        <v>192</v>
-      </c>
-      <c r="L367" t="s">
-        <v>489</v>
-      </c>
-      <c r="M367" t="s">
-        <v>2</v>
-      </c>
-      <c r="N367" t="s">
-        <v>2</v>
-      </c>
-      <c r="O367" t="s">
-        <v>2</v>
-      </c>
-      <c r="P367" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I368" s="2"/>
-      <c r="P368" s="3"/>
-    </row>
-    <row r="369" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D368" t="s">
+        <v>2</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F368" t="s">
+        <v>2</v>
+      </c>
+      <c r="G368" t="s">
+        <v>2</v>
+      </c>
+      <c r="H368" t="s">
+        <v>2</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J368" t="s">
+        <v>2</v>
+      </c>
+      <c r="K368" t="s">
+        <v>274</v>
+      </c>
+      <c r="L368" t="s">
+        <v>490</v>
+      </c>
+      <c r="M368" t="s">
+        <v>2</v>
+      </c>
+      <c r="N368" t="s">
+        <v>2</v>
+      </c>
+      <c r="O368" t="s">
+        <v>2</v>
+      </c>
+      <c r="P368" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>0</v>
       </c>
@@ -14176,17 +14388,17 @@
       <c r="D369" t="s">
         <v>2</v>
       </c>
-      <c r="E369" s="1" t="s">
+      <c r="E369" t="s">
         <v>2</v>
       </c>
       <c r="F369" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G369" t="s">
         <v>2</v>
       </c>
       <c r="H369" t="s">
-        <v>2</v>
+        <v>468</v>
       </c>
       <c r="I369" s="2" t="s">
         <v>2</v>
@@ -14195,7 +14407,7 @@
         <v>2</v>
       </c>
       <c r="K369" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L369" t="s">
         <v>490</v>
@@ -14230,13 +14442,13 @@
         <v>2</v>
       </c>
       <c r="F370" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G370" t="s">
         <v>2</v>
       </c>
       <c r="H370" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I370" s="2" t="s">
         <v>2</v>
@@ -14264,61 +14476,61 @@
       </c>
     </row>
     <row r="371" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A371" t="s">
-        <v>0</v>
-      </c>
-      <c r="B371" s="3" t="s">
+      <c r="E371" s="1"/>
+      <c r="I371" s="2"/>
+      <c r="P371" s="3"/>
+    </row>
+    <row r="372" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A372" t="s">
+        <v>0</v>
+      </c>
+      <c r="B372" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C372" t="s">
         <v>100</v>
       </c>
-      <c r="D371" t="s">
-        <v>2</v>
-      </c>
-      <c r="E371" t="s">
-        <v>2</v>
-      </c>
-      <c r="F371" t="s">
-        <v>194</v>
-      </c>
-      <c r="G371" t="s">
-        <v>2</v>
-      </c>
-      <c r="H371" t="s">
-        <v>469</v>
-      </c>
-      <c r="I371" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J371" t="s">
-        <v>2</v>
-      </c>
-      <c r="K371" t="s">
-        <v>192</v>
-      </c>
-      <c r="L371" t="s">
-        <v>490</v>
-      </c>
-      <c r="M371" t="s">
-        <v>2</v>
-      </c>
-      <c r="N371" t="s">
-        <v>2</v>
-      </c>
-      <c r="O371" t="s">
-        <v>2</v>
-      </c>
-      <c r="P371" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="372" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E372" s="1"/>
-      <c r="I372" s="2"/>
-      <c r="P372" s="3"/>
-    </row>
-    <row r="373" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D372" t="s">
+        <v>2</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F372" t="s">
+        <v>2</v>
+      </c>
+      <c r="G372" t="s">
+        <v>2</v>
+      </c>
+      <c r="H372" t="s">
+        <v>2</v>
+      </c>
+      <c r="I372" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J372" t="s">
+        <v>2</v>
+      </c>
+      <c r="K372" t="s">
+        <v>274</v>
+      </c>
+      <c r="L372" t="s">
+        <v>491</v>
+      </c>
+      <c r="M372" t="s">
+        <v>2</v>
+      </c>
+      <c r="N372" t="s">
+        <v>2</v>
+      </c>
+      <c r="O372" t="s">
+        <v>2</v>
+      </c>
+      <c r="P372" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="373" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>0</v>
       </c>
@@ -14331,17 +14543,17 @@
       <c r="D373" t="s">
         <v>2</v>
       </c>
-      <c r="E373" s="1" t="s">
+      <c r="E373" t="s">
         <v>2</v>
       </c>
       <c r="F373" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G373" t="s">
         <v>2</v>
       </c>
       <c r="H373" t="s">
-        <v>2</v>
+        <v>470</v>
       </c>
       <c r="I373" s="2" t="s">
         <v>2</v>
@@ -14350,7 +14562,7 @@
         <v>2</v>
       </c>
       <c r="K373" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L373" t="s">
         <v>491</v>
@@ -14385,13 +14597,13 @@
         <v>2</v>
       </c>
       <c r="F374" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G374" t="s">
         <v>2</v>
       </c>
       <c r="H374" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I374" s="2" t="s">
         <v>2</v>
@@ -14418,57 +14630,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A375" t="s">
-        <v>0</v>
-      </c>
-      <c r="B375" s="3" t="s">
+    <row r="376" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>0</v>
+      </c>
+      <c r="B376" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C376" t="s">
         <v>100</v>
       </c>
-      <c r="D375" t="s">
-        <v>2</v>
-      </c>
-      <c r="E375" t="s">
-        <v>2</v>
-      </c>
-      <c r="F375" t="s">
-        <v>194</v>
-      </c>
-      <c r="G375" t="s">
-        <v>2</v>
-      </c>
-      <c r="H375" t="s">
-        <v>471</v>
-      </c>
-      <c r="I375" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J375" t="s">
-        <v>2</v>
-      </c>
-      <c r="K375" t="s">
-        <v>192</v>
-      </c>
-      <c r="L375" t="s">
-        <v>491</v>
-      </c>
-      <c r="M375" t="s">
-        <v>2</v>
-      </c>
-      <c r="N375" t="s">
-        <v>2</v>
-      </c>
-      <c r="O375" t="s">
-        <v>2</v>
-      </c>
-      <c r="P375" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="377" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
+        <v>2</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F376" t="s">
+        <v>2</v>
+      </c>
+      <c r="G376" t="s">
+        <v>2</v>
+      </c>
+      <c r="H376" t="s">
+        <v>2</v>
+      </c>
+      <c r="I376" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J376" t="s">
+        <v>2</v>
+      </c>
+      <c r="K376" t="s">
+        <v>274</v>
+      </c>
+      <c r="L376" t="s">
+        <v>492</v>
+      </c>
+      <c r="M376" t="s">
+        <v>2</v>
+      </c>
+      <c r="N376" t="s">
+        <v>2</v>
+      </c>
+      <c r="O376" t="s">
+        <v>2</v>
+      </c>
+      <c r="P376" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="377" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>0</v>
       </c>
@@ -14481,17 +14693,17 @@
       <c r="D377" t="s">
         <v>2</v>
       </c>
-      <c r="E377" s="1" t="s">
+      <c r="E377" t="s">
         <v>2</v>
       </c>
       <c r="F377" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G377" t="s">
         <v>2</v>
       </c>
       <c r="H377" t="s">
-        <v>2</v>
+        <v>472</v>
       </c>
       <c r="I377" s="2" t="s">
         <v>2</v>
@@ -14500,7 +14712,7 @@
         <v>2</v>
       </c>
       <c r="K377" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L377" t="s">
         <v>492</v>
@@ -14535,13 +14747,13 @@
         <v>2</v>
       </c>
       <c r="F378" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G378" t="s">
         <v>2</v>
       </c>
       <c r="H378" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="I378" s="2" t="s">
         <v>2</v>
@@ -14568,57 +14780,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="379" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A379" t="s">
-        <v>0</v>
-      </c>
-      <c r="B379" s="3" t="s">
+    <row r="380" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>0</v>
+      </c>
+      <c r="B380" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C379" t="s">
+      <c r="C380" t="s">
         <v>100</v>
       </c>
-      <c r="D379" t="s">
-        <v>2</v>
-      </c>
-      <c r="E379" t="s">
-        <v>2</v>
-      </c>
-      <c r="F379" t="s">
-        <v>194</v>
-      </c>
-      <c r="G379" t="s">
-        <v>2</v>
-      </c>
-      <c r="H379" t="s">
-        <v>473</v>
-      </c>
-      <c r="I379" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J379" t="s">
-        <v>2</v>
-      </c>
-      <c r="K379" t="s">
-        <v>192</v>
-      </c>
-      <c r="L379" t="s">
-        <v>492</v>
-      </c>
-      <c r="M379" t="s">
-        <v>2</v>
-      </c>
-      <c r="N379" t="s">
-        <v>2</v>
-      </c>
-      <c r="O379" t="s">
-        <v>2</v>
-      </c>
-      <c r="P379" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="381" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D380" t="s">
+        <v>2</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F380" t="s">
+        <v>2</v>
+      </c>
+      <c r="G380" t="s">
+        <v>2</v>
+      </c>
+      <c r="H380" t="s">
+        <v>2</v>
+      </c>
+      <c r="I380" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J380" t="s">
+        <v>2</v>
+      </c>
+      <c r="K380" t="s">
+        <v>274</v>
+      </c>
+      <c r="L380" t="s">
+        <v>493</v>
+      </c>
+      <c r="M380" t="s">
+        <v>2</v>
+      </c>
+      <c r="N380" t="s">
+        <v>2</v>
+      </c>
+      <c r="O380" t="s">
+        <v>2</v>
+      </c>
+      <c r="P380" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="381" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>0</v>
       </c>
@@ -14631,17 +14843,17 @@
       <c r="D381" t="s">
         <v>2</v>
       </c>
-      <c r="E381" s="1" t="s">
+      <c r="E381" t="s">
         <v>2</v>
       </c>
       <c r="F381" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G381" t="s">
         <v>2</v>
       </c>
       <c r="H381" t="s">
-        <v>2</v>
+        <v>474</v>
       </c>
       <c r="I381" s="2" t="s">
         <v>2</v>
@@ -14650,7 +14862,7 @@
         <v>2</v>
       </c>
       <c r="K381" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L381" t="s">
         <v>493</v>
@@ -14685,13 +14897,13 @@
         <v>2</v>
       </c>
       <c r="F382" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G382" t="s">
         <v>2</v>
       </c>
       <c r="H382" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I382" s="2" t="s">
         <v>2</v>
@@ -14719,59 +14931,59 @@
       </c>
     </row>
     <row r="383" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A383" t="s">
-        <v>0</v>
-      </c>
-      <c r="B383" s="3" t="s">
+      <c r="P383" s="3"/>
+    </row>
+    <row r="384" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
+        <v>0</v>
+      </c>
+      <c r="B384" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C383" t="s">
+      <c r="C384" t="s">
         <v>100</v>
       </c>
-      <c r="D383" t="s">
-        <v>2</v>
-      </c>
-      <c r="E383" t="s">
-        <v>2</v>
-      </c>
-      <c r="F383" t="s">
-        <v>194</v>
-      </c>
-      <c r="G383" t="s">
-        <v>2</v>
-      </c>
-      <c r="H383" t="s">
-        <v>475</v>
-      </c>
-      <c r="I383" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J383" t="s">
-        <v>2</v>
-      </c>
-      <c r="K383" t="s">
-        <v>192</v>
-      </c>
-      <c r="L383" t="s">
-        <v>493</v>
-      </c>
-      <c r="M383" t="s">
-        <v>2</v>
-      </c>
-      <c r="N383" t="s">
-        <v>2</v>
-      </c>
-      <c r="O383" t="s">
-        <v>2</v>
-      </c>
-      <c r="P383" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="384" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P384" s="3"/>
-    </row>
-    <row r="385" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D384" t="s">
+        <v>2</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F384" t="s">
+        <v>2</v>
+      </c>
+      <c r="G384" t="s">
+        <v>2</v>
+      </c>
+      <c r="H384" t="s">
+        <v>2</v>
+      </c>
+      <c r="I384" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J384" t="s">
+        <v>2</v>
+      </c>
+      <c r="K384" t="s">
+        <v>274</v>
+      </c>
+      <c r="L384" t="s">
+        <v>494</v>
+      </c>
+      <c r="M384" t="s">
+        <v>2</v>
+      </c>
+      <c r="N384" t="s">
+        <v>2</v>
+      </c>
+      <c r="O384" t="s">
+        <v>2</v>
+      </c>
+      <c r="P384" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>0</v>
       </c>
@@ -14784,17 +14996,17 @@
       <c r="D385" t="s">
         <v>2</v>
       </c>
-      <c r="E385" s="1" t="s">
+      <c r="E385" t="s">
         <v>2</v>
       </c>
       <c r="F385" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G385" t="s">
         <v>2</v>
       </c>
       <c r="H385" t="s">
-        <v>2</v>
+        <v>476</v>
       </c>
       <c r="I385" s="2" t="s">
         <v>2</v>
@@ -14803,7 +15015,7 @@
         <v>2</v>
       </c>
       <c r="K385" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L385" t="s">
         <v>494</v>
@@ -14838,13 +15050,13 @@
         <v>2</v>
       </c>
       <c r="F386" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G386" t="s">
         <v>2</v>
       </c>
       <c r="H386" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="I386" s="2" t="s">
         <v>2</v>
@@ -14872,59 +15084,59 @@
       </c>
     </row>
     <row r="387" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A387" t="s">
-        <v>0</v>
-      </c>
-      <c r="B387" s="3" t="s">
+      <c r="P387" s="3"/>
+    </row>
+    <row r="388" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>0</v>
+      </c>
+      <c r="B388" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C387" t="s">
+      <c r="C388" t="s">
         <v>100</v>
       </c>
-      <c r="D387" t="s">
-        <v>2</v>
-      </c>
-      <c r="E387" t="s">
-        <v>2</v>
-      </c>
-      <c r="F387" t="s">
-        <v>194</v>
-      </c>
-      <c r="G387" t="s">
-        <v>2</v>
-      </c>
-      <c r="H387" t="s">
-        <v>477</v>
-      </c>
-      <c r="I387" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J387" t="s">
-        <v>2</v>
-      </c>
-      <c r="K387" t="s">
-        <v>192</v>
-      </c>
-      <c r="L387" t="s">
-        <v>494</v>
-      </c>
-      <c r="M387" t="s">
-        <v>2</v>
-      </c>
-      <c r="N387" t="s">
-        <v>2</v>
-      </c>
-      <c r="O387" t="s">
-        <v>2</v>
-      </c>
-      <c r="P387" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P388" s="3"/>
-    </row>
-    <row r="389" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D388" t="s">
+        <v>2</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F388" t="s">
+        <v>2</v>
+      </c>
+      <c r="G388" t="s">
+        <v>2</v>
+      </c>
+      <c r="H388" t="s">
+        <v>2</v>
+      </c>
+      <c r="I388" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J388" t="s">
+        <v>2</v>
+      </c>
+      <c r="K388" t="s">
+        <v>274</v>
+      </c>
+      <c r="L388" t="s">
+        <v>495</v>
+      </c>
+      <c r="M388" t="s">
+        <v>2</v>
+      </c>
+      <c r="N388" t="s">
+        <v>2</v>
+      </c>
+      <c r="O388" t="s">
+        <v>2</v>
+      </c>
+      <c r="P388" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>0</v>
       </c>
@@ -14937,17 +15149,17 @@
       <c r="D389" t="s">
         <v>2</v>
       </c>
-      <c r="E389" s="1" t="s">
+      <c r="E389" t="s">
         <v>2</v>
       </c>
       <c r="F389" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G389" t="s">
         <v>2</v>
       </c>
       <c r="H389" t="s">
-        <v>2</v>
+        <v>478</v>
       </c>
       <c r="I389" s="2" t="s">
         <v>2</v>
@@ -14956,7 +15168,7 @@
         <v>2</v>
       </c>
       <c r="K389" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L389" t="s">
         <v>495</v>
@@ -14991,13 +15203,13 @@
         <v>2</v>
       </c>
       <c r="F390" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G390" t="s">
         <v>2</v>
       </c>
       <c r="H390" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I390" s="2" t="s">
         <v>2</v>
@@ -15025,57 +15237,57 @@
       </c>
     </row>
     <row r="391" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A391" t="s">
-        <v>0</v>
-      </c>
-      <c r="B391" s="3" t="s">
+      <c r="P391" s="3"/>
+    </row>
+    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>0</v>
+      </c>
+      <c r="B392" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C391" t="s">
+      <c r="C392" t="s">
         <v>100</v>
       </c>
-      <c r="D391" t="s">
-        <v>2</v>
-      </c>
-      <c r="E391" t="s">
-        <v>2</v>
-      </c>
-      <c r="F391" t="s">
-        <v>194</v>
-      </c>
-      <c r="G391" t="s">
-        <v>2</v>
-      </c>
-      <c r="H391" t="s">
-        <v>479</v>
-      </c>
-      <c r="I391" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J391" t="s">
-        <v>2</v>
-      </c>
-      <c r="K391" t="s">
-        <v>192</v>
-      </c>
-      <c r="L391" t="s">
-        <v>495</v>
-      </c>
-      <c r="M391" t="s">
-        <v>2</v>
-      </c>
-      <c r="N391" t="s">
-        <v>2</v>
-      </c>
-      <c r="O391" t="s">
-        <v>2</v>
-      </c>
-      <c r="P391" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P392" s="3"/>
+      <c r="D392" t="s">
+        <v>2</v>
+      </c>
+      <c r="E392" t="s">
+        <v>2</v>
+      </c>
+      <c r="F392" t="s">
+        <v>2</v>
+      </c>
+      <c r="G392" t="s">
+        <v>2</v>
+      </c>
+      <c r="H392" t="s">
+        <v>2</v>
+      </c>
+      <c r="I392" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J392" t="s">
+        <v>2</v>
+      </c>
+      <c r="K392" t="s">
+        <v>274</v>
+      </c>
+      <c r="L392" t="s">
+        <v>496</v>
+      </c>
+      <c r="M392" t="s">
+        <v>2</v>
+      </c>
+      <c r="N392" t="s">
+        <v>2</v>
+      </c>
+      <c r="O392" t="s">
+        <v>2</v>
+      </c>
+      <c r="P392" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="393" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
@@ -15094,22 +15306,22 @@
         <v>2</v>
       </c>
       <c r="F393" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G393" t="s">
         <v>2</v>
       </c>
       <c r="H393" t="s">
-        <v>2</v>
-      </c>
-      <c r="I393" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I393" t="s">
         <v>2</v>
       </c>
       <c r="J393" t="s">
         <v>2</v>
       </c>
       <c r="K393" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L393" t="s">
         <v>496</v>
@@ -15123,7 +15335,7 @@
       <c r="O393" t="s">
         <v>2</v>
       </c>
-      <c r="P393" s="3" t="s">
+      <c r="P393" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15144,13 +15356,13 @@
         <v>2</v>
       </c>
       <c r="F394" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G394" t="s">
         <v>2</v>
       </c>
       <c r="H394" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="I394" t="s">
         <v>2</v>
@@ -15177,53 +15389,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A395" t="s">
-        <v>0</v>
-      </c>
-      <c r="B395" s="3" t="s">
+    <row r="396" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
+        <v>0</v>
+      </c>
+      <c r="B396" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C395" t="s">
+      <c r="C396" t="s">
         <v>100</v>
       </c>
-      <c r="D395" t="s">
-        <v>2</v>
-      </c>
-      <c r="E395" t="s">
-        <v>2</v>
-      </c>
-      <c r="F395" t="s">
-        <v>194</v>
-      </c>
-      <c r="G395" t="s">
-        <v>2</v>
-      </c>
-      <c r="H395" t="s">
-        <v>481</v>
-      </c>
-      <c r="I395" t="s">
-        <v>2</v>
-      </c>
-      <c r="J395" t="s">
-        <v>2</v>
-      </c>
-      <c r="K395" t="s">
-        <v>192</v>
-      </c>
-      <c r="L395" t="s">
-        <v>496</v>
-      </c>
-      <c r="M395" t="s">
-        <v>2</v>
-      </c>
-      <c r="N395" t="s">
-        <v>2</v>
-      </c>
-      <c r="O395" t="s">
-        <v>2</v>
-      </c>
-      <c r="P395" t="s">
+      <c r="D396" t="s">
+        <v>2</v>
+      </c>
+      <c r="E396" t="s">
+        <v>2</v>
+      </c>
+      <c r="F396" t="s">
+        <v>2</v>
+      </c>
+      <c r="G396" t="s">
+        <v>2</v>
+      </c>
+      <c r="H396" t="s">
+        <v>2</v>
+      </c>
+      <c r="I396" t="s">
+        <v>2</v>
+      </c>
+      <c r="J396" t="s">
+        <v>2</v>
+      </c>
+      <c r="K396" t="s">
+        <v>274</v>
+      </c>
+      <c r="L396" t="s">
+        <v>497</v>
+      </c>
+      <c r="M396" t="s">
+        <v>2</v>
+      </c>
+      <c r="N396" t="s">
+        <v>2</v>
+      </c>
+      <c r="O396" t="s">
+        <v>2</v>
+      </c>
+      <c r="P396" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15244,13 +15456,13 @@
         <v>2</v>
       </c>
       <c r="F397" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="G397" t="s">
         <v>2</v>
       </c>
       <c r="H397" t="s">
-        <v>2</v>
+        <v>482</v>
       </c>
       <c r="I397" t="s">
         <v>2</v>
@@ -15259,7 +15471,7 @@
         <v>2</v>
       </c>
       <c r="K397" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="L397" t="s">
         <v>497</v>
@@ -15294,13 +15506,13 @@
         <v>2</v>
       </c>
       <c r="F398" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G398" t="s">
         <v>2</v>
       </c>
       <c r="H398" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="I398" t="s">
         <v>2</v>
@@ -15327,53 +15539,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A399" t="s">
-        <v>0</v>
-      </c>
-      <c r="B399" s="3" t="s">
+    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>0</v>
+      </c>
+      <c r="B400" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="C399" t="s">
+      <c r="C400" t="s">
         <v>100</v>
       </c>
-      <c r="D399" t="s">
-        <v>2</v>
-      </c>
-      <c r="E399" t="s">
-        <v>2</v>
-      </c>
-      <c r="F399" t="s">
-        <v>194</v>
-      </c>
-      <c r="G399" t="s">
-        <v>2</v>
-      </c>
-      <c r="H399" t="s">
-        <v>483</v>
-      </c>
-      <c r="I399" t="s">
-        <v>2</v>
-      </c>
-      <c r="J399" t="s">
-        <v>2</v>
-      </c>
-      <c r="K399" t="s">
-        <v>192</v>
-      </c>
-      <c r="L399" t="s">
-        <v>497</v>
-      </c>
-      <c r="M399" t="s">
-        <v>2</v>
-      </c>
-      <c r="N399" t="s">
-        <v>2</v>
-      </c>
-      <c r="O399" t="s">
-        <v>2</v>
-      </c>
-      <c r="P399" t="s">
+      <c r="D400" t="s">
+        <v>2</v>
+      </c>
+      <c r="E400" t="s">
+        <v>2</v>
+      </c>
+      <c r="F400" t="s">
+        <v>2</v>
+      </c>
+      <c r="G400" t="s">
+        <v>2</v>
+      </c>
+      <c r="H400" t="s">
+        <v>2</v>
+      </c>
+      <c r="I400" t="s">
+        <v>2</v>
+      </c>
+      <c r="J400" t="s">
+        <v>2</v>
+      </c>
+      <c r="K400" t="s">
+        <v>274</v>
+      </c>
+      <c r="L400" t="s">
+        <v>498</v>
+      </c>
+      <c r="M400" t="s">
+        <v>2</v>
+      </c>
+      <c r="N400" t="s">
+        <v>2</v>
+      </c>
+      <c r="O400" t="s">
+        <v>2</v>
+      </c>
+      <c r="P400" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15427,58 +15639,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="402" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A402" t="s">
-        <v>0</v>
-      </c>
-      <c r="B402" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="C402" t="s">
-        <v>100</v>
-      </c>
-      <c r="D402" t="s">
-        <v>2</v>
-      </c>
-      <c r="E402" t="s">
-        <v>2</v>
-      </c>
-      <c r="F402" t="s">
-        <v>2</v>
-      </c>
-      <c r="G402" t="s">
-        <v>2</v>
-      </c>
-      <c r="H402" t="s">
-        <v>2</v>
-      </c>
-      <c r="I402" t="s">
-        <v>2</v>
-      </c>
-      <c r="J402" t="s">
-        <v>2</v>
-      </c>
-      <c r="K402" t="s">
-        <v>274</v>
-      </c>
-      <c r="L402" t="s">
-        <v>498</v>
-      </c>
-      <c r="M402" t="s">
-        <v>2</v>
-      </c>
-      <c r="N402" t="s">
-        <v>2</v>
-      </c>
-      <c r="O402" t="s">
-        <v>2</v>
-      </c>
-      <c r="P402" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="439" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A439" t="s">
+        <v>0</v>
+      </c>
+      <c r="B439" t="s">
+        <v>11</v>
+      </c>
+      <c r="C439" t="s">
+        <v>101</v>
+      </c>
+      <c r="D439" t="s">
+        <v>2</v>
+      </c>
+      <c r="E439" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F439" t="s">
+        <v>19</v>
+      </c>
+      <c r="G439" t="s">
+        <v>2</v>
+      </c>
+      <c r="H439" t="s">
+        <v>103</v>
+      </c>
+      <c r="I439" t="s">
+        <v>2</v>
+      </c>
+      <c r="J439" t="s">
+        <v>2</v>
+      </c>
+      <c r="K439" t="s">
+        <v>11</v>
+      </c>
+      <c r="L439" t="s">
+        <v>2</v>
+      </c>
+      <c r="M439" t="s">
+        <v>2</v>
+      </c>
+      <c r="N439" t="s">
+        <v>2</v>
+      </c>
+      <c r="O439" t="s">
+        <v>2</v>
+      </c>
+      <c r="P439" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>0</v>
       </c>
@@ -15486,22 +15698,22 @@
         <v>11</v>
       </c>
       <c r="C440" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D440" t="s">
         <v>2</v>
       </c>
-      <c r="E440" s="1" t="s">
-        <v>3</v>
+      <c r="E440" t="s">
+        <v>2</v>
       </c>
       <c r="F440" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G440" t="s">
         <v>2</v>
       </c>
       <c r="H440" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I440" t="s">
         <v>2</v>
@@ -15536,7 +15748,7 @@
         <v>11</v>
       </c>
       <c r="C441" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D441" t="s">
         <v>2</v>
@@ -15545,13 +15757,13 @@
         <v>2</v>
       </c>
       <c r="F441" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G441" t="s">
         <v>2</v>
       </c>
       <c r="H441" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="I441" t="s">
         <v>2</v>
@@ -15583,7 +15795,7 @@
         <v>0</v>
       </c>
       <c r="B442" t="s">
-        <v>11</v>
+        <v>208</v>
       </c>
       <c r="C442" t="s">
         <v>101</v>
@@ -15595,13 +15807,13 @@
         <v>2</v>
       </c>
       <c r="F442" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G442" t="s">
         <v>2</v>
       </c>
       <c r="H442" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="I442" t="s">
         <v>2</v>
@@ -15610,19 +15822,19 @@
         <v>2</v>
       </c>
       <c r="K442" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L442" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="M442" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="N442" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="O442" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="P442" t="s">
         <v>2</v>
@@ -15645,34 +15857,34 @@
         <v>2</v>
       </c>
       <c r="F443" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="G443" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="H443" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="I443" t="s">
-        <v>2</v>
-      </c>
-      <c r="J443" t="s">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="J443">
+        <v>1</v>
       </c>
       <c r="K443" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L443" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="M443" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="N443" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="O443" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="P443" t="s">
         <v>2</v>
@@ -15695,16 +15907,16 @@
         <v>2</v>
       </c>
       <c r="F444" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G444" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H444" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="I444" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="J444">
         <v>1</v>
@@ -15745,16 +15957,16 @@
         <v>2</v>
       </c>
       <c r="F445" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G445" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H445" t="s">
         <v>2</v>
       </c>
       <c r="I445" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J445">
         <v>1</v>
@@ -15795,16 +16007,16 @@
         <v>2</v>
       </c>
       <c r="F446" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G446" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H446" t="s">
         <v>2</v>
       </c>
       <c r="I446" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J446">
         <v>1</v>
@@ -15845,16 +16057,16 @@
         <v>2</v>
       </c>
       <c r="F447" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G447" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H447" t="s">
         <v>2</v>
       </c>
       <c r="I447" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J447">
         <v>1</v>
@@ -15895,16 +16107,16 @@
         <v>2</v>
       </c>
       <c r="F448" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G448" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H448" t="s">
         <v>2</v>
       </c>
       <c r="I448" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J448">
         <v>1</v>
@@ -15945,19 +16157,19 @@
         <v>2</v>
       </c>
       <c r="F449" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G449" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H449" t="s">
         <v>2</v>
       </c>
       <c r="I449" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J449">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K449" t="s">
         <v>15</v>
@@ -15995,19 +16207,19 @@
         <v>2</v>
       </c>
       <c r="F450" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G450" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H450" t="s">
         <v>2</v>
       </c>
       <c r="I450" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J450">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K450" t="s">
         <v>15</v>
@@ -16045,16 +16257,16 @@
         <v>2</v>
       </c>
       <c r="F451" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G451" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H451" t="s">
         <v>2</v>
       </c>
       <c r="I451" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J451">
         <v>1</v>
@@ -16095,16 +16307,16 @@
         <v>2</v>
       </c>
       <c r="F452" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G452" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H452" t="s">
         <v>2</v>
       </c>
       <c r="I452" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J452">
         <v>1</v>
@@ -16133,7 +16345,7 @@
         <v>0</v>
       </c>
       <c r="B453" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C453" t="s">
         <v>101</v>
@@ -16145,22 +16357,22 @@
         <v>2</v>
       </c>
       <c r="F453" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="G453" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="H453" t="s">
-        <v>2</v>
+        <v>248</v>
       </c>
       <c r="I453" t="s">
-        <v>139</v>
-      </c>
-      <c r="J453">
-        <v>1</v>
+        <v>247</v>
+      </c>
+      <c r="J453" t="s">
+        <v>2</v>
       </c>
       <c r="K453" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L453" t="s">
         <v>2</v>
@@ -16195,22 +16407,22 @@
         <v>2</v>
       </c>
       <c r="F454" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="G454" t="s">
         <v>2</v>
       </c>
       <c r="H454" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="I454" t="s">
-        <v>247</v>
-      </c>
-      <c r="J454" t="s">
-        <v>2</v>
+        <v>262</v>
+      </c>
+      <c r="J454">
+        <v>1</v>
       </c>
       <c r="K454" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L454" t="s">
         <v>2</v>
@@ -16251,13 +16463,13 @@
         <v>2</v>
       </c>
       <c r="H455" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="I455" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J455">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K455" t="s">
         <v>15</v>
@@ -16301,13 +16513,13 @@
         <v>2</v>
       </c>
       <c r="H456" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I456" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J456">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K456" t="s">
         <v>15</v>
@@ -16351,10 +16563,10 @@
         <v>2</v>
       </c>
       <c r="H457" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I457" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J457">
         <v>1</v>
@@ -16401,10 +16613,10 @@
         <v>2</v>
       </c>
       <c r="H458" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I458" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J458">
         <v>1</v>
@@ -16451,10 +16663,10 @@
         <v>2</v>
       </c>
       <c r="H459" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I459" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J459">
         <v>1</v>
@@ -16501,10 +16713,10 @@
         <v>2</v>
       </c>
       <c r="H460" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I460" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J460">
         <v>1</v>
@@ -16551,7 +16763,7 @@
         <v>2</v>
       </c>
       <c r="H461" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="I461" t="s">
         <v>268</v>
@@ -16601,13 +16813,13 @@
         <v>2</v>
       </c>
       <c r="H462" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="I462" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J462">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K462" t="s">
         <v>15</v>
@@ -16651,13 +16863,13 @@
         <v>2</v>
       </c>
       <c r="H463" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I463" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J463">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K463" t="s">
         <v>15</v>
@@ -16701,13 +16913,13 @@
         <v>2</v>
       </c>
       <c r="H464" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I464" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J464">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K464" t="s">
         <v>15</v>
@@ -16751,10 +16963,10 @@
         <v>2</v>
       </c>
       <c r="H465" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I465" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J465">
         <v>0</v>
@@ -16778,53 +16990,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="466" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A466" t="s">
-        <v>0</v>
-      </c>
-      <c r="B466" t="s">
-        <v>210</v>
-      </c>
-      <c r="C466" t="s">
+    <row r="467" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A467" t="s">
+        <v>0</v>
+      </c>
+      <c r="B467" t="s">
+        <v>273</v>
+      </c>
+      <c r="C467" t="s">
         <v>101</v>
       </c>
-      <c r="D466" t="s">
-        <v>2</v>
-      </c>
-      <c r="E466" t="s">
-        <v>2</v>
-      </c>
-      <c r="F466" t="s">
-        <v>249</v>
-      </c>
-      <c r="G466" t="s">
-        <v>2</v>
-      </c>
-      <c r="H466" t="s">
-        <v>259</v>
-      </c>
-      <c r="I466" t="s">
-        <v>272</v>
-      </c>
-      <c r="J466">
-        <v>0</v>
-      </c>
-      <c r="K466" t="s">
-        <v>15</v>
-      </c>
-      <c r="L466" t="s">
-        <v>2</v>
-      </c>
-      <c r="M466" t="s">
-        <v>2</v>
-      </c>
-      <c r="N466" t="s">
-        <v>2</v>
-      </c>
-      <c r="O466" t="s">
-        <v>2</v>
-      </c>
-      <c r="P466" t="s">
+      <c r="D467" t="s">
+        <v>2</v>
+      </c>
+      <c r="E467" t="s">
+        <v>2</v>
+      </c>
+      <c r="F467" t="s">
+        <v>2</v>
+      </c>
+      <c r="G467" t="s">
+        <v>2</v>
+      </c>
+      <c r="H467" t="s">
+        <v>2</v>
+      </c>
+      <c r="I467" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J467" t="s">
+        <v>2</v>
+      </c>
+      <c r="K467" t="s">
+        <v>274</v>
+      </c>
+      <c r="L467" t="s">
+        <v>499</v>
+      </c>
+      <c r="M467" t="s">
+        <v>2</v>
+      </c>
+      <c r="N467" t="s">
+        <v>2</v>
+      </c>
+      <c r="O467" t="s">
+        <v>2</v>
+      </c>
+      <c r="P467" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -16845,86 +17057,86 @@
         <v>2</v>
       </c>
       <c r="F468" t="s">
-        <v>2</v>
+        <v>237</v>
       </c>
       <c r="G468" t="s">
         <v>2</v>
       </c>
       <c r="H468" t="s">
-        <v>2</v>
-      </c>
-      <c r="I468" s="2" t="s">
-        <v>2</v>
+        <v>500</v>
+      </c>
+      <c r="I468" t="s">
+        <v>501</v>
       </c>
       <c r="J468" t="s">
         <v>2</v>
       </c>
       <c r="K468" t="s">
+        <v>10</v>
+      </c>
+      <c r="L468" t="s">
+        <v>502</v>
+      </c>
+      <c r="M468" t="s">
+        <v>2</v>
+      </c>
+      <c r="N468" t="s">
+        <v>2</v>
+      </c>
+      <c r="O468" t="s">
+        <v>2</v>
+      </c>
+      <c r="P468" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="470" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A470" t="s">
+        <v>0</v>
+      </c>
+      <c r="B470" t="s">
+        <v>273</v>
+      </c>
+      <c r="C470" t="s">
+        <v>101</v>
+      </c>
+      <c r="D470" t="s">
+        <v>2</v>
+      </c>
+      <c r="E470" t="s">
+        <v>2</v>
+      </c>
+      <c r="F470" t="s">
+        <v>2</v>
+      </c>
+      <c r="G470" t="s">
+        <v>2</v>
+      </c>
+      <c r="H470" t="s">
+        <v>2</v>
+      </c>
+      <c r="I470" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J470" t="s">
+        <v>2</v>
+      </c>
+      <c r="K470" t="s">
         <v>274</v>
       </c>
-      <c r="L468" t="s">
-        <v>499</v>
-      </c>
-      <c r="M468" t="s">
-        <v>2</v>
-      </c>
-      <c r="N468" t="s">
-        <v>2</v>
-      </c>
-      <c r="O468" t="s">
-        <v>2</v>
-      </c>
-      <c r="P468" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="469" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A469" t="s">
-        <v>0</v>
-      </c>
-      <c r="B469" t="s">
-        <v>273</v>
-      </c>
-      <c r="C469" t="s">
-        <v>101</v>
-      </c>
-      <c r="D469" t="s">
-        <v>2</v>
-      </c>
-      <c r="E469" t="s">
-        <v>2</v>
-      </c>
-      <c r="F469" t="s">
-        <v>237</v>
-      </c>
-      <c r="G469" t="s">
-        <v>2</v>
-      </c>
-      <c r="H469" t="s">
-        <v>500</v>
-      </c>
-      <c r="I469" t="s">
-        <v>501</v>
-      </c>
-      <c r="J469" t="s">
-        <v>2</v>
-      </c>
-      <c r="K469" t="s">
-        <v>10</v>
-      </c>
-      <c r="L469" t="s">
-        <v>502</v>
-      </c>
-      <c r="M469" t="s">
-        <v>2</v>
-      </c>
-      <c r="N469" t="s">
-        <v>2</v>
-      </c>
-      <c r="O469" t="s">
-        <v>2</v>
-      </c>
-      <c r="P469" s="3" t="s">
+      <c r="L470" t="s">
+        <v>503</v>
+      </c>
+      <c r="M470" t="s">
+        <v>2</v>
+      </c>
+      <c r="N470" t="s">
+        <v>2</v>
+      </c>
+      <c r="O470" t="s">
+        <v>2</v>
+      </c>
+      <c r="P470" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -16945,25 +17157,25 @@
         <v>2</v>
       </c>
       <c r="F471" t="s">
-        <v>2</v>
+        <v>505</v>
       </c>
       <c r="G471" t="s">
         <v>2</v>
       </c>
       <c r="H471" t="s">
-        <v>2</v>
-      </c>
-      <c r="I471" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J471" t="s">
-        <v>2</v>
+        <v>515</v>
+      </c>
+      <c r="I471" t="s">
+        <v>525</v>
+      </c>
+      <c r="J471">
+        <v>1</v>
       </c>
       <c r="K471" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L471" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="M471" t="s">
         <v>2</v>
@@ -16995,19 +17207,19 @@
         <v>2</v>
       </c>
       <c r="F472" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G472" t="s">
         <v>2</v>
       </c>
       <c r="H472" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I472" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="J472">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K472" t="s">
         <v>15</v>
@@ -17045,19 +17257,19 @@
         <v>2</v>
       </c>
       <c r="F473" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="G473" t="s">
         <v>2</v>
       </c>
       <c r="H473" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I473" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="J473">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K473" t="s">
         <v>15</v>
@@ -17095,19 +17307,19 @@
         <v>2</v>
       </c>
       <c r="F474" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="G474" t="s">
         <v>2</v>
       </c>
       <c r="H474" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="I474" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="J474">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K474" t="s">
         <v>15</v>
@@ -17145,19 +17357,19 @@
         <v>2</v>
       </c>
       <c r="F475" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="G475" t="s">
         <v>2</v>
       </c>
       <c r="H475" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="I475" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="J475">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K475" t="s">
         <v>15</v>
@@ -17195,19 +17407,19 @@
         <v>2</v>
       </c>
       <c r="F476" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G476" t="s">
         <v>2</v>
       </c>
       <c r="H476" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I476" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J476">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K476" t="s">
         <v>15</v>
@@ -17245,19 +17457,19 @@
         <v>2</v>
       </c>
       <c r="F477" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="G477" t="s">
         <v>2</v>
       </c>
       <c r="H477" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I477" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="J477">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K477" t="s">
         <v>15</v>
@@ -17295,19 +17507,19 @@
         <v>2</v>
       </c>
       <c r="F478" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G478" t="s">
         <v>2</v>
       </c>
       <c r="H478" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I478" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J478">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K478" t="s">
         <v>15</v>
@@ -17345,19 +17557,19 @@
         <v>2</v>
       </c>
       <c r="F479" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G479" t="s">
         <v>2</v>
       </c>
       <c r="H479" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I479" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="J479">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K479" t="s">
         <v>15</v>
@@ -17395,19 +17607,19 @@
         <v>2</v>
       </c>
       <c r="F480" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G480" t="s">
         <v>2</v>
       </c>
       <c r="H480" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="I480" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="J480">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K480" t="s">
         <v>15</v>
@@ -17445,25 +17657,25 @@
         <v>2</v>
       </c>
       <c r="F481" t="s">
-        <v>514</v>
+        <v>534</v>
       </c>
       <c r="G481" t="s">
         <v>2</v>
       </c>
       <c r="H481" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="I481" t="s">
-        <v>533</v>
-      </c>
-      <c r="J481">
-        <v>1</v>
+        <v>536</v>
+      </c>
+      <c r="J481" t="s">
+        <v>2</v>
       </c>
       <c r="K481" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L481" t="s">
-        <v>504</v>
+        <v>537</v>
       </c>
       <c r="M481" t="s">
         <v>2</v>
@@ -17474,57 +17686,57 @@
       <c r="O481" t="s">
         <v>2</v>
       </c>
-      <c r="P481" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="482" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A482" t="s">
-        <v>0</v>
-      </c>
-      <c r="B482" t="s">
+      <c r="P481" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="483" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A483" t="s">
+        <v>0</v>
+      </c>
+      <c r="B483" t="s">
         <v>273</v>
       </c>
-      <c r="C482" t="s">
+      <c r="C483" t="s">
         <v>101</v>
       </c>
-      <c r="D482" t="s">
-        <v>2</v>
-      </c>
-      <c r="E482" t="s">
-        <v>2</v>
-      </c>
-      <c r="F482" t="s">
-        <v>534</v>
-      </c>
-      <c r="G482" t="s">
-        <v>2</v>
-      </c>
-      <c r="H482" t="s">
-        <v>535</v>
-      </c>
-      <c r="I482" t="s">
-        <v>536</v>
-      </c>
-      <c r="J482" t="s">
-        <v>2</v>
-      </c>
-      <c r="K482" t="s">
-        <v>10</v>
-      </c>
-      <c r="L482" t="s">
-        <v>537</v>
-      </c>
-      <c r="M482" t="s">
-        <v>2</v>
-      </c>
-      <c r="N482" t="s">
-        <v>2</v>
-      </c>
-      <c r="O482" t="s">
-        <v>2</v>
-      </c>
-      <c r="P482" t="s">
+      <c r="D483" t="s">
+        <v>2</v>
+      </c>
+      <c r="E483" t="s">
+        <v>2</v>
+      </c>
+      <c r="F483" t="s">
+        <v>2</v>
+      </c>
+      <c r="G483" t="s">
+        <v>2</v>
+      </c>
+      <c r="H483" t="s">
+        <v>2</v>
+      </c>
+      <c r="I483" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J483" t="s">
+        <v>2</v>
+      </c>
+      <c r="K483" t="s">
+        <v>274</v>
+      </c>
+      <c r="L483" t="s">
+        <v>538</v>
+      </c>
+      <c r="M483" t="s">
+        <v>2</v>
+      </c>
+      <c r="N483" t="s">
+        <v>2</v>
+      </c>
+      <c r="O483" t="s">
+        <v>2</v>
+      </c>
+      <c r="P483" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -17551,19 +17763,19 @@
         <v>2</v>
       </c>
       <c r="H484" t="s">
-        <v>2</v>
-      </c>
-      <c r="I484" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J484" t="s">
-        <v>2</v>
+        <v>539</v>
+      </c>
+      <c r="I484" t="s">
+        <v>545</v>
+      </c>
+      <c r="J484">
+        <v>0</v>
       </c>
       <c r="K484" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L484" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="M484" t="s">
         <v>2</v>
@@ -17601,13 +17813,13 @@
         <v>2</v>
       </c>
       <c r="H485" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I485" t="s">
         <v>545</v>
       </c>
       <c r="J485">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K485" t="s">
         <v>15</v>
@@ -17628,53 +17840,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="486" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A486" t="s">
-        <v>0</v>
-      </c>
-      <c r="B486" t="s">
+    <row r="487" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>0</v>
+      </c>
+      <c r="B487" t="s">
         <v>273</v>
       </c>
-      <c r="C486" t="s">
+      <c r="C487" t="s">
         <v>101</v>
       </c>
-      <c r="D486" t="s">
-        <v>2</v>
-      </c>
-      <c r="E486" t="s">
-        <v>2</v>
-      </c>
-      <c r="F486" t="s">
-        <v>2</v>
-      </c>
-      <c r="G486" t="s">
-        <v>2</v>
-      </c>
-      <c r="H486" t="s">
-        <v>540</v>
-      </c>
-      <c r="I486" t="s">
-        <v>545</v>
-      </c>
-      <c r="J486">
-        <v>1</v>
-      </c>
-      <c r="K486" t="s">
-        <v>15</v>
-      </c>
-      <c r="L486" t="s">
-        <v>541</v>
-      </c>
-      <c r="M486" t="s">
-        <v>2</v>
-      </c>
-      <c r="N486" t="s">
-        <v>2</v>
-      </c>
-      <c r="O486" t="s">
-        <v>2</v>
-      </c>
-      <c r="P486" s="3" t="s">
+      <c r="D487" t="s">
+        <v>2</v>
+      </c>
+      <c r="E487" t="s">
+        <v>2</v>
+      </c>
+      <c r="F487" t="s">
+        <v>2</v>
+      </c>
+      <c r="G487" t="s">
+        <v>2</v>
+      </c>
+      <c r="H487" t="s">
+        <v>2</v>
+      </c>
+      <c r="I487" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J487" t="s">
+        <v>2</v>
+      </c>
+      <c r="K487" t="s">
+        <v>274</v>
+      </c>
+      <c r="L487" t="s">
+        <v>542</v>
+      </c>
+      <c r="M487" t="s">
+        <v>2</v>
+      </c>
+      <c r="N487" t="s">
+        <v>2</v>
+      </c>
+      <c r="O487" t="s">
+        <v>2</v>
+      </c>
+      <c r="P487" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -17701,19 +17913,19 @@
         <v>2</v>
       </c>
       <c r="H488" t="s">
-        <v>2</v>
-      </c>
-      <c r="I488" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J488" t="s">
-        <v>2</v>
+        <v>543</v>
+      </c>
+      <c r="I488" t="s">
+        <v>548</v>
+      </c>
+      <c r="J488">
+        <v>1</v>
       </c>
       <c r="K488" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L488" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="M488" t="s">
         <v>2</v>
@@ -17751,10 +17963,10 @@
         <v>2</v>
       </c>
       <c r="H489" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I489" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J489">
         <v>1</v>
@@ -17778,53 +17990,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="490" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A490" t="s">
-        <v>0</v>
-      </c>
-      <c r="B490" t="s">
+    <row r="491" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>0</v>
+      </c>
+      <c r="B491" t="s">
         <v>273</v>
       </c>
-      <c r="C490" t="s">
+      <c r="C491" t="s">
         <v>101</v>
       </c>
-      <c r="D490" t="s">
-        <v>2</v>
-      </c>
-      <c r="E490" t="s">
-        <v>2</v>
-      </c>
-      <c r="F490" t="s">
-        <v>2</v>
-      </c>
-      <c r="G490" t="s">
-        <v>2</v>
-      </c>
-      <c r="H490" t="s">
-        <v>544</v>
-      </c>
-      <c r="I490" t="s">
-        <v>546</v>
-      </c>
-      <c r="J490">
-        <v>1</v>
-      </c>
-      <c r="K490" t="s">
-        <v>15</v>
-      </c>
-      <c r="L490" t="s">
-        <v>547</v>
-      </c>
-      <c r="M490" t="s">
-        <v>2</v>
-      </c>
-      <c r="N490" t="s">
-        <v>2</v>
-      </c>
-      <c r="O490" t="s">
-        <v>2</v>
-      </c>
-      <c r="P490" s="3" t="s">
+      <c r="D491" t="s">
+        <v>2</v>
+      </c>
+      <c r="E491" t="s">
+        <v>2</v>
+      </c>
+      <c r="F491" t="s">
+        <v>2</v>
+      </c>
+      <c r="G491" t="s">
+        <v>2</v>
+      </c>
+      <c r="H491" t="s">
+        <v>2</v>
+      </c>
+      <c r="I491" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J491" t="s">
+        <v>2</v>
+      </c>
+      <c r="K491" t="s">
+        <v>274</v>
+      </c>
+      <c r="L491" t="s">
+        <v>556</v>
+      </c>
+      <c r="M491" t="s">
+        <v>2</v>
+      </c>
+      <c r="N491" t="s">
+        <v>2</v>
+      </c>
+      <c r="O491" t="s">
+        <v>2</v>
+      </c>
+      <c r="P491" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -17845,25 +18057,25 @@
         <v>2</v>
       </c>
       <c r="F492" t="s">
-        <v>2</v>
+        <v>549</v>
       </c>
       <c r="G492" t="s">
         <v>2</v>
       </c>
       <c r="H492" t="s">
-        <v>2</v>
-      </c>
-      <c r="I492" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J492" t="s">
-        <v>2</v>
+        <v>553</v>
+      </c>
+      <c r="I492" t="s">
+        <v>550</v>
+      </c>
+      <c r="J492">
+        <v>1</v>
       </c>
       <c r="K492" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L492" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M492" t="s">
         <v>2</v>
@@ -17895,19 +18107,19 @@
         <v>2</v>
       </c>
       <c r="F493" t="s">
-        <v>549</v>
+        <v>2</v>
       </c>
       <c r="G493" t="s">
         <v>2</v>
       </c>
       <c r="H493" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I493" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="J493">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K493" t="s">
         <v>15</v>
@@ -17951,13 +18163,13 @@
         <v>2</v>
       </c>
       <c r="H494" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I494" t="s">
         <v>554</v>
       </c>
       <c r="J494">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K494" t="s">
         <v>15</v>
@@ -17978,53 +18190,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="495" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A495" t="s">
-        <v>0</v>
-      </c>
-      <c r="B495" t="s">
+    <row r="496" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>0</v>
+      </c>
+      <c r="B496" t="s">
         <v>273</v>
       </c>
-      <c r="C495" t="s">
+      <c r="C496" t="s">
         <v>101</v>
       </c>
-      <c r="D495" t="s">
-        <v>2</v>
-      </c>
-      <c r="E495" t="s">
-        <v>2</v>
-      </c>
-      <c r="F495" t="s">
-        <v>2</v>
-      </c>
-      <c r="G495" t="s">
-        <v>2</v>
-      </c>
-      <c r="H495" t="s">
-        <v>552</v>
-      </c>
-      <c r="I495" t="s">
-        <v>554</v>
-      </c>
-      <c r="J495">
-        <v>2</v>
-      </c>
-      <c r="K495" t="s">
-        <v>15</v>
-      </c>
-      <c r="L495" t="s">
-        <v>555</v>
-      </c>
-      <c r="M495" t="s">
-        <v>2</v>
-      </c>
-      <c r="N495" t="s">
-        <v>2</v>
-      </c>
-      <c r="O495" t="s">
-        <v>2</v>
-      </c>
-      <c r="P495" s="3" t="s">
+      <c r="D496" t="s">
+        <v>2</v>
+      </c>
+      <c r="E496" t="s">
+        <v>2</v>
+      </c>
+      <c r="F496" t="s">
+        <v>2</v>
+      </c>
+      <c r="G496" t="s">
+        <v>2</v>
+      </c>
+      <c r="H496" t="s">
+        <v>2</v>
+      </c>
+      <c r="I496" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J496" t="s">
+        <v>2</v>
+      </c>
+      <c r="K496" t="s">
+        <v>274</v>
+      </c>
+      <c r="L496" t="s">
+        <v>563</v>
+      </c>
+      <c r="M496" t="s">
+        <v>2</v>
+      </c>
+      <c r="N496" t="s">
+        <v>2</v>
+      </c>
+      <c r="O496" t="s">
+        <v>2</v>
+      </c>
+      <c r="P496" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -18045,25 +18257,25 @@
         <v>2</v>
       </c>
       <c r="F497" t="s">
-        <v>2</v>
+        <v>557</v>
       </c>
       <c r="G497" t="s">
         <v>2</v>
       </c>
       <c r="H497" t="s">
-        <v>2</v>
-      </c>
-      <c r="I497" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J497" t="s">
-        <v>2</v>
+        <v>559</v>
+      </c>
+      <c r="I497" t="s">
+        <v>561</v>
+      </c>
+      <c r="J497">
+        <v>1</v>
       </c>
       <c r="K497" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L497" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="M497" t="s">
         <v>2</v>
@@ -18095,19 +18307,19 @@
         <v>2</v>
       </c>
       <c r="F498" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="G498" t="s">
         <v>2</v>
       </c>
       <c r="H498" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="I498" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="J498">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K498" t="s">
         <v>15</v>
@@ -18129,57 +18341,57 @@
       </c>
     </row>
     <row r="499" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A499" t="s">
-        <v>0</v>
-      </c>
-      <c r="B499" t="s">
+      <c r="P499" s="3"/>
+    </row>
+    <row r="500" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>0</v>
+      </c>
+      <c r="B500" t="s">
         <v>273</v>
       </c>
-      <c r="C499" t="s">
+      <c r="C500" t="s">
         <v>101</v>
       </c>
-      <c r="D499" t="s">
-        <v>2</v>
-      </c>
-      <c r="E499" t="s">
-        <v>2</v>
-      </c>
-      <c r="F499" t="s">
-        <v>558</v>
-      </c>
-      <c r="G499" t="s">
-        <v>2</v>
-      </c>
-      <c r="H499" t="s">
-        <v>560</v>
-      </c>
-      <c r="I499" t="s">
-        <v>562</v>
-      </c>
-      <c r="J499">
-        <v>0</v>
-      </c>
-      <c r="K499" t="s">
-        <v>15</v>
-      </c>
-      <c r="L499" t="s">
-        <v>564</v>
-      </c>
-      <c r="M499" t="s">
-        <v>2</v>
-      </c>
-      <c r="N499" t="s">
-        <v>2</v>
-      </c>
-      <c r="O499" t="s">
-        <v>2</v>
-      </c>
-      <c r="P499" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="500" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P500" s="3"/>
+      <c r="D500" t="s">
+        <v>2</v>
+      </c>
+      <c r="E500" t="s">
+        <v>2</v>
+      </c>
+      <c r="F500" t="s">
+        <v>2</v>
+      </c>
+      <c r="G500" t="s">
+        <v>2</v>
+      </c>
+      <c r="H500" t="s">
+        <v>2</v>
+      </c>
+      <c r="I500" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J500" t="s">
+        <v>2</v>
+      </c>
+      <c r="K500" t="s">
+        <v>274</v>
+      </c>
+      <c r="L500" t="s">
+        <v>568</v>
+      </c>
+      <c r="M500" t="s">
+        <v>2</v>
+      </c>
+      <c r="N500" t="s">
+        <v>2</v>
+      </c>
+      <c r="O500" t="s">
+        <v>2</v>
+      </c>
+      <c r="P500" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="501" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
@@ -18204,19 +18416,19 @@
         <v>2</v>
       </c>
       <c r="H501" t="s">
-        <v>2</v>
-      </c>
-      <c r="I501" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J501" t="s">
-        <v>2</v>
+        <v>565</v>
+      </c>
+      <c r="I501" t="s">
+        <v>567</v>
+      </c>
+      <c r="J501">
+        <v>0</v>
       </c>
       <c r="K501" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L501" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M501" t="s">
         <v>2</v>
@@ -18254,13 +18466,13 @@
         <v>2</v>
       </c>
       <c r="H502" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="I502" t="s">
         <v>567</v>
       </c>
       <c r="J502">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K502" t="s">
         <v>15</v>
@@ -18281,53 +18493,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="503" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A503" t="s">
-        <v>0</v>
-      </c>
-      <c r="B503" t="s">
+    <row r="504" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>0</v>
+      </c>
+      <c r="B504" t="s">
         <v>273</v>
       </c>
-      <c r="C503" t="s">
+      <c r="C504" t="s">
         <v>101</v>
       </c>
-      <c r="D503" t="s">
-        <v>2</v>
-      </c>
-      <c r="E503" t="s">
-        <v>2</v>
-      </c>
-      <c r="F503" t="s">
-        <v>2</v>
-      </c>
-      <c r="G503" t="s">
-        <v>2</v>
-      </c>
-      <c r="H503" t="s">
-        <v>566</v>
-      </c>
-      <c r="I503" t="s">
-        <v>567</v>
-      </c>
-      <c r="J503">
-        <v>1</v>
-      </c>
-      <c r="K503" t="s">
-        <v>15</v>
-      </c>
-      <c r="L503" t="s">
-        <v>569</v>
-      </c>
-      <c r="M503" t="s">
-        <v>2</v>
-      </c>
-      <c r="N503" t="s">
-        <v>2</v>
-      </c>
-      <c r="O503" t="s">
-        <v>2</v>
-      </c>
-      <c r="P503" s="3" t="s">
+      <c r="D504" t="s">
+        <v>2</v>
+      </c>
+      <c r="E504" t="s">
+        <v>2</v>
+      </c>
+      <c r="F504" t="s">
+        <v>2</v>
+      </c>
+      <c r="G504" t="s">
+        <v>2</v>
+      </c>
+      <c r="H504" t="s">
+        <v>2</v>
+      </c>
+      <c r="I504" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J504" t="s">
+        <v>2</v>
+      </c>
+      <c r="K504" t="s">
+        <v>274</v>
+      </c>
+      <c r="L504" t="s">
+        <v>574</v>
+      </c>
+      <c r="M504" t="s">
+        <v>2</v>
+      </c>
+      <c r="N504" t="s">
+        <v>2</v>
+      </c>
+      <c r="O504" t="s">
+        <v>2</v>
+      </c>
+      <c r="P504" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -18354,19 +18566,19 @@
         <v>2</v>
       </c>
       <c r="H505" t="s">
-        <v>2</v>
-      </c>
-      <c r="I505" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J505" t="s">
-        <v>2</v>
+        <v>570</v>
+      </c>
+      <c r="I505" t="s">
+        <v>572</v>
+      </c>
+      <c r="J505">
+        <v>0</v>
       </c>
       <c r="K505" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="L505" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="M505" t="s">
         <v>2</v>
@@ -18404,10 +18616,10 @@
         <v>2</v>
       </c>
       <c r="H506" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I506" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="J506">
         <v>0</v>
@@ -18428,56 +18640,6 @@
         <v>2</v>
       </c>
       <c r="P506" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="507" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A507" t="s">
-        <v>0</v>
-      </c>
-      <c r="B507" t="s">
-        <v>273</v>
-      </c>
-      <c r="C507" t="s">
-        <v>101</v>
-      </c>
-      <c r="D507" t="s">
-        <v>2</v>
-      </c>
-      <c r="E507" t="s">
-        <v>2</v>
-      </c>
-      <c r="F507" t="s">
-        <v>2</v>
-      </c>
-      <c r="G507" t="s">
-        <v>2</v>
-      </c>
-      <c r="H507" t="s">
-        <v>571</v>
-      </c>
-      <c r="I507" t="s">
-        <v>573</v>
-      </c>
-      <c r="J507">
-        <v>0</v>
-      </c>
-      <c r="K507" t="s">
-        <v>15</v>
-      </c>
-      <c r="L507" t="s">
-        <v>575</v>
-      </c>
-      <c r="M507" t="s">
-        <v>2</v>
-      </c>
-      <c r="N507" t="s">
-        <v>2</v>
-      </c>
-      <c r="O507" t="s">
-        <v>2</v>
-      </c>
-      <c r="P507" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Add initial exam section screens and logic
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71E4745-F52F-F549-B47E-E3483E9A646B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8D0723-2258-F446-BFC0-7C11194AEC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19300" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -1579,9 +1579,6 @@
   </si>
   <si>
     <t xml:space="preserve"> اسبوع  =  ______; مدرسة = ______ ;ذكية = ______</t>
-  </si>
-  <si>
-    <t>With whom did Ali share his story? ______ ; They all agreed that learning English is ______ ;Where did Ali run? ______​; "غداء" ;______ "ام"______</t>
   </si>
   <si>
     <t>She is ______ happy0هي سعيدة جدا ; She is waiting for you ______0هي تنتظرك هنا; She ______ eats eggs0هي لا تأكل بيض ابدا;I will ______ love you0انا سأحبك دائما</t>
@@ -1886,6 +1883,9 @@
   </si>
   <si>
     <t>Write the following in your notebook.</t>
+  </si>
+  <si>
+    <t>With whom did Ali share his story? ______; They all agreed that learning English is ______; Where did Ali run? ______; غداء ______; ام ______</t>
   </si>
 </sst>
 </file>
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:P506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H112" sqref="H112"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2919,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I16" t="s">
         <v>78</v>
@@ -4096,7 +4096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -4118,8 +4118,8 @@
       <c r="G40" t="s">
         <v>1</v>
       </c>
-      <c r="H40" t="s">
-        <v>513</v>
+      <c r="H40" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="I40" t="s">
         <v>156</v>
@@ -4269,7 +4269,7 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>239</v>
@@ -4319,7 +4319,7 @@
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>240</v>
@@ -4369,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>241</v>
@@ -4469,7 +4469,7 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>243</v>
@@ -4622,7 +4622,7 @@
         <v>246</v>
       </c>
       <c r="H51" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>247</v>
@@ -4672,7 +4672,7 @@
         <v>246</v>
       </c>
       <c r="H52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>248</v>
@@ -4722,7 +4722,7 @@
         <v>246</v>
       </c>
       <c r="H53" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>249</v>
@@ -4772,7 +4772,7 @@
         <v>246</v>
       </c>
       <c r="H54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>250</v>
@@ -4822,7 +4822,7 @@
         <v>246</v>
       </c>
       <c r="H55" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>251</v>
@@ -4922,7 +4922,7 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>256</v>
@@ -4972,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>252</v>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>253</v>
@@ -5072,7 +5072,7 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>254</v>
@@ -5122,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>255</v>
@@ -5287,7 +5287,7 @@
         <v>140</v>
       </c>
       <c r="H70" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I70" t="s">
         <v>263</v>
@@ -5391,7 +5391,7 @@
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>265</v>
@@ -5441,7 +5441,7 @@
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>266</v>
@@ -5491,7 +5491,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>146</v>
@@ -5541,7 +5541,7 @@
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>266</v>
@@ -5644,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>268</v>
@@ -5694,7 +5694,7 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>269</v>
@@ -5744,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>149</v>
@@ -5794,7 +5794,7 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>152</v>
@@ -5844,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>270</v>
@@ -5909,7 +5909,7 @@
         <v>235</v>
       </c>
       <c r="L85" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="M85" t="s">
         <v>1</v>
@@ -6239,7 +6239,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G105" t="s">
         <v>1</v>
@@ -6996,7 +6996,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G122" t="s">
         <v>1</v>
@@ -7146,7 +7146,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G126" t="s">
         <v>1</v>
@@ -7296,7 +7296,7 @@
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G130" t="s">
         <v>1</v>
@@ -7446,7 +7446,7 @@
         <v>1</v>
       </c>
       <c r="F134" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G134" t="s">
         <v>1</v>
@@ -7599,7 +7599,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G138" t="s">
         <v>1</v>
@@ -7753,7 +7753,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G142" t="s">
         <v>1</v>
@@ -7907,7 +7907,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G146" t="s">
         <v>1</v>
@@ -8062,7 +8062,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G150" t="s">
         <v>1</v>
@@ -8212,7 +8212,7 @@
         <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G154" t="s">
         <v>1</v>
@@ -8362,7 +8362,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G158" t="s">
         <v>1</v>
@@ -8515,7 +8515,7 @@
         <v>1</v>
       </c>
       <c r="F162" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G162" t="s">
         <v>1</v>
@@ -8668,7 +8668,7 @@
         <v>1</v>
       </c>
       <c r="F166" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G166" t="s">
         <v>1</v>
@@ -9782,7 +9782,7 @@
         <v>1</v>
       </c>
       <c r="H227" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I227" t="s">
         <v>191</v>
@@ -9832,7 +9832,7 @@
         <v>1</v>
       </c>
       <c r="H228" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I228" t="s">
         <v>191</v>
@@ -9882,7 +9882,7 @@
         <v>1</v>
       </c>
       <c r="H229" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I229" t="s">
         <v>191</v>
@@ -9932,7 +9932,7 @@
         <v>1</v>
       </c>
       <c r="H230" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I230" t="s">
         <v>191</v>
@@ -9982,7 +9982,7 @@
         <v>1</v>
       </c>
       <c r="H231" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I231" t="s">
         <v>191</v>
@@ -10032,7 +10032,7 @@
         <v>1</v>
       </c>
       <c r="H232" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I232" t="s">
         <v>191</v>
@@ -10082,7 +10082,7 @@
         <v>1</v>
       </c>
       <c r="H233" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I233" t="s">
         <v>191</v>
@@ -10132,7 +10132,7 @@
         <v>1</v>
       </c>
       <c r="H234" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I234" t="s">
         <v>191</v>
@@ -10532,7 +10532,7 @@
         <v>1</v>
       </c>
       <c r="H242" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I242" t="s">
         <v>201</v>
@@ -10582,7 +10582,7 @@
         <v>1</v>
       </c>
       <c r="H243" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I243" t="s">
         <v>201</v>
@@ -10632,7 +10632,7 @@
         <v>1</v>
       </c>
       <c r="H244" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I244" t="s">
         <v>201</v>
@@ -10682,7 +10682,7 @@
         <v>1</v>
       </c>
       <c r="H245" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I245" t="s">
         <v>201</v>
@@ -10732,7 +10732,7 @@
         <v>1</v>
       </c>
       <c r="H246" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I246" t="s">
         <v>201</v>
@@ -10782,7 +10782,7 @@
         <v>1</v>
       </c>
       <c r="H247" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I247" t="s">
         <v>203</v>
@@ -10932,7 +10932,7 @@
         <v>1</v>
       </c>
       <c r="H251" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I251" t="s">
         <v>320</v>
@@ -10982,7 +10982,7 @@
         <v>1</v>
       </c>
       <c r="H252" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I252" t="s">
         <v>321</v>
@@ -11032,7 +11032,7 @@
         <v>1</v>
       </c>
       <c r="H253" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I253" t="s">
         <v>322</v>
@@ -11082,7 +11082,7 @@
         <v>1</v>
       </c>
       <c r="H254" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I254" t="s">
         <v>323</v>
@@ -11132,7 +11132,7 @@
         <v>1</v>
       </c>
       <c r="H255" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I255" t="s">
         <v>324</v>
@@ -11182,7 +11182,7 @@
         <v>1</v>
       </c>
       <c r="H256" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I256" t="s">
         <v>320</v>
@@ -11232,7 +11232,7 @@
         <v>1</v>
       </c>
       <c r="H257" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I257" t="s">
         <v>321</v>
@@ -11282,7 +11282,7 @@
         <v>1</v>
       </c>
       <c r="H258" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I258" t="s">
         <v>325</v>
@@ -11332,7 +11332,7 @@
         <v>1</v>
       </c>
       <c r="H259" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I259" t="s">
         <v>326</v>
@@ -11382,7 +11382,7 @@
         <v>1</v>
       </c>
       <c r="H260" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I260" t="s">
         <v>327</v>
@@ -11532,7 +11532,7 @@
         <v>1</v>
       </c>
       <c r="H265" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I265" t="s">
         <v>332</v>
@@ -11582,7 +11582,7 @@
         <v>1</v>
       </c>
       <c r="H266" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I266" t="s">
         <v>327</v>
@@ -11632,7 +11632,7 @@
         <v>1</v>
       </c>
       <c r="H267" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I267" t="s">
         <v>329</v>
@@ -11682,7 +11682,7 @@
         <v>1</v>
       </c>
       <c r="H268" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I268" t="s">
         <v>330</v>
@@ -11732,7 +11732,7 @@
         <v>1</v>
       </c>
       <c r="H269" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I269" t="s">
         <v>331</v>
@@ -11782,7 +11782,7 @@
         <v>1</v>
       </c>
       <c r="H270" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I270" t="s">
         <v>327</v>
@@ -11832,7 +11832,7 @@
         <v>1</v>
       </c>
       <c r="H271" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I271" t="s">
         <v>332</v>
@@ -11882,7 +11882,7 @@
         <v>1</v>
       </c>
       <c r="H272" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I272" t="s">
         <v>334</v>
@@ -11932,7 +11932,7 @@
         <v>1</v>
       </c>
       <c r="H273" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I273" t="s">
         <v>333</v>
@@ -11982,7 +11982,7 @@
         <v>1</v>
       </c>
       <c r="H274" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I274" t="s">
         <v>335</v>
@@ -12082,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="H277" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I277" t="s">
         <v>338</v>
@@ -12132,7 +12132,7 @@
         <v>1</v>
       </c>
       <c r="H278" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I278" t="s">
         <v>339</v>
@@ -12182,7 +12182,7 @@
         <v>1</v>
       </c>
       <c r="H279" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I279" t="s">
         <v>340</v>
@@ -12232,7 +12232,7 @@
         <v>1</v>
       </c>
       <c r="H280" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I280" t="s">
         <v>341</v>
@@ -12282,7 +12282,7 @@
         <v>1</v>
       </c>
       <c r="H281" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I281" t="s">
         <v>342</v>
@@ -12332,7 +12332,7 @@
         <v>1</v>
       </c>
       <c r="H282" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I282" t="s">
         <v>343</v>
@@ -12382,7 +12382,7 @@
         <v>1</v>
       </c>
       <c r="H283" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I283" t="s">
         <v>341</v>
@@ -12432,7 +12432,7 @@
         <v>1</v>
       </c>
       <c r="H284" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I284" t="s">
         <v>344</v>
@@ -12482,7 +12482,7 @@
         <v>1</v>
       </c>
       <c r="H285" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I285" t="s">
         <v>345</v>
@@ -12532,7 +12532,7 @@
         <v>1</v>
       </c>
       <c r="H286" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I286" t="s">
         <v>340</v>
@@ -12632,7 +12632,7 @@
         <v>1</v>
       </c>
       <c r="H289" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I289" t="s">
         <v>348</v>
@@ -12682,7 +12682,7 @@
         <v>1</v>
       </c>
       <c r="H290" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I290" t="s">
         <v>350</v>
@@ -12732,7 +12732,7 @@
         <v>1</v>
       </c>
       <c r="H291" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I291" t="s">
         <v>351</v>
@@ -12782,7 +12782,7 @@
         <v>1</v>
       </c>
       <c r="H292" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I292" t="s">
         <v>352</v>
@@ -12832,7 +12832,7 @@
         <v>1</v>
       </c>
       <c r="H293" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I293" t="s">
         <v>353</v>
@@ -12882,7 +12882,7 @@
         <v>1</v>
       </c>
       <c r="H294" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I294" t="s">
         <v>354</v>
@@ -12932,7 +12932,7 @@
         <v>1</v>
       </c>
       <c r="H295" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I295" t="s">
         <v>355</v>
@@ -12982,7 +12982,7 @@
         <v>1</v>
       </c>
       <c r="H296" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I296" t="s">
         <v>349</v>
@@ -13032,7 +13032,7 @@
         <v>1</v>
       </c>
       <c r="H297" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I297" t="s">
         <v>356</v>
@@ -13776,7 +13776,7 @@
         <v>1</v>
       </c>
       <c r="F346" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G346" t="s">
         <v>1</v>
@@ -13926,7 +13926,7 @@
         <v>1</v>
       </c>
       <c r="F350" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G350" t="s">
         <v>1</v>
@@ -14076,7 +14076,7 @@
         <v>1</v>
       </c>
       <c r="F354" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G354" t="s">
         <v>1</v>
@@ -14226,7 +14226,7 @@
         <v>1</v>
       </c>
       <c r="F358" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G358" t="s">
         <v>1</v>
@@ -14379,7 +14379,7 @@
         <v>1</v>
       </c>
       <c r="F362" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G362" t="s">
         <v>1</v>
@@ -14533,7 +14533,7 @@
         <v>1</v>
       </c>
       <c r="F366" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G366" t="s">
         <v>1</v>
@@ -14687,7 +14687,7 @@
         <v>1</v>
       </c>
       <c r="F370" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G370" t="s">
         <v>1</v>
@@ -14842,7 +14842,7 @@
         <v>1</v>
       </c>
       <c r="F374" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G374" t="s">
         <v>1</v>
@@ -14992,7 +14992,7 @@
         <v>1</v>
       </c>
       <c r="F378" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G378" t="s">
         <v>1</v>
@@ -15142,7 +15142,7 @@
         <v>1</v>
       </c>
       <c r="F382" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G382" t="s">
         <v>1</v>
@@ -15295,7 +15295,7 @@
         <v>1</v>
       </c>
       <c r="F386" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G386" t="s">
         <v>1</v>
@@ -15448,7 +15448,7 @@
         <v>1</v>
       </c>
       <c r="F390" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G390" t="s">
         <v>1</v>
@@ -15601,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="F394" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G394" t="s">
         <v>1</v>
@@ -15751,7 +15751,7 @@
         <v>1</v>
       </c>
       <c r="F398" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G398" t="s">
         <v>1</v>
@@ -16608,7 +16608,7 @@
         <v>1</v>
       </c>
       <c r="H453" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I453" t="s">
         <v>211</v>
@@ -17008,7 +17008,7 @@
         <v>1</v>
       </c>
       <c r="H461" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I461" t="s">
         <v>229</v>
@@ -17158,7 +17158,7 @@
         <v>1</v>
       </c>
       <c r="H464" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I464" t="s">
         <v>232</v>
@@ -17308,7 +17308,7 @@
         <v>1</v>
       </c>
       <c r="H468" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I468" t="s">
         <v>401</v>
@@ -17908,7 +17908,7 @@
         <v>1</v>
       </c>
       <c r="H481" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I481" t="s">
         <v>435</v>
@@ -18358,7 +18358,7 @@
         <v>1</v>
       </c>
       <c r="H493" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I493" t="s">
         <v>451</v>
@@ -18408,7 +18408,7 @@
         <v>1</v>
       </c>
       <c r="H494" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I494" t="s">
         <v>451</v>

</xml_diff>

<commit_message>
fix: change wrong image name
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561DE011-EE66-5B40-AF8F-B81236AA58B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACD16E-A413-7D49-9066-41A488455397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -2474,7 +2474,7 @@
   <dimension ref="A4:Q508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H102" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3751,7 +3751,7 @@
         <v>1</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Q27" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
refactor section unit day logic to assign individual days to each unit rather than a sequential pattern across sections
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2959B6-210A-1F4E-B4BE-D0C556C9C25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0518AC35-A81B-554C-9F30-F822A0E1A91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -1549,9 +1549,6 @@
   </si>
   <si>
     <t>unit5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> unit5</t>
   </si>
   <si>
     <t xml:space="preserve"> اسبوع  =  ______; مدرسة = ______ ;ذكية = ______</t>
@@ -2063,6 +2060,9 @@
   </si>
   <si>
     <t>She is waiting for you ______ 0 هي تنتظرك {{aهنا}} ; I will ______ love you 0 انا سأحبك {{aدائما}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> unit3</t>
   </si>
 </sst>
 </file>
@@ -2473,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:Q508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3144,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I16" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J16" t="s">
         <v>1</v>
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>131</v>
@@ -3409,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>132</v>
@@ -3462,7 +3462,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>133</v>
@@ -3674,7 +3674,7 @@
         <v>138</v>
       </c>
       <c r="H26" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I26" t="s">
         <v>139</v>
@@ -4151,7 +4151,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I35" t="s">
         <v>161</v>
@@ -4204,7 +4204,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>164</v>
@@ -4416,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I40" t="s">
         <v>154</v>
@@ -4496,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -4549,7 +4549,7 @@
         <v>1</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -4575,7 +4575,7 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>236</v>
@@ -4628,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>237</v>
@@ -4681,7 +4681,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>238</v>
@@ -4787,7 +4787,7 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>240</v>
@@ -4923,7 +4923,7 @@
         <v>1</v>
       </c>
       <c r="Q50" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -4949,7 +4949,7 @@
         <v>243</v>
       </c>
       <c r="H51" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>244</v>
@@ -5002,7 +5002,7 @@
         <v>243</v>
       </c>
       <c r="H52" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>245</v>
@@ -5055,7 +5055,7 @@
         <v>243</v>
       </c>
       <c r="H53" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>246</v>
@@ -5108,7 +5108,7 @@
         <v>243</v>
       </c>
       <c r="H54" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>247</v>
@@ -5161,7 +5161,7 @@
         <v>243</v>
       </c>
       <c r="H55" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>248</v>
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
       <c r="Q57" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -5294,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="Q58" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="Q59" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -5373,7 +5373,7 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>253</v>
@@ -5426,7 +5426,7 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>249</v>
@@ -5479,7 +5479,7 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>250</v>
@@ -5532,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>251</v>
@@ -5585,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>252</v>
@@ -5668,7 +5668,7 @@
         <v>1</v>
       </c>
       <c r="Q66" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
@@ -5721,7 +5721,7 @@
         <v>1</v>
       </c>
       <c r="Q67" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -5774,7 +5774,7 @@
         <v>1</v>
       </c>
       <c r="Q68" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -5833,7 +5833,7 @@
         <v>1</v>
       </c>
       <c r="Q71" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -5859,7 +5859,7 @@
         <v>138</v>
       </c>
       <c r="H72" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I72" t="s">
         <v>257</v>
@@ -5943,7 +5943,7 @@
         <v>1</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -5969,7 +5969,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>259</v>
@@ -6022,7 +6022,7 @@
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>260</v>
@@ -6075,7 +6075,7 @@
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>144</v>
@@ -6128,7 +6128,7 @@
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>260</v>
@@ -6211,7 +6211,7 @@
         <v>1</v>
       </c>
       <c r="Q80" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -6237,7 +6237,7 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>262</v>
@@ -6290,7 +6290,7 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>263</v>
@@ -6343,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>147</v>
@@ -6396,7 +6396,7 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>150</v>
@@ -6449,7 +6449,7 @@
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>264</v>
@@ -6517,7 +6517,7 @@
         <v>232</v>
       </c>
       <c r="L87" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="M87" t="s">
         <v>1</v>
@@ -6532,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="Q87" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -6591,7 +6591,7 @@
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -6644,7 +6644,7 @@
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
@@ -6697,7 +6697,7 @@
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D104" t="s">
         <v>1</v>
@@ -6750,7 +6750,7 @@
         <v>497</v>
       </c>
       <c r="C105" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D105" t="s">
         <v>1</v>
@@ -6865,7 +6865,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G107" t="s">
         <v>1</v>
@@ -7284,7 +7284,7 @@
         <v>497</v>
       </c>
       <c r="C116" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D116" t="s">
         <v>1</v>
@@ -7326,7 +7326,7 @@
         <v>1</v>
       </c>
       <c r="Q116" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -7337,7 +7337,7 @@
         <v>497</v>
       </c>
       <c r="C117" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D117" t="s">
         <v>1</v>
@@ -7390,7 +7390,7 @@
         <v>497</v>
       </c>
       <c r="C118" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D118" t="s">
         <v>1</v>
@@ -7443,7 +7443,7 @@
         <v>497</v>
       </c>
       <c r="C119" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D119" t="s">
         <v>1</v>
@@ -7461,7 +7461,7 @@
         <v>268</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J119">
         <v>0</v>
@@ -7496,7 +7496,7 @@
         <v>497</v>
       </c>
       <c r="C120" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D120" t="s">
         <v>1</v>
@@ -7552,7 +7552,7 @@
         <v>497</v>
       </c>
       <c r="C122" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D122" t="s">
         <v>1</v>
@@ -7594,7 +7594,7 @@
         <v>1</v>
       </c>
       <c r="Q122" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
@@ -7605,7 +7605,7 @@
         <v>497</v>
       </c>
       <c r="C123" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D123" t="s">
         <v>1</v>
@@ -7658,7 +7658,7 @@
         <v>497</v>
       </c>
       <c r="C124" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D124" t="s">
         <v>1</v>
@@ -7667,7 +7667,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G124" t="s">
         <v>1</v>
@@ -7711,7 +7711,7 @@
         <v>497</v>
       </c>
       <c r="C126" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D126" t="s">
         <v>1</v>
@@ -7753,7 +7753,7 @@
         <v>1</v>
       </c>
       <c r="Q126" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
@@ -7764,7 +7764,7 @@
         <v>497</v>
       </c>
       <c r="C127" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D127" t="s">
         <v>1</v>
@@ -7817,7 +7817,7 @@
         <v>497</v>
       </c>
       <c r="C128" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D128" t="s">
         <v>1</v>
@@ -7826,7 +7826,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G128" t="s">
         <v>1</v>
@@ -7870,7 +7870,7 @@
         <v>497</v>
       </c>
       <c r="C130" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D130" t="s">
         <v>1</v>
@@ -7912,7 +7912,7 @@
         <v>1</v>
       </c>
       <c r="Q130" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
@@ -7923,7 +7923,7 @@
         <v>497</v>
       </c>
       <c r="C131" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D131" t="s">
         <v>1</v>
@@ -7976,7 +7976,7 @@
         <v>497</v>
       </c>
       <c r="C132" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D132" t="s">
         <v>1</v>
@@ -7985,7 +7985,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G132" t="s">
         <v>1</v>
@@ -8029,7 +8029,7 @@
         <v>497</v>
       </c>
       <c r="C134" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D134" t="s">
         <v>1</v>
@@ -8071,7 +8071,7 @@
         <v>1</v>
       </c>
       <c r="Q134" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
@@ -8082,7 +8082,7 @@
         <v>497</v>
       </c>
       <c r="C135" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D135" t="s">
         <v>1</v>
@@ -8135,7 +8135,7 @@
         <v>497</v>
       </c>
       <c r="C136" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D136" t="s">
         <v>1</v>
@@ -8144,7 +8144,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G136" t="s">
         <v>1</v>
@@ -8191,7 +8191,7 @@
         <v>497</v>
       </c>
       <c r="C138" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D138" t="s">
         <v>1</v>
@@ -8233,7 +8233,7 @@
         <v>1</v>
       </c>
       <c r="Q138" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
@@ -8244,7 +8244,7 @@
         <v>497</v>
       </c>
       <c r="C139" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D139" t="s">
         <v>1</v>
@@ -8297,7 +8297,7 @@
         <v>497</v>
       </c>
       <c r="C140" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D140" t="s">
         <v>1</v>
@@ -8306,7 +8306,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G140" t="s">
         <v>1</v>
@@ -8354,7 +8354,7 @@
         <v>497</v>
       </c>
       <c r="C142" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D142" t="s">
         <v>1</v>
@@ -8396,7 +8396,7 @@
         <v>1</v>
       </c>
       <c r="Q142" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
@@ -8407,7 +8407,7 @@
         <v>497</v>
       </c>
       <c r="C143" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D143" t="s">
         <v>1</v>
@@ -8460,7 +8460,7 @@
         <v>497</v>
       </c>
       <c r="C144" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D144" t="s">
         <v>1</v>
@@ -8469,7 +8469,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G144" t="s">
         <v>1</v>
@@ -8517,7 +8517,7 @@
         <v>497</v>
       </c>
       <c r="C146" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D146" t="s">
         <v>1</v>
@@ -8559,7 +8559,7 @@
         <v>1</v>
       </c>
       <c r="Q146" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -8570,7 +8570,7 @@
         <v>497</v>
       </c>
       <c r="C147" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D147" t="s">
         <v>1</v>
@@ -8623,7 +8623,7 @@
         <v>497</v>
       </c>
       <c r="C148" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D148" t="s">
         <v>1</v>
@@ -8632,7 +8632,7 @@
         <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G148" t="s">
         <v>1</v>
@@ -8681,7 +8681,7 @@
         <v>497</v>
       </c>
       <c r="C150" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D150" t="s">
         <v>1</v>
@@ -8723,7 +8723,7 @@
         <v>1</v>
       </c>
       <c r="Q150" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
@@ -8734,7 +8734,7 @@
         <v>497</v>
       </c>
       <c r="C151" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D151" t="s">
         <v>1</v>
@@ -8787,7 +8787,7 @@
         <v>497</v>
       </c>
       <c r="C152" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D152" t="s">
         <v>1</v>
@@ -8796,7 +8796,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G152" t="s">
         <v>1</v>
@@ -8840,7 +8840,7 @@
         <v>497</v>
       </c>
       <c r="C154" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D154" t="s">
         <v>1</v>
@@ -8882,7 +8882,7 @@
         <v>1</v>
       </c>
       <c r="Q154" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -8893,7 +8893,7 @@
         <v>497</v>
       </c>
       <c r="C155" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D155" t="s">
         <v>1</v>
@@ -8946,7 +8946,7 @@
         <v>497</v>
       </c>
       <c r="C156" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D156" t="s">
         <v>1</v>
@@ -8955,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G156" t="s">
         <v>1</v>
@@ -8999,7 +8999,7 @@
         <v>497</v>
       </c>
       <c r="C158" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D158" t="s">
         <v>1</v>
@@ -9041,7 +9041,7 @@
         <v>1</v>
       </c>
       <c r="Q158" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
@@ -9052,7 +9052,7 @@
         <v>497</v>
       </c>
       <c r="C159" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D159" t="s">
         <v>1</v>
@@ -9105,7 +9105,7 @@
         <v>497</v>
       </c>
       <c r="C160" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D160" t="s">
         <v>1</v>
@@ -9114,7 +9114,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G160" t="s">
         <v>1</v>
@@ -9161,7 +9161,7 @@
         <v>497</v>
       </c>
       <c r="C162" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D162" t="s">
         <v>1</v>
@@ -9203,7 +9203,7 @@
         <v>1</v>
       </c>
       <c r="Q162" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
@@ -9214,7 +9214,7 @@
         <v>497</v>
       </c>
       <c r="C163" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D163" t="s">
         <v>1</v>
@@ -9267,7 +9267,7 @@
         <v>497</v>
       </c>
       <c r="C164" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D164" t="s">
         <v>1</v>
@@ -9276,7 +9276,7 @@
         <v>1</v>
       </c>
       <c r="F164" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G164" t="s">
         <v>1</v>
@@ -9323,7 +9323,7 @@
         <v>497</v>
       </c>
       <c r="C166" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D166" t="s">
         <v>1</v>
@@ -9365,7 +9365,7 @@
         <v>1</v>
       </c>
       <c r="Q166" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
@@ -9376,7 +9376,7 @@
         <v>497</v>
       </c>
       <c r="C167" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D167" t="s">
         <v>1</v>
@@ -9429,7 +9429,7 @@
         <v>497</v>
       </c>
       <c r="C168" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D168" t="s">
         <v>1</v>
@@ -9438,7 +9438,7 @@
         <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G168" t="s">
         <v>1</v>
@@ -9485,7 +9485,7 @@
         <v>497</v>
       </c>
       <c r="C170" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D170" t="s">
         <v>1</v>
@@ -9542,7 +9542,7 @@
         <v>497</v>
       </c>
       <c r="C172" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D172" t="s">
         <v>1</v>
@@ -9584,7 +9584,7 @@
         <v>1</v>
       </c>
       <c r="Q172" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="173" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -9595,7 +9595,7 @@
         <v>497</v>
       </c>
       <c r="C173" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D173" t="s">
         <v>1</v>
@@ -9637,7 +9637,7 @@
         <v>1</v>
       </c>
       <c r="Q173" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="174" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -9648,7 +9648,7 @@
         <v>497</v>
       </c>
       <c r="C174" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D174" t="s">
         <v>1</v>
@@ -9690,7 +9690,7 @@
         <v>1</v>
       </c>
       <c r="Q174" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
@@ -9752,7 +9752,7 @@
         <v>9</v>
       </c>
       <c r="C213" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D213" t="s">
         <v>1</v>
@@ -9805,7 +9805,7 @@
         <v>9</v>
       </c>
       <c r="C214" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D214" t="s">
         <v>1</v>
@@ -9858,7 +9858,7 @@
         <v>9</v>
       </c>
       <c r="C215" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D215" t="s">
         <v>1</v>
@@ -9911,7 +9911,7 @@
         <v>184</v>
       </c>
       <c r="C216" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D216" t="s">
         <v>1</v>
@@ -9964,7 +9964,7 @@
         <v>184</v>
       </c>
       <c r="C217" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D217" t="s">
         <v>1</v>
@@ -10017,7 +10017,7 @@
         <v>184</v>
       </c>
       <c r="C218" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D218" t="s">
         <v>1</v>
@@ -10070,7 +10070,7 @@
         <v>184</v>
       </c>
       <c r="C219" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D219" t="s">
         <v>1</v>
@@ -10123,7 +10123,7 @@
         <v>184</v>
       </c>
       <c r="C220" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D220" t="s">
         <v>1</v>
@@ -10176,7 +10176,7 @@
         <v>184</v>
       </c>
       <c r="C221" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D221" t="s">
         <v>1</v>
@@ -10229,7 +10229,7 @@
         <v>184</v>
       </c>
       <c r="C222" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D222" t="s">
         <v>1</v>
@@ -10282,7 +10282,7 @@
         <v>184</v>
       </c>
       <c r="C223" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D223" t="s">
         <v>1</v>
@@ -10335,7 +10335,7 @@
         <v>184</v>
       </c>
       <c r="C224" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D224" t="s">
         <v>1</v>
@@ -10388,7 +10388,7 @@
         <v>184</v>
       </c>
       <c r="C225" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D225" t="s">
         <v>1</v>
@@ -10406,7 +10406,7 @@
         <v>1</v>
       </c>
       <c r="I225" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J225">
         <v>0</v>
@@ -10441,7 +10441,7 @@
         <v>184</v>
       </c>
       <c r="C226" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D226" t="s">
         <v>1</v>
@@ -10494,7 +10494,7 @@
         <v>184</v>
       </c>
       <c r="C227" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D227" t="s">
         <v>1</v>
@@ -10547,7 +10547,7 @@
         <v>184</v>
       </c>
       <c r="C228" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D228" t="s">
         <v>1</v>
@@ -10615,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="H229" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I229" t="s">
         <v>188</v>
@@ -10668,7 +10668,7 @@
         <v>1</v>
       </c>
       <c r="H230" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I230" t="s">
         <v>188</v>
@@ -10721,7 +10721,7 @@
         <v>1</v>
       </c>
       <c r="H231" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I231" t="s">
         <v>188</v>
@@ -10774,7 +10774,7 @@
         <v>1</v>
       </c>
       <c r="H232" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I232" t="s">
         <v>188</v>
@@ -10827,7 +10827,7 @@
         <v>1</v>
       </c>
       <c r="H233" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I233" t="s">
         <v>188</v>
@@ -10880,7 +10880,7 @@
         <v>1</v>
       </c>
       <c r="H234" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I234" t="s">
         <v>188</v>
@@ -10933,7 +10933,7 @@
         <v>1</v>
       </c>
       <c r="H235" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I235" t="s">
         <v>188</v>
@@ -10986,7 +10986,7 @@
         <v>1</v>
       </c>
       <c r="H236" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I236" t="s">
         <v>188</v>
@@ -11410,7 +11410,7 @@
         <v>1</v>
       </c>
       <c r="H244" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I244" t="s">
         <v>198</v>
@@ -11463,7 +11463,7 @@
         <v>1</v>
       </c>
       <c r="H245" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I245" t="s">
         <v>198</v>
@@ -11516,7 +11516,7 @@
         <v>1</v>
       </c>
       <c r="H246" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I246" t="s">
         <v>198</v>
@@ -11569,7 +11569,7 @@
         <v>1</v>
       </c>
       <c r="H247" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I247" t="s">
         <v>198</v>
@@ -11622,7 +11622,7 @@
         <v>1</v>
       </c>
       <c r="H248" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I248" t="s">
         <v>198</v>
@@ -11675,7 +11675,7 @@
         <v>1</v>
       </c>
       <c r="H249" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I249" t="s">
         <v>200</v>
@@ -11713,7 +11713,7 @@
         <v>231</v>
       </c>
       <c r="C251" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D251" t="s">
         <v>1</v>
@@ -11755,7 +11755,7 @@
         <v>1</v>
       </c>
       <c r="Q251" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.2">
@@ -11766,7 +11766,7 @@
         <v>231</v>
       </c>
       <c r="C252" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D252" t="s">
         <v>1</v>
@@ -11808,7 +11808,7 @@
         <v>1</v>
       </c>
       <c r="Q252" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="253" spans="1:17" x14ac:dyDescent="0.2">
@@ -11819,7 +11819,7 @@
         <v>231</v>
       </c>
       <c r="C253" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D253" t="s">
         <v>1</v>
@@ -11834,7 +11834,7 @@
         <v>1</v>
       </c>
       <c r="H253" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I253" t="s">
         <v>313</v>
@@ -11872,7 +11872,7 @@
         <v>231</v>
       </c>
       <c r="C254" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D254" t="s">
         <v>1</v>
@@ -11887,7 +11887,7 @@
         <v>1</v>
       </c>
       <c r="H254" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I254" t="s">
         <v>314</v>
@@ -11925,7 +11925,7 @@
         <v>231</v>
       </c>
       <c r="C255" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D255" t="s">
         <v>1</v>
@@ -11940,7 +11940,7 @@
         <v>1</v>
       </c>
       <c r="H255" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I255" t="s">
         <v>315</v>
@@ -11978,7 +11978,7 @@
         <v>231</v>
       </c>
       <c r="C256" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D256" t="s">
         <v>1</v>
@@ -11993,7 +11993,7 @@
         <v>1</v>
       </c>
       <c r="H256" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I256" t="s">
         <v>316</v>
@@ -12031,7 +12031,7 @@
         <v>231</v>
       </c>
       <c r="C257" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D257" t="s">
         <v>1</v>
@@ -12046,7 +12046,7 @@
         <v>1</v>
       </c>
       <c r="H257" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I257" t="s">
         <v>317</v>
@@ -12084,7 +12084,7 @@
         <v>231</v>
       </c>
       <c r="C258" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D258" t="s">
         <v>1</v>
@@ -12099,7 +12099,7 @@
         <v>1</v>
       </c>
       <c r="H258" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I258" t="s">
         <v>313</v>
@@ -12137,7 +12137,7 @@
         <v>231</v>
       </c>
       <c r="C259" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D259" t="s">
         <v>1</v>
@@ -12152,7 +12152,7 @@
         <v>1</v>
       </c>
       <c r="H259" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I259" t="s">
         <v>314</v>
@@ -12190,7 +12190,7 @@
         <v>231</v>
       </c>
       <c r="C260" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D260" t="s">
         <v>1</v>
@@ -12205,7 +12205,7 @@
         <v>1</v>
       </c>
       <c r="H260" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I260" t="s">
         <v>318</v>
@@ -12243,7 +12243,7 @@
         <v>231</v>
       </c>
       <c r="C261" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D261" t="s">
         <v>1</v>
@@ -12258,7 +12258,7 @@
         <v>1</v>
       </c>
       <c r="H261" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I261" t="s">
         <v>319</v>
@@ -12296,7 +12296,7 @@
         <v>231</v>
       </c>
       <c r="C262" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D262" t="s">
         <v>1</v>
@@ -12311,7 +12311,7 @@
         <v>1</v>
       </c>
       <c r="H262" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I262" t="s">
         <v>320</v>
@@ -12349,7 +12349,7 @@
         <v>231</v>
       </c>
       <c r="C265" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D265" t="s">
         <v>1</v>
@@ -12391,7 +12391,7 @@
         <v>1</v>
       </c>
       <c r="Q265" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.2">
@@ -12402,7 +12402,7 @@
         <v>231</v>
       </c>
       <c r="C266" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D266" t="s">
         <v>1</v>
@@ -12444,7 +12444,7 @@
         <v>1</v>
       </c>
       <c r="Q266" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.2">
@@ -12455,7 +12455,7 @@
         <v>231</v>
       </c>
       <c r="C267" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D267" t="s">
         <v>1</v>
@@ -12470,7 +12470,7 @@
         <v>1</v>
       </c>
       <c r="H267" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I267" t="s">
         <v>325</v>
@@ -12508,7 +12508,7 @@
         <v>231</v>
       </c>
       <c r="C268" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D268" t="s">
         <v>1</v>
@@ -12523,7 +12523,7 @@
         <v>1</v>
       </c>
       <c r="H268" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I268" t="s">
         <v>320</v>
@@ -12561,7 +12561,7 @@
         <v>231</v>
       </c>
       <c r="C269" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D269" t="s">
         <v>1</v>
@@ -12576,7 +12576,7 @@
         <v>1</v>
       </c>
       <c r="H269" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I269" t="s">
         <v>322</v>
@@ -12614,7 +12614,7 @@
         <v>231</v>
       </c>
       <c r="C270" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D270" t="s">
         <v>1</v>
@@ -12629,7 +12629,7 @@
         <v>1</v>
       </c>
       <c r="H270" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I270" t="s">
         <v>323</v>
@@ -12667,7 +12667,7 @@
         <v>231</v>
       </c>
       <c r="C271" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D271" t="s">
         <v>1</v>
@@ -12682,7 +12682,7 @@
         <v>1</v>
       </c>
       <c r="H271" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I271" t="s">
         <v>324</v>
@@ -12720,7 +12720,7 @@
         <v>231</v>
       </c>
       <c r="C272" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D272" t="s">
         <v>1</v>
@@ -12735,7 +12735,7 @@
         <v>1</v>
       </c>
       <c r="H272" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I272" t="s">
         <v>320</v>
@@ -12773,7 +12773,7 @@
         <v>231</v>
       </c>
       <c r="C273" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D273" t="s">
         <v>1</v>
@@ -12788,7 +12788,7 @@
         <v>1</v>
       </c>
       <c r="H273" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I273" t="s">
         <v>325</v>
@@ -12826,7 +12826,7 @@
         <v>231</v>
       </c>
       <c r="C274" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D274" t="s">
         <v>1</v>
@@ -12841,7 +12841,7 @@
         <v>1</v>
       </c>
       <c r="H274" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I274" t="s">
         <v>327</v>
@@ -12879,7 +12879,7 @@
         <v>231</v>
       </c>
       <c r="C275" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D275" t="s">
         <v>1</v>
@@ -12894,7 +12894,7 @@
         <v>1</v>
       </c>
       <c r="H275" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I275" t="s">
         <v>326</v>
@@ -12932,7 +12932,7 @@
         <v>231</v>
       </c>
       <c r="C276" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D276" t="s">
         <v>1</v>
@@ -12947,7 +12947,7 @@
         <v>1</v>
       </c>
       <c r="H276" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I276" t="s">
         <v>328</v>
@@ -12985,7 +12985,7 @@
         <v>231</v>
       </c>
       <c r="C278" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D278" t="s">
         <v>1</v>
@@ -13027,7 +13027,7 @@
         <v>1</v>
       </c>
       <c r="Q278" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="279" spans="1:17" x14ac:dyDescent="0.2">
@@ -13038,7 +13038,7 @@
         <v>231</v>
       </c>
       <c r="C279" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D279" t="s">
         <v>1</v>
@@ -13053,7 +13053,7 @@
         <v>1</v>
       </c>
       <c r="H279" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I279" t="s">
         <v>331</v>
@@ -13091,7 +13091,7 @@
         <v>231</v>
       </c>
       <c r="C280" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D280" t="s">
         <v>1</v>
@@ -13106,7 +13106,7 @@
         <v>1</v>
       </c>
       <c r="H280" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I280" t="s">
         <v>332</v>
@@ -13144,7 +13144,7 @@
         <v>231</v>
       </c>
       <c r="C281" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D281" t="s">
         <v>1</v>
@@ -13159,7 +13159,7 @@
         <v>1</v>
       </c>
       <c r="H281" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I281" t="s">
         <v>333</v>
@@ -13197,7 +13197,7 @@
         <v>231</v>
       </c>
       <c r="C282" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D282" t="s">
         <v>1</v>
@@ -13212,7 +13212,7 @@
         <v>1</v>
       </c>
       <c r="H282" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I282" t="s">
         <v>334</v>
@@ -13250,7 +13250,7 @@
         <v>231</v>
       </c>
       <c r="C283" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D283" t="s">
         <v>1</v>
@@ -13265,7 +13265,7 @@
         <v>1</v>
       </c>
       <c r="H283" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I283" t="s">
         <v>335</v>
@@ -13303,7 +13303,7 @@
         <v>231</v>
       </c>
       <c r="C284" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D284" t="s">
         <v>1</v>
@@ -13318,7 +13318,7 @@
         <v>1</v>
       </c>
       <c r="H284" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I284" t="s">
         <v>336</v>
@@ -13356,7 +13356,7 @@
         <v>231</v>
       </c>
       <c r="C285" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D285" t="s">
         <v>1</v>
@@ -13371,7 +13371,7 @@
         <v>1</v>
       </c>
       <c r="H285" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I285" t="s">
         <v>334</v>
@@ -13409,7 +13409,7 @@
         <v>231</v>
       </c>
       <c r="C286" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D286" t="s">
         <v>1</v>
@@ -13424,7 +13424,7 @@
         <v>1</v>
       </c>
       <c r="H286" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I286" t="s">
         <v>337</v>
@@ -13462,7 +13462,7 @@
         <v>231</v>
       </c>
       <c r="C287" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D287" t="s">
         <v>1</v>
@@ -13477,7 +13477,7 @@
         <v>1</v>
       </c>
       <c r="H287" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I287" t="s">
         <v>338</v>
@@ -13515,7 +13515,7 @@
         <v>231</v>
       </c>
       <c r="C288" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D288" t="s">
         <v>1</v>
@@ -13530,7 +13530,7 @@
         <v>1</v>
       </c>
       <c r="H288" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I288" t="s">
         <v>333</v>
@@ -13568,7 +13568,7 @@
         <v>231</v>
       </c>
       <c r="C290" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D290" t="s">
         <v>1</v>
@@ -13610,7 +13610,7 @@
         <v>1</v>
       </c>
       <c r="Q290" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.2">
@@ -13621,7 +13621,7 @@
         <v>231</v>
       </c>
       <c r="C291" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D291" t="s">
         <v>1</v>
@@ -13636,7 +13636,7 @@
         <v>1</v>
       </c>
       <c r="H291" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I291" t="s">
         <v>341</v>
@@ -13674,7 +13674,7 @@
         <v>231</v>
       </c>
       <c r="C292" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D292" t="s">
         <v>1</v>
@@ -13689,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="H292" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I292" t="s">
         <v>343</v>
@@ -13727,7 +13727,7 @@
         <v>231</v>
       </c>
       <c r="C293" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D293" t="s">
         <v>1</v>
@@ -13742,7 +13742,7 @@
         <v>1</v>
       </c>
       <c r="H293" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I293" t="s">
         <v>344</v>
@@ -13780,7 +13780,7 @@
         <v>231</v>
       </c>
       <c r="C294" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D294" t="s">
         <v>1</v>
@@ -13795,7 +13795,7 @@
         <v>1</v>
       </c>
       <c r="H294" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I294" t="s">
         <v>345</v>
@@ -13833,7 +13833,7 @@
         <v>231</v>
       </c>
       <c r="C295" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D295" t="s">
         <v>1</v>
@@ -13848,7 +13848,7 @@
         <v>1</v>
       </c>
       <c r="H295" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I295" t="s">
         <v>346</v>
@@ -13886,7 +13886,7 @@
         <v>231</v>
       </c>
       <c r="C296" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D296" t="s">
         <v>1</v>
@@ -13901,7 +13901,7 @@
         <v>1</v>
       </c>
       <c r="H296" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I296" t="s">
         <v>347</v>
@@ -13939,7 +13939,7 @@
         <v>231</v>
       </c>
       <c r="C297" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D297" t="s">
         <v>1</v>
@@ -13954,7 +13954,7 @@
         <v>1</v>
       </c>
       <c r="H297" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I297" t="s">
         <v>348</v>
@@ -13992,7 +13992,7 @@
         <v>231</v>
       </c>
       <c r="C298" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D298" t="s">
         <v>1</v>
@@ -14007,7 +14007,7 @@
         <v>1</v>
       </c>
       <c r="H298" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I298" t="s">
         <v>342</v>
@@ -14045,7 +14045,7 @@
         <v>231</v>
       </c>
       <c r="C299" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D299" t="s">
         <v>1</v>
@@ -14060,7 +14060,7 @@
         <v>1</v>
       </c>
       <c r="H299" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I299" t="s">
         <v>349</v>
@@ -14098,7 +14098,7 @@
         <v>9</v>
       </c>
       <c r="C332" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D332" t="s">
         <v>1</v>
@@ -14151,7 +14151,7 @@
         <v>9</v>
       </c>
       <c r="C333" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D333" t="s">
         <v>1</v>
@@ -14204,7 +14204,7 @@
         <v>497</v>
       </c>
       <c r="C334" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D334" t="s">
         <v>1</v>
@@ -14734,7 +14734,7 @@
         <v>497</v>
       </c>
       <c r="C346" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D346" t="s">
         <v>1</v>
@@ -14776,7 +14776,7 @@
         <v>1</v>
       </c>
       <c r="Q346" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="347" spans="1:17" x14ac:dyDescent="0.2">
@@ -14787,7 +14787,7 @@
         <v>497</v>
       </c>
       <c r="C347" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D347" t="s">
         <v>1</v>
@@ -14840,7 +14840,7 @@
         <v>497</v>
       </c>
       <c r="C348" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D348" t="s">
         <v>1</v>
@@ -14849,7 +14849,7 @@
         <v>1</v>
       </c>
       <c r="F348" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G348" t="s">
         <v>1</v>
@@ -14893,7 +14893,7 @@
         <v>497</v>
       </c>
       <c r="C350" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D350" t="s">
         <v>1</v>
@@ -14935,7 +14935,7 @@
         <v>1</v>
       </c>
       <c r="Q350" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="351" spans="1:17" x14ac:dyDescent="0.2">
@@ -14946,7 +14946,7 @@
         <v>497</v>
       </c>
       <c r="C351" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D351" t="s">
         <v>1</v>
@@ -14999,7 +14999,7 @@
         <v>497</v>
       </c>
       <c r="C352" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D352" t="s">
         <v>1</v>
@@ -15008,7 +15008,7 @@
         <v>1</v>
       </c>
       <c r="F352" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G352" t="s">
         <v>1</v>
@@ -15052,7 +15052,7 @@
         <v>497</v>
       </c>
       <c r="C354" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D354" t="s">
         <v>1</v>
@@ -15094,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="Q354" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="355" spans="1:17" x14ac:dyDescent="0.2">
@@ -15105,7 +15105,7 @@
         <v>497</v>
       </c>
       <c r="C355" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D355" t="s">
         <v>1</v>
@@ -15158,7 +15158,7 @@
         <v>497</v>
       </c>
       <c r="C356" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D356" t="s">
         <v>1</v>
@@ -15167,7 +15167,7 @@
         <v>1</v>
       </c>
       <c r="F356" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G356" t="s">
         <v>1</v>
@@ -15211,7 +15211,7 @@
         <v>497</v>
       </c>
       <c r="C358" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D358" t="s">
         <v>1</v>
@@ -15253,7 +15253,7 @@
         <v>1</v>
       </c>
       <c r="Q358" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="359" spans="1:17" x14ac:dyDescent="0.2">
@@ -15264,7 +15264,7 @@
         <v>497</v>
       </c>
       <c r="C359" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D359" t="s">
         <v>1</v>
@@ -15317,7 +15317,7 @@
         <v>497</v>
       </c>
       <c r="C360" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D360" t="s">
         <v>1</v>
@@ -15326,7 +15326,7 @@
         <v>1</v>
       </c>
       <c r="F360" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G360" t="s">
         <v>1</v>
@@ -15373,7 +15373,7 @@
         <v>497</v>
       </c>
       <c r="C362" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D362" t="s">
         <v>1</v>
@@ -15415,7 +15415,7 @@
         <v>1</v>
       </c>
       <c r="Q362" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="363" spans="1:17" x14ac:dyDescent="0.2">
@@ -15426,7 +15426,7 @@
         <v>497</v>
       </c>
       <c r="C363" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D363" t="s">
         <v>1</v>
@@ -15479,7 +15479,7 @@
         <v>497</v>
       </c>
       <c r="C364" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D364" t="s">
         <v>1</v>
@@ -15488,7 +15488,7 @@
         <v>1</v>
       </c>
       <c r="F364" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G364" t="s">
         <v>1</v>
@@ -15536,7 +15536,7 @@
         <v>497</v>
       </c>
       <c r="C366" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D366" t="s">
         <v>1</v>
@@ -15578,7 +15578,7 @@
         <v>1</v>
       </c>
       <c r="Q366" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="367" spans="1:17" x14ac:dyDescent="0.2">
@@ -15589,7 +15589,7 @@
         <v>497</v>
       </c>
       <c r="C367" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D367" t="s">
         <v>1</v>
@@ -15642,7 +15642,7 @@
         <v>497</v>
       </c>
       <c r="C368" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D368" t="s">
         <v>1</v>
@@ -15651,7 +15651,7 @@
         <v>1</v>
       </c>
       <c r="F368" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G368" t="s">
         <v>1</v>
@@ -15699,7 +15699,7 @@
         <v>497</v>
       </c>
       <c r="C370" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D370" t="s">
         <v>1</v>
@@ -15741,7 +15741,7 @@
         <v>1</v>
       </c>
       <c r="Q370" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="371" spans="1:17" x14ac:dyDescent="0.2">
@@ -15752,7 +15752,7 @@
         <v>497</v>
       </c>
       <c r="C371" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D371" t="s">
         <v>1</v>
@@ -15805,7 +15805,7 @@
         <v>497</v>
       </c>
       <c r="C372" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D372" t="s">
         <v>1</v>
@@ -15814,7 +15814,7 @@
         <v>1</v>
       </c>
       <c r="F372" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G372" t="s">
         <v>1</v>
@@ -15863,7 +15863,7 @@
         <v>497</v>
       </c>
       <c r="C374" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D374" t="s">
         <v>1</v>
@@ -15905,7 +15905,7 @@
         <v>1</v>
       </c>
       <c r="Q374" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="375" spans="1:17" x14ac:dyDescent="0.2">
@@ -15916,7 +15916,7 @@
         <v>497</v>
       </c>
       <c r="C375" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D375" t="s">
         <v>1</v>
@@ -15969,7 +15969,7 @@
         <v>497</v>
       </c>
       <c r="C376" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D376" t="s">
         <v>1</v>
@@ -15978,7 +15978,7 @@
         <v>1</v>
       </c>
       <c r="F376" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G376" t="s">
         <v>1</v>
@@ -16022,7 +16022,7 @@
         <v>497</v>
       </c>
       <c r="C378" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D378" t="s">
         <v>1</v>
@@ -16064,7 +16064,7 @@
         <v>1</v>
       </c>
       <c r="Q378" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="379" spans="1:17" x14ac:dyDescent="0.2">
@@ -16075,7 +16075,7 @@
         <v>497</v>
       </c>
       <c r="C379" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D379" t="s">
         <v>1</v>
@@ -16128,7 +16128,7 @@
         <v>497</v>
       </c>
       <c r="C380" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D380" t="s">
         <v>1</v>
@@ -16137,7 +16137,7 @@
         <v>1</v>
       </c>
       <c r="F380" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G380" t="s">
         <v>1</v>
@@ -16181,7 +16181,7 @@
         <v>497</v>
       </c>
       <c r="C382" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D382" t="s">
         <v>1</v>
@@ -16223,7 +16223,7 @@
         <v>1</v>
       </c>
       <c r="Q382" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="383" spans="1:17" x14ac:dyDescent="0.2">
@@ -16234,7 +16234,7 @@
         <v>497</v>
       </c>
       <c r="C383" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D383" t="s">
         <v>1</v>
@@ -16287,7 +16287,7 @@
         <v>497</v>
       </c>
       <c r="C384" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D384" t="s">
         <v>1</v>
@@ -16296,7 +16296,7 @@
         <v>1</v>
       </c>
       <c r="F384" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G384" t="s">
         <v>1</v>
@@ -16343,7 +16343,7 @@
         <v>497</v>
       </c>
       <c r="C386" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D386" t="s">
         <v>1</v>
@@ -16385,7 +16385,7 @@
         <v>1</v>
       </c>
       <c r="Q386" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.2">
@@ -16396,7 +16396,7 @@
         <v>497</v>
       </c>
       <c r="C387" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D387" t="s">
         <v>1</v>
@@ -16449,7 +16449,7 @@
         <v>497</v>
       </c>
       <c r="C388" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D388" t="s">
         <v>1</v>
@@ -16458,7 +16458,7 @@
         <v>1</v>
       </c>
       <c r="F388" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G388" t="s">
         <v>1</v>
@@ -16505,7 +16505,7 @@
         <v>497</v>
       </c>
       <c r="C390" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D390" t="s">
         <v>1</v>
@@ -16547,7 +16547,7 @@
         <v>1</v>
       </c>
       <c r="Q390" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="391" spans="1:17" x14ac:dyDescent="0.2">
@@ -16558,7 +16558,7 @@
         <v>497</v>
       </c>
       <c r="C391" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D391" t="s">
         <v>1</v>
@@ -16611,7 +16611,7 @@
         <v>497</v>
       </c>
       <c r="C392" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D392" t="s">
         <v>1</v>
@@ -16620,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="F392" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G392" t="s">
         <v>1</v>
@@ -16667,7 +16667,7 @@
         <v>497</v>
       </c>
       <c r="C394" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D394" t="s">
         <v>1</v>
@@ -16709,7 +16709,7 @@
         <v>1</v>
       </c>
       <c r="Q394" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="395" spans="1:17" x14ac:dyDescent="0.2">
@@ -16720,7 +16720,7 @@
         <v>497</v>
       </c>
       <c r="C395" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D395" t="s">
         <v>1</v>
@@ -16773,7 +16773,7 @@
         <v>497</v>
       </c>
       <c r="C396" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D396" t="s">
         <v>1</v>
@@ -16782,7 +16782,7 @@
         <v>1</v>
       </c>
       <c r="F396" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G396" t="s">
         <v>1</v>
@@ -16826,7 +16826,7 @@
         <v>497</v>
       </c>
       <c r="C398" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D398" t="s">
         <v>1</v>
@@ -16868,7 +16868,7 @@
         <v>1</v>
       </c>
       <c r="Q398" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="399" spans="1:17" x14ac:dyDescent="0.2">
@@ -16879,7 +16879,7 @@
         <v>497</v>
       </c>
       <c r="C399" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D399" t="s">
         <v>1</v>
@@ -16932,7 +16932,7 @@
         <v>497</v>
       </c>
       <c r="C400" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D400" t="s">
         <v>1</v>
@@ -16941,7 +16941,7 @@
         <v>1</v>
       </c>
       <c r="F400" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G400" t="s">
         <v>1</v>
@@ -16985,7 +16985,7 @@
         <v>497</v>
       </c>
       <c r="C402" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D402" t="s">
         <v>1</v>
@@ -17027,7 +17027,7 @@
         <v>1</v>
       </c>
       <c r="Q402" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="403" spans="1:17" x14ac:dyDescent="0.2">
@@ -17038,7 +17038,7 @@
         <v>497</v>
       </c>
       <c r="C403" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D403" t="s">
         <v>1</v>
@@ -17080,7 +17080,7 @@
         <v>1</v>
       </c>
       <c r="Q403" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="440" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17092,7 +17092,7 @@
         <v>9</v>
       </c>
       <c r="C441" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D441" t="s">
         <v>1</v>
@@ -17145,7 +17145,7 @@
         <v>9</v>
       </c>
       <c r="C442" t="s">
-        <v>503</v>
+        <v>656</v>
       </c>
       <c r="D442" t="s">
         <v>1</v>
@@ -17198,7 +17198,7 @@
         <v>9</v>
       </c>
       <c r="C443" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D443" t="s">
         <v>1</v>
@@ -17251,7 +17251,7 @@
         <v>184</v>
       </c>
       <c r="C444" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D444" t="s">
         <v>1</v>
@@ -17304,7 +17304,7 @@
         <v>184</v>
       </c>
       <c r="C445" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D445" t="s">
         <v>1</v>
@@ -17357,7 +17357,7 @@
         <v>184</v>
       </c>
       <c r="C446" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D446" t="s">
         <v>1</v>
@@ -17410,7 +17410,7 @@
         <v>184</v>
       </c>
       <c r="C447" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D447" t="s">
         <v>1</v>
@@ -17463,7 +17463,7 @@
         <v>184</v>
       </c>
       <c r="C448" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D448" t="s">
         <v>1</v>
@@ -17516,7 +17516,7 @@
         <v>184</v>
       </c>
       <c r="C449" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D449" t="s">
         <v>1</v>
@@ -17569,7 +17569,7 @@
         <v>184</v>
       </c>
       <c r="C450" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D450" t="s">
         <v>1</v>
@@ -17622,7 +17622,7 @@
         <v>184</v>
       </c>
       <c r="C451" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D451" t="s">
         <v>1</v>
@@ -17675,7 +17675,7 @@
         <v>184</v>
       </c>
       <c r="C452" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D452" t="s">
         <v>1</v>
@@ -17728,7 +17728,7 @@
         <v>184</v>
       </c>
       <c r="C453" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D453" t="s">
         <v>1</v>
@@ -17781,7 +17781,7 @@
         <v>184</v>
       </c>
       <c r="C454" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D454" t="s">
         <v>1</v>
@@ -17849,7 +17849,7 @@
         <v>1</v>
       </c>
       <c r="H455" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I455" t="s">
         <v>208</v>
@@ -18273,7 +18273,7 @@
         <v>1</v>
       </c>
       <c r="H463" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I463" t="s">
         <v>226</v>
@@ -18432,7 +18432,7 @@
         <v>1</v>
       </c>
       <c r="H466" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I466" t="s">
         <v>229</v>
@@ -18523,7 +18523,7 @@
         <v>231</v>
       </c>
       <c r="C469" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D469" t="s">
         <v>1</v>
@@ -18565,7 +18565,7 @@
         <v>1</v>
       </c>
       <c r="Q469" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="470" spans="1:17" x14ac:dyDescent="0.2">
@@ -18576,7 +18576,7 @@
         <v>231</v>
       </c>
       <c r="C470" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D470" t="s">
         <v>1</v>
@@ -18591,7 +18591,7 @@
         <v>1</v>
       </c>
       <c r="H470" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I470" t="s">
         <v>394</v>
@@ -18629,7 +18629,7 @@
         <v>231</v>
       </c>
       <c r="C472" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D472" t="s">
         <v>1</v>
@@ -18671,7 +18671,7 @@
         <v>1</v>
       </c>
       <c r="Q472" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="473" spans="1:17" x14ac:dyDescent="0.2">
@@ -18682,7 +18682,7 @@
         <v>231</v>
       </c>
       <c r="C473" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D473" t="s">
         <v>1</v>
@@ -18735,7 +18735,7 @@
         <v>231</v>
       </c>
       <c r="C474" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D474" t="s">
         <v>1</v>
@@ -18788,7 +18788,7 @@
         <v>231</v>
       </c>
       <c r="C475" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D475" t="s">
         <v>1</v>
@@ -18841,7 +18841,7 @@
         <v>231</v>
       </c>
       <c r="C476" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D476" t="s">
         <v>1</v>
@@ -18894,7 +18894,7 @@
         <v>231</v>
       </c>
       <c r="C477" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D477" t="s">
         <v>1</v>
@@ -18947,7 +18947,7 @@
         <v>231</v>
       </c>
       <c r="C478" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D478" t="s">
         <v>1</v>
@@ -19000,7 +19000,7 @@
         <v>231</v>
       </c>
       <c r="C479" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D479" t="s">
         <v>1</v>
@@ -19053,7 +19053,7 @@
         <v>231</v>
       </c>
       <c r="C480" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D480" t="s">
         <v>1</v>
@@ -19106,7 +19106,7 @@
         <v>231</v>
       </c>
       <c r="C481" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D481" t="s">
         <v>1</v>
@@ -19159,7 +19159,7 @@
         <v>231</v>
       </c>
       <c r="C482" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D482" t="s">
         <v>1</v>
@@ -19212,7 +19212,7 @@
         <v>231</v>
       </c>
       <c r="C483" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D483" t="s">
         <v>1</v>
@@ -19227,7 +19227,7 @@
         <v>1</v>
       </c>
       <c r="H483" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I483" t="s">
         <v>428</v>
@@ -19265,7 +19265,7 @@
         <v>231</v>
       </c>
       <c r="C485" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D485" t="s">
         <v>1</v>
@@ -19307,7 +19307,7 @@
         <v>1</v>
       </c>
       <c r="Q485" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="486" spans="1:17" x14ac:dyDescent="0.2">
@@ -19318,7 +19318,7 @@
         <v>231</v>
       </c>
       <c r="C486" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D486" t="s">
         <v>1</v>
@@ -19371,7 +19371,7 @@
         <v>231</v>
       </c>
       <c r="C487" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D487" t="s">
         <v>1</v>
@@ -19424,7 +19424,7 @@
         <v>231</v>
       </c>
       <c r="C489" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D489" t="s">
         <v>1</v>
@@ -19466,7 +19466,7 @@
         <v>1</v>
       </c>
       <c r="Q489" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="490" spans="1:17" x14ac:dyDescent="0.2">
@@ -19477,7 +19477,7 @@
         <v>231</v>
       </c>
       <c r="C490" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D490" t="s">
         <v>1</v>
@@ -19530,7 +19530,7 @@
         <v>231</v>
       </c>
       <c r="C491" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D491" t="s">
         <v>1</v>
@@ -19583,7 +19583,7 @@
         <v>231</v>
       </c>
       <c r="C493" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D493" t="s">
         <v>1</v>
@@ -19625,7 +19625,7 @@
         <v>1</v>
       </c>
       <c r="Q493" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="494" spans="1:17" x14ac:dyDescent="0.2">
@@ -19636,7 +19636,7 @@
         <v>231</v>
       </c>
       <c r="C494" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D494" t="s">
         <v>1</v>
@@ -19689,7 +19689,7 @@
         <v>231</v>
       </c>
       <c r="C495" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D495" t="s">
         <v>1</v>
@@ -19704,7 +19704,7 @@
         <v>1</v>
       </c>
       <c r="H495" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I495" t="s">
         <v>444</v>
@@ -19742,7 +19742,7 @@
         <v>231</v>
       </c>
       <c r="C496" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D496" t="s">
         <v>1</v>
@@ -19757,7 +19757,7 @@
         <v>1</v>
       </c>
       <c r="H496" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I496" t="s">
         <v>444</v>
@@ -19795,7 +19795,7 @@
         <v>231</v>
       </c>
       <c r="C498" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D498" t="s">
         <v>1</v>
@@ -19837,7 +19837,7 @@
         <v>1</v>
       </c>
       <c r="Q498" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="499" spans="1:17" x14ac:dyDescent="0.2">
@@ -19848,7 +19848,7 @@
         <v>231</v>
       </c>
       <c r="C499" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D499" t="s">
         <v>1</v>
@@ -19901,7 +19901,7 @@
         <v>231</v>
       </c>
       <c r="C500" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D500" t="s">
         <v>1</v>
@@ -19957,7 +19957,7 @@
         <v>231</v>
       </c>
       <c r="C502" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D502" t="s">
         <v>1</v>
@@ -19999,7 +19999,7 @@
         <v>1</v>
       </c>
       <c r="Q502" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="503" spans="1:17" x14ac:dyDescent="0.2">
@@ -20010,7 +20010,7 @@
         <v>231</v>
       </c>
       <c r="C503" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D503" t="s">
         <v>1</v>
@@ -20063,7 +20063,7 @@
         <v>231</v>
       </c>
       <c r="C504" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D504" t="s">
         <v>1</v>
@@ -20116,7 +20116,7 @@
         <v>231</v>
       </c>
       <c r="C506" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D506" t="s">
         <v>1</v>
@@ -20158,7 +20158,7 @@
         <v>1</v>
       </c>
       <c r="Q506" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="507" spans="1:17" x14ac:dyDescent="0.2">
@@ -20169,7 +20169,7 @@
         <v>231</v>
       </c>
       <c r="C507" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D507" t="s">
         <v>1</v>
@@ -20222,7 +20222,7 @@
         <v>231</v>
       </c>
       <c r="C508" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D508" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
fix: correct unit number assignment logic vocabulary section
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0518AC35-A81B-554C-9F30-F822A0E1A91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103997F2-0914-034D-A8D5-2DD7499A54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="656">
   <si>
     <t>A1</t>
   </si>
@@ -2060,9 +2060,6 @@
   </si>
   <si>
     <t>She is waiting for you ______ 0 هي تنتظرك {{aهنا}} ; I will ______ love you 0 انا سأحبك {{aدائما}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> unit3</t>
   </si>
 </sst>
 </file>
@@ -2473,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:Q508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A372" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="H376" sqref="H376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6591,7 +6588,7 @@
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -6644,7 +6641,7 @@
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
@@ -6697,7 +6694,7 @@
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D104" t="s">
         <v>1</v>
@@ -6750,7 +6747,7 @@
         <v>497</v>
       </c>
       <c r="C105" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D105" t="s">
         <v>1</v>
@@ -9752,7 +9749,7 @@
         <v>9</v>
       </c>
       <c r="C213" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D213" t="s">
         <v>1</v>
@@ -9805,7 +9802,7 @@
         <v>9</v>
       </c>
       <c r="C214" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D214" t="s">
         <v>1</v>
@@ -9858,7 +9855,7 @@
         <v>9</v>
       </c>
       <c r="C215" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D215" t="s">
         <v>1</v>
@@ -14098,7 +14095,7 @@
         <v>9</v>
       </c>
       <c r="C332" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D332" t="s">
         <v>1</v>
@@ -14151,7 +14148,7 @@
         <v>9</v>
       </c>
       <c r="C333" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D333" t="s">
         <v>1</v>
@@ -14204,7 +14201,7 @@
         <v>497</v>
       </c>
       <c r="C334" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D334" t="s">
         <v>1</v>
@@ -17092,7 +17089,7 @@
         <v>9</v>
       </c>
       <c r="C441" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D441" t="s">
         <v>1</v>
@@ -17145,7 +17142,7 @@
         <v>9</v>
       </c>
       <c r="C442" t="s">
-        <v>656</v>
+        <v>502</v>
       </c>
       <c r="D442" t="s">
         <v>1</v>
@@ -17198,7 +17195,7 @@
         <v>9</v>
       </c>
       <c r="C443" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D443" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
feat: Implement dynamic day selection dropdown
</commit_message>
<xml_diff>
--- a/assets/questions.xlsx
+++ b/assets/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ribhibish/Desktop/FLutter/az-english/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103997F2-0914-034D-A8D5-2DD7499A54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD17AEE-CDB7-B44D-84A2-CB019450508D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{6AEEC35D-FFE0-0C48-BE89-BDD07A570BA2}"/>
   </bookViews>
@@ -2470,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543F04A-C5C9-5445-AC86-CB4890E27EED}">
   <dimension ref="A4:Q508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H376" sqref="H376"/>
+    <sheetView tabSelected="1" topLeftCell="A502" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="H523" sqref="H523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6747,7 +6747,7 @@
         <v>497</v>
       </c>
       <c r="C105" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D105" t="s">
         <v>1</v>
@@ -14201,7 +14201,7 @@
         <v>497</v>
       </c>
       <c r="C334" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D334" t="s">
         <v>1</v>

</xml_diff>